<commit_message>
Initial commit search for NLP reduced cost
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Rafael\Models\MaxProfitFeeding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Gabriel\Models\EMB_MaxProfitDiet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TODOS" sheetId="1" r:id="rId1"/>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="377">
   <si>
     <t>TODO</t>
   </si>
@@ -1417,6 +1417,9 @@
   </si>
   <si>
     <t>batch_2_GSS-Max</t>
+  </si>
+  <si>
+    <t>Find Reduced Cost</t>
   </si>
 </sst>
 </file>
@@ -3047,6 +3050,390 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="AutoShape 20"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="AutoShape 18"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="AutoShape 16"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="AutoShape 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="AutoShape 8"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3191,6 +3578,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3223,9 +3658,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scenario" displayName="Scenario" ref="A1:S5" totalsRowShown="0">
-  <autoFilter ref="A1:S5"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scenario" displayName="Scenario" ref="A1:T5" totalsRowShown="0">
+  <autoFilter ref="A1:T5"/>
+  <tableColumns count="20">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Feed Scenario"/>
     <tableColumn id="3" name="Batch"/>
@@ -3245,6 +3680,7 @@
     <tableColumn id="17" name="UB"/>
     <tableColumn id="18" name="Tol"/>
     <tableColumn id="19" name="Obj"/>
+    <tableColumn id="20" name="Find Reduced Cost"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3765,8 +4201,8 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4572,10 +5008,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4597,7 +5033,7 @@
     <col min="21" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -4655,8 +5091,11 @@
       <c r="S1" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="T1" t="s">
+        <v>376</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4714,8 +5153,11 @@
       <c r="S2" t="s">
         <v>48</v>
       </c>
+      <c r="T2" s="6">
+        <v>59</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4773,8 +5215,11 @@
       <c r="S3" t="s">
         <v>49</v>
       </c>
+      <c r="T3" s="6">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4832,8 +5277,11 @@
       <c r="S4" t="s">
         <v>51</v>
       </c>
+      <c r="T4" s="6">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4890,6 +5338,9 @@
       </c>
       <c r="S5" t="s">
         <v>49</v>
+      </c>
+      <c r="T5" s="6">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Partial implementation of target weight
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Documents\GitHub\EMB_MaxProfitDiet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Gabriel\Models\EMB_MaxProfitDiet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2E630-38C8-475A-8125-74DEEB74B0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TODOS" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="Feed Library" sheetId="5" r:id="rId5"/>
     <sheet name="Parameters List" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="383">
   <si>
     <t>TODO</t>
   </si>
@@ -1182,11 +1181,17 @@
   <si>
     <t>Only Costs Batch</t>
   </si>
+  <si>
+    <t>Feeding Time</t>
+  </si>
+  <si>
+    <t>Target Weight</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
     <numFmt numFmtId="165" formatCode="0.00;0.00;0;@"/>
@@ -4784,7 +4789,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>784860</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -4833,7 +4838,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>784860</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -4887,7 +4892,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>784860</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -4941,7 +4946,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>784860</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -4995,7 +5000,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5049,7 +5054,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5103,7 +5108,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5153,139 +5158,141 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0">
-  <autoFilter ref="A1:D10" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0">
+  <autoFilter ref="A1:D10"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TODO"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Meliante"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Script"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description"/>
+    <tableColumn id="1" name="TODO"/>
+    <tableColumn id="2" name="Meliante"/>
+    <tableColumn id="3" name="Script"/>
+    <tableColumn id="4" name="Description"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela2" displayName="Tabela2" ref="A1:F12" totalsRowShown="0">
-  <autoFilter ref="A1:F12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela2" displayName="Tabela2" ref="A1:F12" totalsRowShown="0">
+  <autoFilter ref="A1:F12"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Feed Scenario"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ID"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Min %DM"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Max %DM"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Cost [US$/kg AF]"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Name"/>
+    <tableColumn id="1" name="Feed Scenario"/>
+    <tableColumn id="2" name="ID"/>
+    <tableColumn id="3" name="Min %DM"/>
+    <tableColumn id="4" name="Max %DM"/>
+    <tableColumn id="5" name="Cost [US$/kg AF]"/>
+    <tableColumn id="6" name="Name"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Scenario" displayName="Scenario" ref="A1:T2" totalsRowShown="0">
-  <autoFilter ref="A1:T2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Feed Scenario"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Batch"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Breed"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="SBW"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="BCS"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="BE"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="L"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="SEX"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="a2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="PH"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Selling Price [US$]"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Linearization factor"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Algorithm"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Identifier"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="LB"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="UB"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Tol"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Obj"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Find Reduced Cost"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scenario" displayName="Scenario" ref="A1:V2" totalsRowShown="0">
+  <autoFilter ref="A1:V2"/>
+  <tableColumns count="22">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Feed Scenario"/>
+    <tableColumn id="3" name="Batch"/>
+    <tableColumn id="4" name="Breed"/>
+    <tableColumn id="5" name="SBW"/>
+    <tableColumn id="22" name="Feeding Time"/>
+    <tableColumn id="21" name="Target Weight"/>
+    <tableColumn id="6" name="BCS"/>
+    <tableColumn id="7" name="BE"/>
+    <tableColumn id="8" name="L"/>
+    <tableColumn id="9" name="SEX"/>
+    <tableColumn id="10" name="a2"/>
+    <tableColumn id="11" name="PH"/>
+    <tableColumn id="12" name="Selling Price [US$]"/>
+    <tableColumn id="13" name="Linearization factor"/>
+    <tableColumn id="14" name="Algorithm"/>
+    <tableColumn id="15" name="Identifier"/>
+    <tableColumn id="16" name="LB"/>
+    <tableColumn id="17" name="UB"/>
+    <tableColumn id="18" name="Tol"/>
+    <tableColumn id="19" name="Obj"/>
+    <tableColumn id="20" name="Find Reduced Cost"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table6" displayName="Table6" ref="A1:F3" totalsRowShown="0">
-  <autoFilter ref="A1:F3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table6" displayName="Table6" ref="A1:F3" totalsRowShown="0">
+  <autoFilter ref="A1:F3"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Batch ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Filename"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Period col"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Initial Period"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Final Period"/>
-    <tableColumn id="6" xr3:uid="{0AFD491A-7288-4D16-9112-826D8C29AA9E}" name="Only Costs Batch"/>
+    <tableColumn id="1" name="Batch ID"/>
+    <tableColumn id="2" name="Filename"/>
+    <tableColumn id="3" name="Period col"/>
+    <tableColumn id="4" name="Initial Period"/>
+    <tableColumn id="5" name="Final Period"/>
+    <tableColumn id="6" name="Only Costs Batch"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="FeedLib" displayName="FeedLib" ref="A1:BF234" totalsRowShown="0">
-  <autoFilter ref="A1:BF234" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF234" totalsRowShown="0">
+  <autoFilter ref="A1:BF234"/>
   <tableColumns count="58">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Feed"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="IFN"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Cost, $/Tonne AF"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Forage, %DM"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="DM, %AF"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="CP, %DM"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="SP, %CP"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="ADICP, %CP"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Sugars, %DM"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="OA, %DM"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="Fat, %DM"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="Ash, %DM"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="Starch, %DM"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="NDF, %DM"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="Lignin, %DM"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0400-000011000000}" name="TDN, %DM"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="ME, Mcal/kg"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0400-000013000000}" name="NEma, Mcal/kg"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0400-000014000000}" name="NEga, Mcal/kg"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0400-000015000000}" name="RUP, %CP"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0400-000016000000}" name="kd PB, %/h"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0400-000017000000}" name="kd CB1, %/h"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0400-000018000000}" name="kd CB2, %/h"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0400-000019000000}" name="kd CB3, %/h"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0400-00001A000000}" name="PBID, %"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0400-00001B000000}" name="CB1ID, %"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0400-00001C000000}" name="CB2ID, %"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0400-00001D000000}" name="pef, %NDF"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0400-00001E000000}" name="ARG, %DM"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0400-00001F000000}" name="HIS, %DM"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0400-000020000000}" name="ILE, %DM"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0400-000021000000}" name="LEU, %DM"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0400-000022000000}" name="LYS, %DM"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0400-000023000000}" name="MET, %DM"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0400-000024000000}" name="CYS, %DM"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0400-000025000000}" name="PHE, %DM"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0400-000026000000}" name="TYR, %DM"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0400-000027000000}" name="THR, %DM"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0400-000028000000}" name="TRP, %DM"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0400-000029000000}" name="VAL, %DM"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0400-00002A000000}" name="Ca, % DM"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0400-00002B000000}" name="P, % DM"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0400-00002C000000}" name="Mg, % DM"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0400-00002D000000}" name="Cl, % DM"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0400-00002E000000}" name="K, % DM"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0400-00002F000000}" name="Na, % DM"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0400-000030000000}" name="S, % DM"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0400-000031000000}" name="Co, mg/kg"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0400-000032000000}" name="Cu, mg/kg"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0400-000033000000}" name="I, mg/kg"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0400-000034000000}" name="Fe, mg/kg"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0400-000035000000}" name="Mn, mg/kg"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0400-000036000000}" name="Se, mg/kg"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0400-000037000000}" name="Zn, mg/kg"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0400-000038000000}" name="Vit A, IU/g"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0400-000039000000}" name="Vit D, IU/g"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0400-00003A000000}" name="Vit E, IU/kg"/>
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Feed"/>
+    <tableColumn id="3" name="IFN"/>
+    <tableColumn id="4" name="Cost, $/Tonne AF"/>
+    <tableColumn id="5" name="Forage, %DM"/>
+    <tableColumn id="6" name="DM, %AF"/>
+    <tableColumn id="7" name="CP, %DM"/>
+    <tableColumn id="8" name="SP, %CP"/>
+    <tableColumn id="9" name="ADICP, %CP"/>
+    <tableColumn id="10" name="Sugars, %DM"/>
+    <tableColumn id="11" name="OA, %DM"/>
+    <tableColumn id="12" name="Fat, %DM"/>
+    <tableColumn id="13" name="Ash, %DM"/>
+    <tableColumn id="14" name="Starch, %DM"/>
+    <tableColumn id="15" name="NDF, %DM"/>
+    <tableColumn id="16" name="Lignin, %DM"/>
+    <tableColumn id="17" name="TDN, %DM"/>
+    <tableColumn id="18" name="ME, Mcal/kg"/>
+    <tableColumn id="19" name="NEma, Mcal/kg"/>
+    <tableColumn id="20" name="NEga, Mcal/kg"/>
+    <tableColumn id="21" name="RUP, %CP"/>
+    <tableColumn id="22" name="kd PB, %/h"/>
+    <tableColumn id="23" name="kd CB1, %/h"/>
+    <tableColumn id="24" name="kd CB2, %/h"/>
+    <tableColumn id="25" name="kd CB3, %/h"/>
+    <tableColumn id="26" name="PBID, %"/>
+    <tableColumn id="27" name="CB1ID, %"/>
+    <tableColumn id="28" name="CB2ID, %"/>
+    <tableColumn id="29" name="pef, %NDF"/>
+    <tableColumn id="30" name="ARG, %DM"/>
+    <tableColumn id="31" name="HIS, %DM"/>
+    <tableColumn id="32" name="ILE, %DM"/>
+    <tableColumn id="33" name="LEU, %DM"/>
+    <tableColumn id="34" name="LYS, %DM"/>
+    <tableColumn id="35" name="MET, %DM"/>
+    <tableColumn id="36" name="CYS, %DM"/>
+    <tableColumn id="37" name="PHE, %DM"/>
+    <tableColumn id="38" name="TYR, %DM"/>
+    <tableColumn id="39" name="THR, %DM"/>
+    <tableColumn id="40" name="TRP, %DM"/>
+    <tableColumn id="41" name="VAL, %DM"/>
+    <tableColumn id="42" name="Ca, % DM"/>
+    <tableColumn id="43" name="P, % DM"/>
+    <tableColumn id="44" name="Mg, % DM"/>
+    <tableColumn id="45" name="Cl, % DM"/>
+    <tableColumn id="46" name="K, % DM"/>
+    <tableColumn id="47" name="Na, % DM"/>
+    <tableColumn id="48" name="S, % DM"/>
+    <tableColumn id="49" name="Co, mg/kg"/>
+    <tableColumn id="50" name="Cu, mg/kg"/>
+    <tableColumn id="51" name="I, mg/kg"/>
+    <tableColumn id="52" name="Fe, mg/kg"/>
+    <tableColumn id="53" name="Mn, mg/kg"/>
+    <tableColumn id="54" name="Se, mg/kg"/>
+    <tableColumn id="55" name="Zn, mg/kg"/>
+    <tableColumn id="56" name="Vit A, IU/g"/>
+    <tableColumn id="57" name="Vit D, IU/g"/>
+    <tableColumn id="58" name="Vit E, IU/kg"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5553,7 +5560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -5563,16 +5570,16 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="68.42578125" customWidth="1"/>
-    <col min="5" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
+    <col min="4" max="4" width="68.44140625" customWidth="1"/>
+    <col min="5" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5586,7 +5593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -5597,7 +5604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -5611,7 +5618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -5625,7 +5632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -5639,7 +5646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -5653,7 +5660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -5667,7 +5674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -5681,7 +5688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -5695,7 +5702,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -5719,7 +5726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -5729,18 +5736,18 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="6" width="29.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -5760,7 +5767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5781,7 +5788,7 @@
         <v>Sugarcane bagase - BR</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -5802,7 +5809,7 @@
         <v>Citrus Pulp - BR</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -5823,7 +5830,7 @@
         <v>Corn, grain - BR</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -5844,7 +5851,7 @@
         <v>Cottonseed Meal 38% - BR</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -5865,7 +5872,7 @@
         <v>Cottonseed Whole - BR</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -5886,7 +5893,7 @@
         <v>Soybean Hulls - BR</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -5907,7 +5914,7 @@
         <v>Soybean Meal 49% - BR</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -5928,7 +5935,7 @@
         <v>Wheat Meal - BR</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -5949,7 +5956,7 @@
         <v>Urea - BR</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -5970,7 +5977,7 @@
         <v>Ammonium Sulfate - BR</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -6010,37 +6017,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="8.7109375" customWidth="1"/>
-    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="3" width="8.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="7" width="7.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" customWidth="1"/>
+    <col min="13" max="14" width="14.109375" customWidth="1"/>
+    <col min="15" max="15" width="20.5546875" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="8.6640625" customWidth="1"/>
+    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="1027" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -6057,52 +6065,58 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6119,63 +6133,69 @@
         <v>446</v>
       </c>
       <c r="F2" s="4">
+        <v>150</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
         <v>4</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1</v>
       </c>
       <c r="I2" s="4">
         <v>1</v>
       </c>
       <c r="J2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="4">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
         <v>6.03</v>
       </c>
-      <c r="L2" s="4">
+      <c r="N2" s="4">
         <v>7.9331307870370509</v>
       </c>
-      <c r="M2" s="4">
+      <c r="O2" s="4">
         <v>0.87</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="P2" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="S2" s="4">
         <v>3</v>
       </c>
-      <c r="R2" s="4">
+      <c r="T2" s="4">
         <v>0.01</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="T2" s="4">
+      <c r="V2" s="4">
         <v>900</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -6185,18 +6205,18 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="7" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -6216,7 +6236,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -6236,7 +6256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6266,7 +6286,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFE7E6E6"/>
   </sheetPr>
@@ -6276,64 +6296,64 @@
       <selection activeCell="A220" sqref="A220:BF234"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="16.28515625" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125"/>
-    <col min="22" max="22" width="12.42578125" customWidth="1"/>
-    <col min="23" max="25" width="13.42578125" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" customWidth="1"/>
-    <col min="27" max="28" width="10.7109375" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125"/>
-    <col min="32" max="32" width="11.140625" customWidth="1"/>
-    <col min="33" max="33" width="11.85546875" customWidth="1"/>
-    <col min="34" max="34" width="11.5703125" customWidth="1"/>
-    <col min="35" max="35" width="12.42578125" customWidth="1"/>
-    <col min="36" max="36" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625"/>
+    <col min="22" max="22" width="12.44140625" customWidth="1"/>
+    <col min="23" max="25" width="13.44140625" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" customWidth="1"/>
+    <col min="27" max="28" width="10.6640625" customWidth="1"/>
+    <col min="29" max="29" width="11.88671875" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
+    <col min="31" max="31" width="11.44140625"/>
+    <col min="32" max="32" width="11.109375" customWidth="1"/>
+    <col min="33" max="33" width="11.88671875" customWidth="1"/>
+    <col min="34" max="34" width="11.5546875" customWidth="1"/>
+    <col min="35" max="35" width="12.44140625" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" customWidth="1"/>
     <col min="37" max="37" width="12" customWidth="1"/>
-    <col min="38" max="38" width="11.7109375" customWidth="1"/>
+    <col min="38" max="38" width="11.6640625" customWidth="1"/>
     <col min="39" max="39" width="12" customWidth="1"/>
-    <col min="40" max="40" width="11.85546875" customWidth="1"/>
+    <col min="40" max="40" width="11.88671875" customWidth="1"/>
     <col min="41" max="41" width="12" customWidth="1"/>
-    <col min="42" max="42" width="11.28515625" customWidth="1"/>
-    <col min="43" max="43" width="10.28515625" customWidth="1"/>
-    <col min="44" max="44" width="11.85546875" customWidth="1"/>
-    <col min="45" max="45" width="10.7109375" customWidth="1"/>
-    <col min="46" max="46" width="10.28515625" customWidth="1"/>
-    <col min="47" max="47" width="11.42578125"/>
-    <col min="48" max="48" width="10.140625" customWidth="1"/>
+    <col min="42" max="42" width="11.33203125" customWidth="1"/>
+    <col min="43" max="43" width="10.33203125" customWidth="1"/>
+    <col min="44" max="44" width="11.88671875" customWidth="1"/>
+    <col min="45" max="45" width="10.6640625" customWidth="1"/>
+    <col min="46" max="46" width="10.33203125" customWidth="1"/>
+    <col min="47" max="47" width="11.44140625"/>
+    <col min="48" max="48" width="10.109375" customWidth="1"/>
     <col min="49" max="50" width="12" customWidth="1"/>
-    <col min="51" max="51" width="10.28515625" customWidth="1"/>
-    <col min="52" max="52" width="11.7109375" customWidth="1"/>
-    <col min="53" max="53" width="12.7109375" customWidth="1"/>
-    <col min="54" max="54" width="11.7109375" customWidth="1"/>
-    <col min="55" max="55" width="11.85546875" customWidth="1"/>
+    <col min="51" max="51" width="10.33203125" customWidth="1"/>
+    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="53" max="53" width="12.6640625" customWidth="1"/>
+    <col min="54" max="54" width="11.6640625" customWidth="1"/>
+    <col min="55" max="55" width="11.88671875" customWidth="1"/>
     <col min="56" max="57" width="12" customWidth="1"/>
-    <col min="58" max="58" width="12.7109375" customWidth="1"/>
-    <col min="59" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="58" max="58" width="12.6640625" customWidth="1"/>
+    <col min="59" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -6509,7 +6529,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -6683,7 +6703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -6857,7 +6877,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -7031,7 +7051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -7205,7 +7225,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -7379,7 +7399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -7553,7 +7573,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -7727,7 +7747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -7901,7 +7921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -8075,7 +8095,7 @@
         <v>44.9</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -8249,7 +8269,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -8423,7 +8443,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -8597,7 +8617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -8771,7 +8791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -8945,7 +8965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -9119,7 +9139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -9293,7 +9313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -9467,7 +9487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -9641,7 +9661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -9815,7 +9835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -9989,7 +10009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -10163,7 +10183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -10337,7 +10357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -10511,7 +10531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -10685,7 +10705,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>25</v>
       </c>
@@ -10859,7 +10879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -11033,7 +11053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -11207,7 +11227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -11381,7 +11401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -11555,7 +11575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -11729,7 +11749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>31</v>
       </c>
@@ -11903,7 +11923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>32</v>
       </c>
@@ -12077,7 +12097,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>33</v>
       </c>
@@ -12251,7 +12271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>34</v>
       </c>
@@ -12425,7 +12445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>35</v>
       </c>
@@ -12599,7 +12619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>36</v>
       </c>
@@ -12773,7 +12793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>37</v>
       </c>
@@ -12947,7 +12967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>38</v>
       </c>
@@ -13121,7 +13141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>39</v>
       </c>
@@ -13295,7 +13315,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>40</v>
       </c>
@@ -13469,7 +13489,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="42" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>41</v>
       </c>
@@ -13643,7 +13663,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>42</v>
       </c>
@@ -13817,7 +13837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <v>43</v>
       </c>
@@ -13991,7 +14011,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>44</v>
       </c>
@@ -14165,7 +14185,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <v>45</v>
       </c>
@@ -14339,7 +14359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>46</v>
       </c>
@@ -14513,7 +14533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <v>47</v>
       </c>
@@ -14687,7 +14707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>48</v>
       </c>
@@ -14861,7 +14881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>49</v>
       </c>
@@ -15035,7 +15055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>50</v>
       </c>
@@ -15209,7 +15229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>51</v>
       </c>
@@ -15383,7 +15403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>52</v>
       </c>
@@ -15557,7 +15577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>53</v>
       </c>
@@ -15731,7 +15751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>54</v>
       </c>
@@ -15905,7 +15925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>55</v>
       </c>
@@ -16079,7 +16099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>56</v>
       </c>
@@ -16253,7 +16273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>57</v>
       </c>
@@ -16427,7 +16447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>58</v>
       </c>
@@ -16601,7 +16621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>59</v>
       </c>
@@ -16775,7 +16795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>60</v>
       </c>
@@ -16949,7 +16969,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="62" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>61</v>
       </c>
@@ -17123,7 +17143,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="63" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <v>62</v>
       </c>
@@ -17297,7 +17317,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="64" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>63</v>
       </c>
@@ -17471,7 +17491,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
         <v>64</v>
       </c>
@@ -17645,7 +17665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
         <v>65</v>
       </c>
@@ -17819,7 +17839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
         <v>66</v>
       </c>
@@ -17993,7 +18013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A68" s="8">
         <v>67</v>
       </c>
@@ -18167,7 +18187,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A69" s="8">
         <v>68</v>
       </c>
@@ -18341,7 +18361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A70" s="8">
         <v>69</v>
       </c>
@@ -18515,7 +18535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A71" s="8">
         <v>70</v>
       </c>
@@ -18689,7 +18709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A72" s="8">
         <v>71</v>
       </c>
@@ -18863,7 +18883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A73" s="8">
         <v>72</v>
       </c>
@@ -19037,7 +19057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A74" s="8">
         <v>73</v>
       </c>
@@ -19211,7 +19231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A75" s="8">
         <v>74</v>
       </c>
@@ -19385,7 +19405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A76" s="8">
         <v>75</v>
       </c>
@@ -19559,7 +19579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A77" s="8">
         <v>76</v>
       </c>
@@ -19733,7 +19753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A78" s="8">
         <v>77</v>
       </c>
@@ -19907,7 +19927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A79" s="8">
         <v>78</v>
       </c>
@@ -20081,7 +20101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A80" s="8">
         <v>79</v>
       </c>
@@ -20255,7 +20275,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A81" s="8">
         <v>80</v>
       </c>
@@ -20429,7 +20449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A82" s="8">
         <v>81</v>
       </c>
@@ -20603,7 +20623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A83" s="8">
         <v>82</v>
       </c>
@@ -20777,7 +20797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A84" s="8">
         <v>83</v>
       </c>
@@ -20951,7 +20971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A85" s="8">
         <v>84</v>
       </c>
@@ -21125,7 +21145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A86" s="8">
         <v>85</v>
       </c>
@@ -21299,7 +21319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A87" s="8">
         <v>86</v>
       </c>
@@ -21473,7 +21493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A88" s="8">
         <v>87</v>
       </c>
@@ -21647,7 +21667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A89" s="8">
         <v>88</v>
       </c>
@@ -21821,7 +21841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A90" s="8">
         <v>89</v>
       </c>
@@ -21995,7 +22015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A91" s="8">
         <v>90</v>
       </c>
@@ -22169,7 +22189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A92" s="8">
         <v>91</v>
       </c>
@@ -22343,7 +22363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A93" s="8">
         <v>92</v>
       </c>
@@ -22517,7 +22537,7 @@
         <v>135.6</v>
       </c>
     </row>
-    <row r="94" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A94" s="8">
         <v>93</v>
       </c>
@@ -22691,7 +22711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A95" s="8">
         <v>94</v>
       </c>
@@ -22865,7 +22885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A96" s="8">
         <v>95</v>
       </c>
@@ -23039,7 +23059,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="97" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A97" s="8">
         <v>96</v>
       </c>
@@ -23213,7 +23233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A98" s="8">
         <v>97</v>
       </c>
@@ -23387,7 +23407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A99" s="8">
         <v>98</v>
       </c>
@@ -23561,7 +23581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A100" s="8">
         <v>99</v>
       </c>
@@ -23735,7 +23755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A101" s="8">
         <v>100</v>
       </c>
@@ -23909,7 +23929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A102" s="8">
         <v>101</v>
       </c>
@@ -24083,7 +24103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A103" s="8">
         <v>102</v>
       </c>
@@ -24257,7 +24277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A104" s="8">
         <v>103</v>
       </c>
@@ -24431,7 +24451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A105" s="8">
         <v>104</v>
       </c>
@@ -24605,7 +24625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A106" s="8">
         <v>105</v>
       </c>
@@ -24779,7 +24799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A107" s="8">
         <v>106</v>
       </c>
@@ -24953,7 +24973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A108" s="8">
         <v>107</v>
       </c>
@@ -25127,7 +25147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A109" s="8">
         <v>108</v>
       </c>
@@ -25301,7 +25321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A110" s="8">
         <v>109</v>
       </c>
@@ -25475,7 +25495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A111" s="8">
         <v>110</v>
       </c>
@@ -25649,7 +25669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A112" s="8">
         <v>111</v>
       </c>
@@ -25823,7 +25843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A113" s="8">
         <v>112</v>
       </c>
@@ -25997,7 +26017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A114" s="8">
         <v>113</v>
       </c>
@@ -26171,7 +26191,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A115" s="8">
         <v>114</v>
       </c>
@@ -26345,7 +26365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A116" s="8">
         <v>115</v>
       </c>
@@ -26519,7 +26539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A117" s="8">
         <v>116</v>
       </c>
@@ -26693,7 +26713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A118" s="8">
         <v>117</v>
       </c>
@@ -26867,7 +26887,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A119" s="8">
         <v>118</v>
       </c>
@@ -27041,7 +27061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A120" s="8">
         <v>119</v>
       </c>
@@ -27215,7 +27235,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="121" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A121" s="8">
         <v>120</v>
       </c>
@@ -27389,7 +27409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A122" s="8">
         <v>121</v>
       </c>
@@ -27563,7 +27583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A123" s="8">
         <v>122</v>
       </c>
@@ -27737,7 +27757,7 @@
         <v>66.7</v>
       </c>
     </row>
-    <row r="124" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A124" s="8">
         <v>123</v>
       </c>
@@ -27911,7 +27931,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="125" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A125" s="8">
         <v>124</v>
       </c>
@@ -28085,7 +28105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A126" s="8">
         <v>125</v>
       </c>
@@ -28259,7 +28279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A127" s="8">
         <v>126</v>
       </c>
@@ -28433,7 +28453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A128" s="8">
         <v>127</v>
       </c>
@@ -28607,7 +28627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A129" s="8">
         <v>128</v>
       </c>
@@ -28781,7 +28801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A130" s="8">
         <v>129</v>
       </c>
@@ -28955,7 +28975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A131" s="8">
         <v>130</v>
       </c>
@@ -29129,7 +29149,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A132" s="8">
         <v>131</v>
       </c>
@@ -29303,7 +29323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A133" s="8">
         <v>132</v>
       </c>
@@ -29477,7 +29497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A134" s="8">
         <v>133</v>
       </c>
@@ -29651,7 +29671,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="135" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A135" s="8">
         <v>134</v>
       </c>
@@ -29825,7 +29845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A136" s="8">
         <v>135</v>
       </c>
@@ -29999,7 +30019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A137" s="8">
         <v>136</v>
       </c>
@@ -30173,7 +30193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A138" s="8">
         <v>137</v>
       </c>
@@ -30347,7 +30367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A139" s="8">
         <v>138</v>
       </c>
@@ -30521,7 +30541,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="140" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A140" s="8">
         <v>139</v>
       </c>
@@ -30695,7 +30715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A141" s="8">
         <v>140</v>
       </c>
@@ -30869,7 +30889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A142" s="8">
         <v>141</v>
       </c>
@@ -31043,7 +31063,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="143" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A143" s="8">
         <v>142</v>
       </c>
@@ -31217,7 +31237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A144" s="8">
         <v>143</v>
       </c>
@@ -31391,7 +31411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A145" s="8">
         <v>144</v>
       </c>
@@ -31565,7 +31585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A146" s="8">
         <v>145</v>
       </c>
@@ -31739,7 +31759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A147" s="8">
         <v>146</v>
       </c>
@@ -31913,7 +31933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A148" s="8">
         <v>147</v>
       </c>
@@ -32087,7 +32107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A149" s="8">
         <v>148</v>
       </c>
@@ -32261,7 +32281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A150" s="8">
         <v>149</v>
       </c>
@@ -32435,7 +32455,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="151" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A151" s="8">
         <v>150</v>
       </c>
@@ -32609,7 +32629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A152" s="8">
         <v>151</v>
       </c>
@@ -32783,7 +32803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A153" s="8">
         <v>152</v>
       </c>
@@ -32957,7 +32977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A154" s="8">
         <v>153</v>
       </c>
@@ -33131,7 +33151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A155" s="8">
         <v>154</v>
       </c>
@@ -33305,7 +33325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A156" s="8">
         <v>155</v>
       </c>
@@ -33479,7 +33499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A157" s="8">
         <v>156</v>
       </c>
@@ -33653,7 +33673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A158" s="8">
         <v>157</v>
       </c>
@@ -33827,7 +33847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A159" s="8">
         <v>158</v>
       </c>
@@ -34001,7 +34021,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="160" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A160" s="8">
         <v>159</v>
       </c>
@@ -34175,7 +34195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A161" s="8">
         <v>160</v>
       </c>
@@ -34349,7 +34369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A162" s="8">
         <v>161</v>
       </c>
@@ -34523,7 +34543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A163" s="8">
         <v>162</v>
       </c>
@@ -34697,7 +34717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A164" s="8">
         <v>163</v>
       </c>
@@ -34871,7 +34891,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="165" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A165" s="8">
         <v>164</v>
       </c>
@@ -35045,7 +35065,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="166" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A166" s="8">
         <v>165</v>
       </c>
@@ -35219,7 +35239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A167" s="8">
         <v>166</v>
       </c>
@@ -35393,7 +35413,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="168" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A168" s="8">
         <v>167</v>
       </c>
@@ -35567,7 +35587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A169" s="8">
         <v>168</v>
       </c>
@@ -35741,7 +35761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A170" s="8">
         <v>169</v>
       </c>
@@ -35915,7 +35935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A171" s="8">
         <v>170</v>
       </c>
@@ -36089,7 +36109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A172" s="8">
         <v>800</v>
       </c>
@@ -36265,7 +36285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A173" s="8">
         <v>801</v>
       </c>
@@ -36441,7 +36461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A174" s="8">
         <v>802</v>
       </c>
@@ -36617,7 +36637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A175" s="8">
         <v>803</v>
       </c>
@@ -36793,7 +36813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A176" s="8">
         <v>804</v>
       </c>
@@ -36969,7 +36989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A177" s="8">
         <v>805</v>
       </c>
@@ -37143,7 +37163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A178" s="8">
         <v>806</v>
       </c>
@@ -37317,7 +37337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A179" s="8">
         <v>807</v>
       </c>
@@ -37491,7 +37511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A180" s="8">
         <v>808</v>
       </c>
@@ -37665,7 +37685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A181" s="8">
         <v>809</v>
       </c>
@@ -37841,7 +37861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A182" s="8">
         <v>810</v>
       </c>
@@ -38017,7 +38037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A183" s="8">
         <v>811</v>
       </c>
@@ -38193,7 +38213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A184" s="8">
         <v>812</v>
       </c>
@@ -38369,7 +38389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A185" s="8">
         <v>813</v>
       </c>
@@ -38545,7 +38565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A186" s="8">
         <v>814</v>
       </c>
@@ -38721,7 +38741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A187" s="8">
         <v>815</v>
       </c>
@@ -38897,7 +38917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A188" s="8">
         <v>816</v>
       </c>
@@ -39073,7 +39093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A189" s="8">
         <v>817</v>
       </c>
@@ -39249,7 +39269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A190" s="8">
         <v>818</v>
       </c>
@@ -39425,7 +39445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A191" s="8">
         <v>819</v>
       </c>
@@ -39599,7 +39619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A192" s="8">
         <v>820</v>
       </c>
@@ -39773,7 +39793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A193" s="8">
         <v>821</v>
       </c>
@@ -39949,7 +39969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A194" s="8">
         <v>822</v>
       </c>
@@ -40125,7 +40145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A195" s="8">
         <v>823</v>
       </c>
@@ -40301,7 +40321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A196" s="8">
         <v>824</v>
       </c>
@@ -40477,7 +40497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A197" s="8">
         <v>825</v>
       </c>
@@ -40651,7 +40671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A198" s="8">
         <v>826</v>
       </c>
@@ -40825,7 +40845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A199" s="8">
         <v>827</v>
       </c>
@@ -41001,7 +41021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A200" s="8">
         <v>828</v>
       </c>
@@ -41177,7 +41197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A201" s="8">
         <v>829</v>
       </c>
@@ -41353,7 +41373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A202" s="8">
         <v>830</v>
       </c>
@@ -41529,7 +41549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A203" s="8">
         <v>831</v>
       </c>
@@ -41705,7 +41725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A204" s="8">
         <v>832</v>
       </c>
@@ -41881,7 +41901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A205" s="8">
         <v>833</v>
       </c>
@@ -42057,7 +42077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A206" s="8">
         <v>834</v>
       </c>
@@ -42233,7 +42253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A207" s="8">
         <v>835</v>
       </c>
@@ -42407,7 +42427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A208" s="8">
         <v>836</v>
       </c>
@@ -42583,7 +42603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A209" s="8">
         <v>837</v>
       </c>
@@ -42759,7 +42779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A210" s="8">
         <v>838</v>
       </c>
@@ -42935,7 +42955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A211" s="8">
         <v>839</v>
       </c>
@@ -43111,7 +43131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A212" s="8">
         <v>840</v>
       </c>
@@ -43287,7 +43307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A213" s="8">
         <v>841</v>
       </c>
@@ -43463,7 +43483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A214" s="8">
         <v>842</v>
       </c>
@@ -43639,7 +43659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A215" s="8">
         <v>843</v>
       </c>
@@ -43815,7 +43835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A216" s="8">
         <v>844</v>
       </c>
@@ -43991,7 +44011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A217" s="8">
         <v>845</v>
       </c>
@@ -44165,7 +44185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A218" s="8">
         <v>846</v>
       </c>
@@ -44341,7 +44361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A219" s="8">
         <v>847</v>
       </c>
@@ -44517,7 +44537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A220" s="18">
         <v>900</v>
       </c>
@@ -44691,7 +44711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A221" s="18">
         <v>901</v>
       </c>
@@ -44865,7 +44885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A222" s="18">
         <v>902</v>
       </c>
@@ -45039,7 +45059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A223" s="18">
         <v>903</v>
       </c>
@@ -45213,7 +45233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A224" s="18">
         <v>904</v>
       </c>
@@ -45387,7 +45407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A225" s="18">
         <v>905</v>
       </c>
@@ -45561,7 +45581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A226" s="18">
         <v>906</v>
       </c>
@@ -45735,7 +45755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A227" s="18">
         <v>907</v>
       </c>
@@ -45909,7 +45929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A228" s="18">
         <v>908</v>
       </c>
@@ -46083,7 +46103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A229" s="18">
         <v>909</v>
       </c>
@@ -46257,7 +46277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A230" s="18">
         <v>910</v>
       </c>
@@ -46431,7 +46451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A231" s="18">
         <v>911</v>
       </c>
@@ -46605,7 +46625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A232" s="18">
         <v>912</v>
       </c>
@@ -46779,7 +46799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A233" s="18">
         <v>913</v>
       </c>
@@ -46953,7 +46973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A234" s="18">
         <v>914</v>
       </c>
@@ -47153,305 +47173,305 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
Improving model (correting SWG calculation and feasibility)
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="382">
   <si>
     <t>TODO</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>Selling Price [US$]</t>
-  </si>
-  <si>
-    <t>Linearization factor</t>
   </si>
   <si>
     <t>Algorithm</t>
@@ -4790,7 +4787,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -4839,7 +4836,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -4893,7 +4890,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -4947,7 +4944,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -5001,7 +4998,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -5055,7 +5052,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -5109,7 +5106,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -5186,9 +5183,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scenario" displayName="Scenario" ref="A1:V2" totalsRowShown="0">
-  <autoFilter ref="A1:V2"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scenario" displayName="Scenario" ref="A1:U2" totalsRowShown="0">
+  <autoFilter ref="A1:U2"/>
+  <tableColumns count="21">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Feed Scenario"/>
     <tableColumn id="3" name="Batch"/>
@@ -5203,7 +5200,6 @@
     <tableColumn id="10" name="a2"/>
     <tableColumn id="11" name="PH"/>
     <tableColumn id="12" name="Selling Price [US$]"/>
-    <tableColumn id="13" name="Linearization factor"/>
     <tableColumn id="14" name="Algorithm"/>
     <tableColumn id="15" name="Identifier"/>
     <tableColumn id="16" name="LB"/>
@@ -6021,10 +6017,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6039,16 +6035,15 @@
     <col min="11" max="11" width="6.33203125" customWidth="1"/>
     <col min="12" max="12" width="5.6640625" customWidth="1"/>
     <col min="13" max="14" width="14.109375" customWidth="1"/>
-    <col min="15" max="15" width="20.5546875" customWidth="1"/>
-    <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="17" max="17" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="8.6640625" customWidth="1"/>
-    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="1027" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="8.6640625" customWidth="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="1026" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -6065,10 +6060,10 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>28</v>
@@ -6109,14 +6104,11 @@
       <c r="T1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" t="s">
-        <v>363</v>
+      <c r="U1" t="s">
+        <v>362</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6127,7 +6119,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4">
         <v>446</v>
@@ -6159,28 +6151,25 @@
       <c r="N2" s="4">
         <v>7.9331307870370509</v>
       </c>
-      <c r="O2" s="4">
-        <v>0.87</v>
+      <c r="O2" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>0.5</v>
       </c>
       <c r="R2" s="4">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="S2" s="4">
-        <v>3</v>
-      </c>
-      <c r="T2" s="4">
         <v>0.01</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="V2" s="4">
+      <c r="T2" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="U2" s="4">
         <v>900</v>
       </c>
     </row>
@@ -6218,22 +6207,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="F1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -6241,10 +6230,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4">
         <v>5</v>
@@ -6261,10 +6250,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -6358,175 +6347,175 @@
         <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AY1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="BA1" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BB1" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BD1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BE1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BF1" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="BF1" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.3">
@@ -6534,7 +6523,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9">
@@ -6708,7 +6697,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="9">
@@ -6882,7 +6871,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9">
@@ -7056,7 +7045,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="9">
@@ -7230,7 +7219,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9">
@@ -7404,7 +7393,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9">
@@ -7578,7 +7567,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9">
@@ -7752,7 +7741,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="9">
@@ -7926,7 +7915,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9">
@@ -8100,7 +8089,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9">
@@ -8274,7 +8263,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9">
@@ -8448,7 +8437,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9">
@@ -8622,7 +8611,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9">
@@ -8796,7 +8785,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9">
@@ -8970,7 +8959,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9">
@@ -9144,7 +9133,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9">
@@ -9318,7 +9307,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9">
@@ -9492,7 +9481,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9">
@@ -9666,7 +9655,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9">
@@ -9840,7 +9829,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9">
@@ -10014,7 +10003,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9">
@@ -10188,7 +10177,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9">
@@ -10362,7 +10351,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9">
@@ -10536,7 +10525,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="9">
@@ -10710,7 +10699,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="9">
@@ -10884,7 +10873,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="9">
@@ -11058,7 +11047,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9">
@@ -11232,7 +11221,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="9">
@@ -11406,7 +11395,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="9">
@@ -11580,7 +11569,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="9">
@@ -11754,7 +11743,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="9">
@@ -11928,7 +11917,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9">
@@ -12102,7 +12091,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="9">
@@ -12276,7 +12265,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="9">
@@ -12450,7 +12439,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="9">
@@ -12624,7 +12613,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="9">
@@ -12798,7 +12787,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="9">
@@ -12972,7 +12961,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="9">
@@ -13146,7 +13135,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="9">
@@ -13320,7 +13309,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="9">
@@ -13494,7 +13483,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="9">
@@ -13668,7 +13657,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="9">
@@ -13842,7 +13831,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="9">
@@ -14016,7 +14005,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="9">
@@ -14190,7 +14179,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="9">
@@ -14364,7 +14353,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="9">
@@ -14538,7 +14527,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="9">
@@ -14712,7 +14701,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="9">
@@ -14886,7 +14875,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="9">
@@ -15060,7 +15049,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="9">
@@ -15234,7 +15223,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="9">
@@ -15408,7 +15397,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="9">
@@ -15582,7 +15571,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="9">
@@ -15756,7 +15745,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="9">
@@ -15930,7 +15919,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="9">
@@ -16104,7 +16093,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="9">
@@ -16278,7 +16267,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="9">
@@ -16452,7 +16441,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="9">
@@ -16626,7 +16615,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="9">
@@ -16800,7 +16789,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="9">
@@ -16974,7 +16963,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="9">
@@ -17148,7 +17137,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="9">
@@ -17322,7 +17311,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="9">
@@ -17496,7 +17485,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="9">
@@ -17670,7 +17659,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="9">
@@ -17844,7 +17833,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="9">
@@ -18018,7 +18007,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="9">
@@ -18192,7 +18181,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="9">
@@ -18366,7 +18355,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="9">
@@ -18540,7 +18529,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="9">
@@ -18714,7 +18703,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="9">
@@ -18888,7 +18877,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="9">
@@ -19062,7 +19051,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="9">
@@ -19236,7 +19225,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="9">
@@ -19410,7 +19399,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="9">
@@ -19584,7 +19573,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="9">
@@ -19758,7 +19747,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="9">
@@ -19932,7 +19921,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="9">
@@ -20106,7 +20095,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="9">
@@ -20280,7 +20269,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="9">
@@ -20454,7 +20443,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="9">
@@ -20628,7 +20617,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="9">
@@ -20802,7 +20791,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="9">
@@ -20976,7 +20965,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="9">
@@ -21150,7 +21139,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="9">
@@ -21324,7 +21313,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="9">
@@ -21498,7 +21487,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="9">
@@ -21672,7 +21661,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="9">
@@ -21846,7 +21835,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="9">
@@ -22020,7 +22009,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C91" s="8"/>
       <c r="D91" s="9">
@@ -22194,7 +22183,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C92" s="8"/>
       <c r="D92" s="9">
@@ -22368,7 +22357,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="9">
@@ -22542,7 +22531,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="9">
@@ -22716,7 +22705,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="9">
@@ -22890,7 +22879,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="9">
@@ -23064,7 +23053,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="9">
@@ -23238,7 +23227,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="9">
@@ -23412,7 +23401,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="9">
@@ -23586,7 +23575,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="9">
@@ -23760,7 +23749,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="9">
@@ -23934,7 +23923,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="9">
@@ -24108,7 +24097,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="9">
@@ -24282,7 +24271,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="9">
@@ -24456,7 +24445,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="9">
@@ -24630,7 +24619,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="9">
@@ -24804,7 +24793,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C107" s="8"/>
       <c r="D107" s="9">
@@ -24978,7 +24967,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C108" s="8"/>
       <c r="D108" s="9">
@@ -25152,7 +25141,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C109" s="8"/>
       <c r="D109" s="9">
@@ -25326,7 +25315,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C110" s="8"/>
       <c r="D110" s="9">
@@ -25500,7 +25489,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="9">
@@ -25674,7 +25663,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C112" s="8"/>
       <c r="D112" s="9">
@@ -25848,7 +25837,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C113" s="8"/>
       <c r="D113" s="9">
@@ -26022,7 +26011,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C114" s="8"/>
       <c r="D114" s="9">
@@ -26196,7 +26185,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C115" s="8"/>
       <c r="D115" s="9">
@@ -26370,7 +26359,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C116" s="8"/>
       <c r="D116" s="9">
@@ -26544,7 +26533,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C117" s="8"/>
       <c r="D117" s="9">
@@ -26718,7 +26707,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C118" s="8"/>
       <c r="D118" s="9">
@@ -26892,7 +26881,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="9">
@@ -27066,7 +27055,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="9">
@@ -27240,7 +27229,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="9">
@@ -27414,7 +27403,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="9">
@@ -27588,7 +27577,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="9">
@@ -27762,7 +27751,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="9">
@@ -27936,7 +27925,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C125" s="8"/>
       <c r="D125" s="9">
@@ -28110,7 +28099,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="9">
@@ -28284,7 +28273,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C127" s="8"/>
       <c r="D127" s="9">
@@ -28458,7 +28447,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C128" s="8"/>
       <c r="D128" s="9">
@@ -28632,7 +28621,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C129" s="8"/>
       <c r="D129" s="9">
@@ -28806,7 +28795,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="9">
@@ -28980,7 +28969,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="9">
@@ -29154,7 +29143,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="9">
@@ -29328,7 +29317,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C133" s="8"/>
       <c r="D133" s="9">
@@ -29502,7 +29491,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C134" s="8"/>
       <c r="D134" s="9">
@@ -29676,7 +29665,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="9">
@@ -29850,7 +29839,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="9">
@@ -30024,7 +30013,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="9">
@@ -30198,7 +30187,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="9">
@@ -30372,7 +30361,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="9">
@@ -30546,7 +30535,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="9">
@@ -30720,7 +30709,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="9">
@@ -30894,7 +30883,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C142" s="8"/>
       <c r="D142" s="9">
@@ -31068,7 +31057,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="9">
@@ -31242,7 +31231,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="9">
@@ -31416,7 +31405,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C145" s="8"/>
       <c r="D145" s="9">
@@ -31590,7 +31579,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="9">
@@ -31764,7 +31753,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C147" s="8"/>
       <c r="D147" s="9">
@@ -31938,7 +31927,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="9">
@@ -32112,7 +32101,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C149" s="8"/>
       <c r="D149" s="9">
@@ -32286,7 +32275,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="9">
@@ -32460,7 +32449,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="9">
@@ -32634,7 +32623,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="9">
@@ -32808,7 +32797,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C153" s="8"/>
       <c r="D153" s="9">
@@ -32982,7 +32971,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="9">
@@ -33156,7 +33145,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="9">
@@ -33330,7 +33319,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C156" s="8"/>
       <c r="D156" s="9">
@@ -33504,7 +33493,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="9">
@@ -33678,7 +33667,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C158" s="8"/>
       <c r="D158" s="9">
@@ -33852,7 +33841,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C159" s="8"/>
       <c r="D159" s="9">
@@ -34026,7 +34015,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C160" s="8"/>
       <c r="D160" s="9">
@@ -34200,7 +34189,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C161" s="8"/>
       <c r="D161" s="9">
@@ -34374,7 +34363,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C162" s="8"/>
       <c r="D162" s="9">
@@ -34548,7 +34537,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="9">
@@ -34722,7 +34711,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="9">
@@ -34896,7 +34885,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="9">
@@ -35070,7 +35059,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="9">
@@ -35244,7 +35233,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="9">
@@ -35418,7 +35407,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C168" s="8"/>
       <c r="D168" s="9">
@@ -35592,7 +35581,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="9">
@@ -35766,7 +35755,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="9">
@@ -35940,7 +35929,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C171" s="8"/>
       <c r="D171" s="9">
@@ -36114,10 +36103,10 @@
         <v>800</v>
       </c>
       <c r="B172" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C172" s="8" t="s">
         <v>278</v>
-      </c>
-      <c r="C172" s="8" t="s">
-        <v>279</v>
       </c>
       <c r="D172" s="9">
         <v>0</v>
@@ -36290,10 +36279,10 @@
         <v>801</v>
       </c>
       <c r="B173" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C173" s="8" t="s">
         <v>280</v>
-      </c>
-      <c r="C173" s="8" t="s">
-        <v>281</v>
       </c>
       <c r="D173" s="9">
         <v>0</v>
@@ -36466,10 +36455,10 @@
         <v>802</v>
       </c>
       <c r="B174" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C174" s="8" t="s">
         <v>282</v>
-      </c>
-      <c r="C174" s="8" t="s">
-        <v>283</v>
       </c>
       <c r="D174" s="9">
         <v>0</v>
@@ -36642,10 +36631,10 @@
         <v>803</v>
       </c>
       <c r="B175" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C175" s="8" t="s">
         <v>284</v>
-      </c>
-      <c r="C175" s="8" t="s">
-        <v>285</v>
       </c>
       <c r="D175" s="9">
         <v>0</v>
@@ -36818,10 +36807,10 @@
         <v>804</v>
       </c>
       <c r="B176" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C176" s="8" t="s">
         <v>286</v>
-      </c>
-      <c r="C176" s="8" t="s">
-        <v>287</v>
       </c>
       <c r="D176" s="9">
         <v>0</v>
@@ -36994,7 +36983,7 @@
         <v>805</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="9">
@@ -37168,7 +37157,7 @@
         <v>806</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="9">
@@ -37342,7 +37331,7 @@
         <v>807</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C179" s="8"/>
       <c r="D179" s="9">
@@ -37516,7 +37505,7 @@
         <v>808</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C180" s="8"/>
       <c r="D180" s="9">
@@ -37690,10 +37679,10 @@
         <v>809</v>
       </c>
       <c r="B181" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C181" s="8" t="s">
         <v>292</v>
-      </c>
-      <c r="C181" s="8" t="s">
-        <v>293</v>
       </c>
       <c r="D181" s="9">
         <v>0</v>
@@ -37866,10 +37855,10 @@
         <v>810</v>
       </c>
       <c r="B182" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C182" s="8" t="s">
         <v>294</v>
-      </c>
-      <c r="C182" s="8" t="s">
-        <v>295</v>
       </c>
       <c r="D182" s="9">
         <v>0</v>
@@ -38042,10 +38031,10 @@
         <v>811</v>
       </c>
       <c r="B183" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="C183" s="8" t="s">
         <v>296</v>
-      </c>
-      <c r="C183" s="8" t="s">
-        <v>297</v>
       </c>
       <c r="D183" s="9">
         <v>0</v>
@@ -38218,10 +38207,10 @@
         <v>812</v>
       </c>
       <c r="B184" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C184" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="C184" s="8" t="s">
-        <v>299</v>
       </c>
       <c r="D184" s="9">
         <v>0</v>
@@ -38394,10 +38383,10 @@
         <v>813</v>
       </c>
       <c r="B185" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C185" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="C185" s="8" t="s">
-        <v>301</v>
       </c>
       <c r="D185" s="9">
         <v>0</v>
@@ -38570,10 +38559,10 @@
         <v>814</v>
       </c>
       <c r="B186" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="C186" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C186" s="8" t="s">
-        <v>303</v>
       </c>
       <c r="D186" s="9">
         <v>0</v>
@@ -38746,10 +38735,10 @@
         <v>815</v>
       </c>
       <c r="B187" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C187" s="8" t="s">
         <v>304</v>
-      </c>
-      <c r="C187" s="8" t="s">
-        <v>305</v>
       </c>
       <c r="D187" s="9">
         <v>0</v>
@@ -38922,10 +38911,10 @@
         <v>816</v>
       </c>
       <c r="B188" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="C188" s="8" t="s">
         <v>306</v>
-      </c>
-      <c r="C188" s="8" t="s">
-        <v>307</v>
       </c>
       <c r="D188" s="9">
         <v>0</v>
@@ -39098,10 +39087,10 @@
         <v>817</v>
       </c>
       <c r="B189" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C189" s="8" t="s">
         <v>308</v>
-      </c>
-      <c r="C189" s="8" t="s">
-        <v>309</v>
       </c>
       <c r="D189" s="9">
         <v>0</v>
@@ -39274,10 +39263,10 @@
         <v>818</v>
       </c>
       <c r="B190" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="C190" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="C190" s="8" t="s">
-        <v>311</v>
       </c>
       <c r="D190" s="9">
         <v>0</v>
@@ -39450,7 +39439,7 @@
         <v>819</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="9">
@@ -39624,7 +39613,7 @@
         <v>820</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="9">
@@ -39798,10 +39787,10 @@
         <v>821</v>
       </c>
       <c r="B193" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C193" s="8" t="s">
         <v>314</v>
-      </c>
-      <c r="C193" s="8" t="s">
-        <v>315</v>
       </c>
       <c r="D193" s="9">
         <v>0</v>
@@ -39974,10 +39963,10 @@
         <v>822</v>
       </c>
       <c r="B194" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C194" s="8" t="s">
         <v>316</v>
-      </c>
-      <c r="C194" s="8" t="s">
-        <v>317</v>
       </c>
       <c r="D194" s="9">
         <v>0</v>
@@ -40150,10 +40139,10 @@
         <v>823</v>
       </c>
       <c r="B195" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="C195" s="8" t="s">
         <v>318</v>
-      </c>
-      <c r="C195" s="8" t="s">
-        <v>319</v>
       </c>
       <c r="D195" s="9">
         <v>0</v>
@@ -40326,10 +40315,10 @@
         <v>824</v>
       </c>
       <c r="B196" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="C196" s="8" t="s">
         <v>320</v>
-      </c>
-      <c r="C196" s="8" t="s">
-        <v>321</v>
       </c>
       <c r="D196" s="9">
         <v>0</v>
@@ -40502,7 +40491,7 @@
         <v>825</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="9">
@@ -40676,7 +40665,7 @@
         <v>826</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="9">
@@ -40850,10 +40839,10 @@
         <v>827</v>
       </c>
       <c r="B199" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C199" s="8" t="s">
         <v>324</v>
-      </c>
-      <c r="C199" s="8" t="s">
-        <v>325</v>
       </c>
       <c r="D199" s="9">
         <v>0</v>
@@ -41026,10 +41015,10 @@
         <v>828</v>
       </c>
       <c r="B200" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="C200" s="8" t="s">
         <v>326</v>
-      </c>
-      <c r="C200" s="8" t="s">
-        <v>327</v>
       </c>
       <c r="D200" s="9">
         <v>0</v>
@@ -41202,10 +41191,10 @@
         <v>829</v>
       </c>
       <c r="B201" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="C201" s="8" t="s">
         <v>328</v>
-      </c>
-      <c r="C201" s="8" t="s">
-        <v>329</v>
       </c>
       <c r="D201" s="9">
         <v>0</v>
@@ -41378,10 +41367,10 @@
         <v>830</v>
       </c>
       <c r="B202" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="C202" s="8" t="s">
         <v>330</v>
-      </c>
-      <c r="C202" s="8" t="s">
-        <v>331</v>
       </c>
       <c r="D202" s="9">
         <v>0</v>
@@ -41554,10 +41543,10 @@
         <v>831</v>
       </c>
       <c r="B203" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="C203" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="C203" s="8" t="s">
-        <v>333</v>
       </c>
       <c r="D203" s="9">
         <v>0</v>
@@ -41730,10 +41719,10 @@
         <v>832</v>
       </c>
       <c r="B204" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="C204" s="8" t="s">
         <v>334</v>
-      </c>
-      <c r="C204" s="8" t="s">
-        <v>335</v>
       </c>
       <c r="D204" s="9">
         <v>0</v>
@@ -41906,10 +41895,10 @@
         <v>833</v>
       </c>
       <c r="B205" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="C205" s="8" t="s">
         <v>336</v>
-      </c>
-      <c r="C205" s="8" t="s">
-        <v>337</v>
       </c>
       <c r="D205" s="9">
         <v>0</v>
@@ -42082,10 +42071,10 @@
         <v>834</v>
       </c>
       <c r="B206" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C206" s="8" t="s">
         <v>338</v>
-      </c>
-      <c r="C206" s="8" t="s">
-        <v>339</v>
       </c>
       <c r="D206" s="9">
         <v>0</v>
@@ -42258,7 +42247,7 @@
         <v>835</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C207" s="8"/>
       <c r="D207" s="9">
@@ -42432,10 +42421,10 @@
         <v>836</v>
       </c>
       <c r="B208" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C208" s="8" t="s">
         <v>341</v>
-      </c>
-      <c r="C208" s="8" t="s">
-        <v>342</v>
       </c>
       <c r="D208" s="9">
         <v>0</v>
@@ -42608,10 +42597,10 @@
         <v>837</v>
       </c>
       <c r="B209" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="C209" s="8" t="s">
         <v>343</v>
-      </c>
-      <c r="C209" s="8" t="s">
-        <v>344</v>
       </c>
       <c r="D209" s="9">
         <v>0</v>
@@ -42784,10 +42773,10 @@
         <v>838</v>
       </c>
       <c r="B210" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C210" s="8" t="s">
         <v>345</v>
-      </c>
-      <c r="C210" s="8" t="s">
-        <v>346</v>
       </c>
       <c r="D210" s="9">
         <v>0</v>
@@ -42960,10 +42949,10 @@
         <v>839</v>
       </c>
       <c r="B211" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C211" s="8" t="s">
         <v>347</v>
-      </c>
-      <c r="C211" s="8" t="s">
-        <v>348</v>
       </c>
       <c r="D211" s="9">
         <v>0</v>
@@ -43136,10 +43125,10 @@
         <v>840</v>
       </c>
       <c r="B212" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C212" s="8" t="s">
         <v>349</v>
-      </c>
-      <c r="C212" s="8" t="s">
-        <v>350</v>
       </c>
       <c r="D212" s="9">
         <v>0</v>
@@ -43312,10 +43301,10 @@
         <v>841</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D213" s="9">
         <v>0</v>
@@ -43488,10 +43477,10 @@
         <v>842</v>
       </c>
       <c r="B214" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="C214" s="8" t="s">
         <v>352</v>
-      </c>
-      <c r="C214" s="8" t="s">
-        <v>353</v>
       </c>
       <c r="D214" s="9">
         <v>0</v>
@@ -43664,10 +43653,10 @@
         <v>843</v>
       </c>
       <c r="B215" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="C215" s="8" t="s">
         <v>354</v>
-      </c>
-      <c r="C215" s="8" t="s">
-        <v>355</v>
       </c>
       <c r="D215" s="9">
         <v>0</v>
@@ -43840,10 +43829,10 @@
         <v>844</v>
       </c>
       <c r="B216" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="C216" s="8" t="s">
         <v>356</v>
-      </c>
-      <c r="C216" s="8" t="s">
-        <v>357</v>
       </c>
       <c r="D216" s="9">
         <v>0</v>
@@ -44016,7 +44005,7 @@
         <v>845</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C217" s="8"/>
       <c r="D217" s="9">
@@ -44190,10 +44179,10 @@
         <v>846</v>
       </c>
       <c r="B218" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C218" s="8" t="s">
         <v>359</v>
-      </c>
-      <c r="C218" s="8" t="s">
-        <v>360</v>
       </c>
       <c r="D218" s="9">
         <v>0</v>
@@ -44366,10 +44355,10 @@
         <v>847</v>
       </c>
       <c r="B219" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="C219" s="8" t="s">
         <v>361</v>
-      </c>
-      <c r="C219" s="8" t="s">
-        <v>362</v>
       </c>
       <c r="D219" s="9">
         <v>0</v>
@@ -44542,7 +44531,7 @@
         <v>900</v>
       </c>
       <c r="B220" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C220" s="19"/>
       <c r="D220" s="20">
@@ -44716,7 +44705,7 @@
         <v>901</v>
       </c>
       <c r="B221" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C221" s="19"/>
       <c r="D221" s="20">
@@ -44890,7 +44879,7 @@
         <v>902</v>
       </c>
       <c r="B222" s="19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C222" s="19"/>
       <c r="D222" s="20">
@@ -45064,7 +45053,7 @@
         <v>903</v>
       </c>
       <c r="B223" s="19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C223" s="19"/>
       <c r="D223" s="20">
@@ -45238,7 +45227,7 @@
         <v>904</v>
       </c>
       <c r="B224" s="19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C224" s="19"/>
       <c r="D224" s="20">
@@ -45412,7 +45401,7 @@
         <v>905</v>
       </c>
       <c r="B225" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C225" s="19"/>
       <c r="D225" s="20">
@@ -45586,7 +45575,7 @@
         <v>906</v>
       </c>
       <c r="B226" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C226" s="19"/>
       <c r="D226" s="20">
@@ -45760,7 +45749,7 @@
         <v>907</v>
       </c>
       <c r="B227" s="19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C227" s="19"/>
       <c r="D227" s="20">
@@ -45934,7 +45923,7 @@
         <v>908</v>
       </c>
       <c r="B228" s="19" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C228" s="19"/>
       <c r="D228" s="20">
@@ -46108,7 +46097,7 @@
         <v>909</v>
       </c>
       <c r="B229" s="19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C229" s="19"/>
       <c r="D229" s="20">
@@ -46282,7 +46271,7 @@
         <v>910</v>
       </c>
       <c r="B230" s="19" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C230" s="19"/>
       <c r="D230" s="20">
@@ -46456,7 +46445,7 @@
         <v>911</v>
       </c>
       <c r="B231" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C231" s="19"/>
       <c r="D231" s="20">
@@ -46630,7 +46619,7 @@
         <v>912</v>
       </c>
       <c r="B232" s="19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C232" s="19"/>
       <c r="D232" s="20">
@@ -46804,7 +46793,7 @@
         <v>913</v>
       </c>
       <c r="B233" s="19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C233" s="19"/>
       <c r="D233" s="20">
@@ -46978,7 +46967,7 @@
         <v>914</v>
       </c>
       <c r="B234" s="19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C234" s="19"/>
       <c r="D234" s="20">
@@ -47193,287 +47182,287 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Output handler creates folders 'output' and 'temp_output' if they do not exist. Correct input file. Solver changed to HiGHS.
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15228" windowHeight="6648" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TODOS" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Feed Library" sheetId="5" r:id="rId5"/>
     <sheet name="Parameters List" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="384">
   <si>
     <t>TODO</t>
   </si>
@@ -1173,9 +1173,6 @@
     <t>Ammonium Sulfate - BR</t>
   </si>
   <si>
-    <t>MinCost</t>
-  </si>
-  <si>
     <t>Only Costs Batch</t>
   </si>
   <si>
@@ -1183,6 +1180,15 @@
   </si>
   <si>
     <t>Target Weight</t>
+  </si>
+  <si>
+    <t>Time_1</t>
+  </si>
+  <si>
+    <t>Time_10</t>
+  </si>
+  <si>
+    <t>MaxProfit</t>
   </si>
 </sst>
 </file>
@@ -5183,8 +5189,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scenario" displayName="Scenario" ref="A1:U2" totalsRowShown="0">
-  <autoFilter ref="A1:U2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scenario" displayName="Scenario" ref="A1:U3" totalsRowShown="0">
+  <autoFilter ref="A1:U3"/>
   <tableColumns count="21">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Feed Scenario"/>
@@ -5728,8 +5734,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5777,7 +5783,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="4">
-        <v>1.0891396604025601</v>
+        <v>0.94766132700000005</v>
       </c>
       <c r="F2" s="3" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5798,7 +5804,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="4">
-        <v>1.5</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="F3" s="3" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5818,8 +5824,8 @@
       <c r="D4" s="4">
         <v>100</v>
       </c>
-      <c r="E4" s="1">
-        <v>1.3</v>
+      <c r="E4" s="4">
+        <v>0.78900000000000003</v>
       </c>
       <c r="F4" s="4" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -6017,10 +6023,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6060,10 +6066,10 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>28</v>
@@ -6125,7 +6131,7 @@
         <v>446</v>
       </c>
       <c r="F2" s="4">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -6155,10 +6161,10 @@
         <v>42</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="Q2" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="R2" s="4">
         <v>3</v>
@@ -6167,10 +6173,75 @@
         <v>0.01</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="U2" s="4">
-        <v>900</v>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="4">
+        <v>446</v>
+      </c>
+      <c r="F3" s="4">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>4</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>6.03</v>
+      </c>
+      <c r="N3" s="4">
+        <v>7.9331307870370509</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="R3" s="4">
+        <v>3</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="U3" s="4">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -6222,7 +6293,7 @@
         <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SBW + FSBW /2
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15228" windowHeight="6648" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15228" windowHeight="6648" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -1028,7 +1028,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
-    <numFmt numFmtId="166" formatCode="0.00;0.00;0.00;@"/>
+    <numFmt numFmtId="165" formatCode="0.00;0.00;0.00;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1164,7 +1164,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -5629,8 +5629,8 @@
   </sheetPr>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5735,7 +5735,7 @@
         <v>446</v>
       </c>
       <c r="F2" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
@@ -5799,11 +5799,8 @@
       <c r="E3" s="3">
         <v>446</v>
       </c>
-      <c r="F3" s="3">
-        <v>10</v>
-      </c>
       <c r="G3" s="3">
-        <v>0</v>
+        <v>553</v>
       </c>
       <c r="H3" s="3">
         <v>4</v>
@@ -5954,7 +5951,7 @@
   </sheetPr>
   <dimension ref="A1:S234"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update find red cost
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Documents\GitHub\EMB_MaxProfitDiet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917799B-7D7E-4EC4-A2D9-1EFF1FFAF3DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966AA7B5-B736-4274-87F4-E83C0D3B7E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="342">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -1035,178 +1035,34 @@
     <t>Peanut Meal</t>
   </si>
   <si>
-    <t>Milho</t>
-  </si>
-  <si>
-    <t>Sorgo</t>
-  </si>
-  <si>
-    <t>PolpaCitrica</t>
-  </si>
-  <si>
-    <t>FareloArroz</t>
-  </si>
-  <si>
-    <t>FareloGermenDesengordurado</t>
-  </si>
-  <si>
-    <t>FareloSoja</t>
-  </si>
-  <si>
-    <t>FareloAmendoim</t>
-  </si>
-  <si>
-    <t>FareloAlgodao</t>
-  </si>
-  <si>
-    <t>TortaAlgodao</t>
-  </si>
-  <si>
-    <t>CarocoAlgodao</t>
-  </si>
-  <si>
-    <t>DDG</t>
-  </si>
-  <si>
-    <t>MelacoSoja</t>
-  </si>
-  <si>
-    <t>CascaSoja</t>
-  </si>
-  <si>
-    <t>SilagemMilho</t>
-  </si>
-  <si>
-    <t>SilagemSorgo</t>
-  </si>
-  <si>
-    <t>SilagemCana</t>
-  </si>
-  <si>
-    <t>SilagemCapim</t>
-  </si>
-  <si>
-    <t>FenoTifton85</t>
-  </si>
-  <si>
-    <t>BagacoCana</t>
-  </si>
-  <si>
     <t>F1 Nelore x Britânicas</t>
   </si>
   <si>
-    <t>Ibitiuva.A</t>
-  </si>
-  <si>
-    <t>Barretos.A</t>
-  </si>
-  <si>
-    <t>Riolândia1.A</t>
-  </si>
-  <si>
-    <t>Riolândia2.A</t>
-  </si>
-  <si>
-    <t>Estrela D'Oeste.A</t>
-  </si>
-  <si>
-    <t>Sales1.A</t>
-  </si>
-  <si>
-    <t>Buritama.A</t>
-  </si>
-  <si>
-    <t>Sales2.A</t>
-  </si>
-  <si>
-    <t>Sabino1.A</t>
-  </si>
-  <si>
-    <t>Sabino2.A</t>
-  </si>
-  <si>
-    <t>Presidente Venceslau.A</t>
-  </si>
-  <si>
-    <t>Guarantã.A</t>
-  </si>
-  <si>
-    <t>Birigui.A</t>
-  </si>
-  <si>
-    <t>Clementina.A</t>
-  </si>
-  <si>
-    <t>Irapuã.A</t>
-  </si>
-  <si>
-    <t>Tupã.A</t>
-  </si>
-  <si>
-    <t>Ibitiuva.B</t>
-  </si>
-  <si>
     <t>MinCost</t>
   </si>
   <si>
-    <t>Barretos.B</t>
-  </si>
-  <si>
-    <t>Riolândia1.B</t>
-  </si>
-  <si>
-    <t>Riolândia2.B</t>
-  </si>
-  <si>
-    <t>Estrela D'Oeste.B</t>
-  </si>
-  <si>
-    <t>Sales1.B</t>
-  </si>
-  <si>
-    <t>Buritama.B</t>
-  </si>
-  <si>
-    <t>Sales2.B</t>
-  </si>
-  <si>
-    <t>Sabino1.B</t>
-  </si>
-  <si>
-    <t>Sabino2.B</t>
-  </si>
-  <si>
-    <t>Presidente Venceslau.B</t>
-  </si>
-  <si>
-    <t>Guarantã.B</t>
-  </si>
-  <si>
-    <t>Birigui.B</t>
-  </si>
-  <si>
-    <t>Clementina.B</t>
-  </si>
-  <si>
-    <t>Irapuã.B</t>
-  </si>
-  <si>
-    <t>Tupã.B</t>
-  </si>
-  <si>
-    <t>FeedPricesConfinaBrasil2020.csv</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>NRC1996</t>
+    <t>DMI Equation</t>
   </si>
   <si>
     <t>NRC2016</t>
   </si>
   <si>
-    <t>DMI Equation</t>
+    <t>Ingredient Lower</t>
+  </si>
+  <si>
+    <t>Ingredient Upper</t>
+  </si>
+  <si>
+    <t>Teste1</t>
+  </si>
+  <si>
+    <t>Teste2</t>
+  </si>
+  <si>
+    <t>Batch_02.csv</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -1482,7 +1338,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1510,6 +1366,22 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4925,7 +4797,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4974,7 +4846,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5028,7 +4900,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5082,7 +4954,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5136,7 +5008,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5190,7 +5062,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5244,7 +5116,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5307,9 +5179,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scenario" displayName="Scenario" ref="A1:V34" totalsRowShown="0">
-  <autoFilter ref="A1:V34" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scenario" displayName="Scenario" ref="A1:X3" totalsRowShown="0">
+  <autoFilter ref="A1:X3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Feed Scenario"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Batch"/>
@@ -5334,14 +5206,16 @@
     <tableColumn id="13" xr3:uid="{A53F67F4-C308-48B0-8F56-0EAE9F733C72}" name="DMI Equation"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Obj"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Find Reduced Cost"/>
+    <tableColumn id="23" xr3:uid="{2EB88023-A01D-4F2A-891A-411E6B928938}" name="Ingredient Lower"/>
+    <tableColumn id="24" xr3:uid="{E4EFE318-D5E2-4D25-9645-0936290C9B8C}" name="Ingredient Upper"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table6" displayName="Table6" ref="A1:F17" totalsRowShown="0">
-  <autoFilter ref="A1:F17" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table6" displayName="Table6" ref="A1:F3" totalsRowShown="0">
+  <autoFilter ref="A1:F3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Batch ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Filename"/>
@@ -5650,8 +5524,8 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5698,8 +5572,8 @@
       <c r="D2" s="3">
         <v>100</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>350</v>
+      <c r="E2" s="3">
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5719,8 +5593,8 @@
       <c r="D3" s="3">
         <v>100</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>342</v>
+      <c r="E3" s="3">
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5737,11 +5611,11 @@
       <c r="C4" s="25">
         <v>0</v>
       </c>
-      <c r="D4" s="25">
-        <v>100</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>347</v>
+      <c r="D4" s="3">
+        <v>100</v>
+      </c>
+      <c r="E4" s="25">
+        <v>1</v>
       </c>
       <c r="F4" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5758,11 +5632,11 @@
       <c r="C5" s="25">
         <v>0</v>
       </c>
-      <c r="D5" s="25">
-        <v>100</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>345</v>
+      <c r="D5" s="3">
+        <v>100</v>
+      </c>
+      <c r="E5" s="25">
+        <v>1</v>
       </c>
       <c r="F5" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5779,11 +5653,11 @@
       <c r="C6" s="25">
         <v>0</v>
       </c>
-      <c r="D6" s="25">
-        <v>100</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>334</v>
+      <c r="D6" s="3">
+        <v>100</v>
+      </c>
+      <c r="E6" s="25">
+        <v>1</v>
       </c>
       <c r="F6" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5800,11 +5674,11 @@
       <c r="C7" s="25">
         <v>0</v>
       </c>
-      <c r="D7" s="25">
-        <v>100</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>332</v>
+      <c r="D7" s="3">
+        <v>100</v>
+      </c>
+      <c r="E7" s="25">
+        <v>1</v>
       </c>
       <c r="F7" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5821,11 +5695,11 @@
       <c r="C8" s="25">
         <v>0</v>
       </c>
-      <c r="D8" s="25">
-        <v>100</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>339</v>
+      <c r="D8" s="3">
+        <v>100</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1</v>
       </c>
       <c r="F8" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5842,11 +5716,11 @@
       <c r="C9" s="25">
         <v>0</v>
       </c>
-      <c r="D9" s="25">
-        <v>100</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>341</v>
+      <c r="D9" s="3">
+        <v>100</v>
+      </c>
+      <c r="E9" s="25">
+        <v>1</v>
       </c>
       <c r="F9" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5863,11 +5737,11 @@
       <c r="C10" s="25">
         <v>0</v>
       </c>
-      <c r="D10" s="25">
-        <v>100</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>333</v>
+      <c r="D10" s="3">
+        <v>100</v>
+      </c>
+      <c r="E10" s="25">
+        <v>1</v>
       </c>
       <c r="F10" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5884,11 +5758,11 @@
       <c r="C11" s="25">
         <v>0</v>
       </c>
-      <c r="D11" s="25">
-        <v>100</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>344</v>
+      <c r="D11" s="3">
+        <v>100</v>
+      </c>
+      <c r="E11" s="25">
+        <v>1</v>
       </c>
       <c r="F11" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5905,11 +5779,11 @@
       <c r="C12" s="25">
         <v>0</v>
       </c>
-      <c r="D12" s="25">
-        <v>100</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>337</v>
+      <c r="D12" s="3">
+        <v>100</v>
+      </c>
+      <c r="E12" s="25">
+        <v>1</v>
       </c>
       <c r="F12" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5926,12 +5800,11 @@
       <c r="C13" s="25">
         <v>0</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="3">
         <v>100</v>
       </c>
       <c r="E13" s="25">
-        <f>2960/1000</f>
-        <v>2.96</v>
+        <v>1</v>
       </c>
       <c r="F13" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5948,11 +5821,11 @@
       <c r="C14" s="25">
         <v>0</v>
       </c>
-      <c r="D14" s="25">
-        <v>100</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>340</v>
+      <c r="D14" s="3">
+        <v>100</v>
+      </c>
+      <c r="E14" s="25">
+        <v>1</v>
       </c>
       <c r="F14" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5969,11 +5842,11 @@
       <c r="C15" s="25">
         <v>0</v>
       </c>
-      <c r="D15" s="25">
-        <v>100</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>343</v>
+      <c r="D15" s="3">
+        <v>100</v>
+      </c>
+      <c r="E15" s="25">
+        <v>1</v>
       </c>
       <c r="F15" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5990,11 +5863,11 @@
       <c r="C16" s="25">
         <v>0</v>
       </c>
-      <c r="D16" s="25">
-        <v>100</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>325</v>
+      <c r="D16" s="3">
+        <v>100</v>
+      </c>
+      <c r="E16" s="25">
+        <v>1</v>
       </c>
       <c r="F16" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -6011,11 +5884,11 @@
       <c r="C17" s="25">
         <v>0</v>
       </c>
-      <c r="D17" s="25">
-        <v>100</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>336</v>
+      <c r="D17" s="3">
+        <v>100</v>
+      </c>
+      <c r="E17" s="25">
+        <v>1</v>
       </c>
       <c r="F17" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -6032,11 +5905,11 @@
       <c r="C18" s="25">
         <v>0</v>
       </c>
-      <c r="D18" s="25">
-        <v>100</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>348</v>
+      <c r="D18" s="3">
+        <v>100</v>
+      </c>
+      <c r="E18" s="25">
+        <v>1</v>
       </c>
       <c r="F18" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -6053,11 +5926,11 @@
       <c r="C19" s="25">
         <v>0</v>
       </c>
-      <c r="D19" s="25">
-        <v>100</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>346</v>
+      <c r="D19" s="3">
+        <v>100</v>
+      </c>
+      <c r="E19" s="25">
+        <v>1</v>
       </c>
       <c r="F19" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -6074,11 +5947,11 @@
       <c r="C20" s="25">
         <v>0</v>
       </c>
-      <c r="D20" s="25">
-        <v>100</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>349</v>
+      <c r="D20" s="3">
+        <v>100</v>
+      </c>
+      <c r="E20" s="25">
+        <v>1</v>
       </c>
       <c r="F20" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -6095,11 +5968,11 @@
       <c r="C21" s="25">
         <v>0</v>
       </c>
-      <c r="D21" s="25">
-        <v>100</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>335</v>
+      <c r="D21" s="3">
+        <v>100</v>
+      </c>
+      <c r="E21" s="25">
+        <v>1</v>
       </c>
       <c r="F21" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -6116,11 +5989,11 @@
       <c r="C22" s="25">
         <v>0</v>
       </c>
-      <c r="D22" s="25">
-        <v>100</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>338</v>
+      <c r="D22" s="3">
+        <v>100</v>
+      </c>
+      <c r="E22" s="25">
+        <v>1</v>
       </c>
       <c r="F22" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -6150,34 +6023,42 @@
   <sheetPr codeName="Planilha2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
-    <col min="6" max="7" width="7.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
-    <col min="13" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="1027" width="8.7109375" customWidth="1"/>
+    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="1027" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6236,7 +6117,7 @@
         <v>20</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>389</v>
+        <v>334</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>21</v>
@@ -6244,8 +6125,14 @@
       <c r="V1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W1" t="s">
+        <v>336</v>
+      </c>
+      <c r="X1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -6256,28 +6143,28 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="E2" s="3">
-        <v>384</v>
+        <v>350</v>
       </c>
       <c r="F2" s="3">
         <v>0</v>
       </c>
       <c r="G2" s="3">
-        <v>528</v>
+        <v>550</v>
       </c>
       <c r="H2" s="3">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="I2" s="3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="J2" s="3">
         <v>1</v>
       </c>
       <c r="K2" s="3">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="L2" s="3">
         <v>0</v>
@@ -6286,25 +6173,25 @@
         <v>6.03</v>
       </c>
       <c r="N2" s="3">
-        <v>8.7083333333333339</v>
+        <v>8</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="Q2" s="3">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="R2" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S2" s="3">
         <v>0.01</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>387</v>
+        <v>335</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>322</v>
@@ -6312,40 +6199,46 @@
       <c r="V2" s="3">
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E3" s="3">
+        <v>350</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>550</v>
+      </c>
+      <c r="H3" s="3">
+        <v>4</v>
+      </c>
+      <c r="I3" s="3">
         <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E3" s="3">
-        <v>384</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>528</v>
-      </c>
-      <c r="H3" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.95</v>
       </c>
       <c r="J3" s="3">
         <v>1</v>
       </c>
       <c r="K3" s="3">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="L3" s="3">
         <v>0</v>
@@ -6354,2155 +6247,37 @@
         <v>6.03</v>
       </c>
       <c r="N3" s="3">
-        <v>8.7083333333333339</v>
+        <v>8</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>388</v>
+        <v>339</v>
       </c>
       <c r="Q3" s="3">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="R3" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S3" s="3">
         <v>0.01</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>388</v>
+        <v>335</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="V3" s="3">
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="W3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="X3" s="3">
         <v>1</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E4" s="3">
-        <v>381.12</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>556.79999999999995</v>
-      </c>
-      <c r="H4" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1</v>
-      </c>
-      <c r="K4" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N4" s="3">
-        <v>8.7541666666666664</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R4" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S4" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V4" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>3</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E5" s="3">
-        <v>341.76</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>528.96</v>
-      </c>
-      <c r="H5" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N5" s="3">
-        <v>8.7083333333333339</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R5" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V5" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E6" s="3">
-        <v>345.6</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>480</v>
-      </c>
-      <c r="H6" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J6" s="3">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N6" s="3">
-        <v>8.3263888888888893</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R6" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S6" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V6" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E7" s="3">
-        <v>384</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>537.6</v>
-      </c>
-      <c r="H7" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N7" s="3">
-        <v>8.4791666666666661</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R7" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S7" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V7" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E8" s="3">
-        <v>384</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>528</v>
-      </c>
-      <c r="H8" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J8" s="3">
-        <v>1</v>
-      </c>
-      <c r="K8" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N8" s="3">
-        <v>8.5555555555555554</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R8" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S8" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V8" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E9" s="3">
-        <v>345.6</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>480</v>
-      </c>
-      <c r="H9" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J9" s="3">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N9" s="3">
-        <v>8.25</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R9" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S9" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V9" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>8</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E10" s="3">
-        <v>384</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>499.2</v>
-      </c>
-      <c r="H10" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J10" s="3">
-        <v>1</v>
-      </c>
-      <c r="K10" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L10" s="3">
-        <v>0</v>
-      </c>
-      <c r="M10" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N10" s="3">
-        <v>8.25</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R10" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S10" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V10" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E11" s="3">
-        <v>361.92</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>504</v>
-      </c>
-      <c r="H11" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J11" s="3">
-        <v>1</v>
-      </c>
-      <c r="K11" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0</v>
-      </c>
-      <c r="M11" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N11" s="3">
-        <v>8.6472222222222221</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R11" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S11" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V11" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E12" s="3">
-        <v>384</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>537.6</v>
-      </c>
-      <c r="H12" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J12" s="3">
-        <v>1</v>
-      </c>
-      <c r="K12" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L12" s="3">
-        <v>0</v>
-      </c>
-      <c r="M12" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N12" s="3">
-        <v>8.7083333333333339</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R12" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S12" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V12" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>11</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E13" s="3">
-        <v>288</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>441.6</v>
-      </c>
-      <c r="H13" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J13" s="3">
-        <v>1</v>
-      </c>
-      <c r="K13" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N13" s="3">
-        <v>8.5250000000000004</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R13" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S13" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V13" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E14" s="3">
-        <v>355.2</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>537.6</v>
-      </c>
-      <c r="H14" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I14" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J14" s="3">
-        <v>1</v>
-      </c>
-      <c r="K14" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L14" s="3">
-        <v>0</v>
-      </c>
-      <c r="M14" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N14" s="3">
-        <v>8.4027777777777786</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R14" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S14" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V14" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3">
-        <v>13</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E15" s="3">
-        <v>326.39999999999998</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>489.6</v>
-      </c>
-      <c r="H15" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J15" s="3">
-        <v>1</v>
-      </c>
-      <c r="K15" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L15" s="3">
-        <v>0</v>
-      </c>
-      <c r="M15" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N15" s="3">
-        <v>8.4027777777777786</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R15" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S15" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U15" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V15" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3">
-        <v>14</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E16" s="3">
-        <v>345.6</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>537.6</v>
-      </c>
-      <c r="H16" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J16" s="3">
-        <v>1</v>
-      </c>
-      <c r="K16" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L16" s="3">
-        <v>0</v>
-      </c>
-      <c r="M16" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N16" s="3">
-        <v>8.4791666666666661</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R16" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S16" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U16" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V16" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3">
-        <v>15</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E17" s="3">
-        <v>364.8</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>528</v>
-      </c>
-      <c r="H17" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I17" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J17" s="3">
-        <v>1</v>
-      </c>
-      <c r="K17" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L17" s="3">
-        <v>0</v>
-      </c>
-      <c r="M17" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N17" s="3">
-        <v>8.6319444444444446</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R17" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S17" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T17" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U17" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V17" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3">
-        <v>16</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E18" s="3">
-        <v>366.72</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>464.64</v>
-      </c>
-      <c r="H18" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J18" s="3">
-        <v>1</v>
-      </c>
-      <c r="K18" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L18" s="3">
-        <v>0</v>
-      </c>
-      <c r="M18" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N18" s="3">
-        <v>8.3263888888888893</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="R18" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="S18" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T18" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U18" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="V18" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E19" s="3">
-        <v>384</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>528</v>
-      </c>
-      <c r="H19" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="K19" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L19" s="3">
-        <v>0</v>
-      </c>
-      <c r="M19" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N19" s="3">
-        <v>8.7083333333333339</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>1.84</v>
-      </c>
-      <c r="R19" s="3">
-        <f>Q19+2*S19</f>
-        <v>1.86</v>
-      </c>
-      <c r="S19" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U19" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V19" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E20" s="3">
-        <v>381.12</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <v>556.79999999999995</v>
-      </c>
-      <c r="H20" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J20" s="3">
-        <v>1</v>
-      </c>
-      <c r="K20" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L20" s="3">
-        <v>0</v>
-      </c>
-      <c r="M20" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N20" s="3">
-        <v>8.7541666666666664</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>1.81</v>
-      </c>
-      <c r="R20" s="3">
-        <f t="shared" ref="R20:R34" si="0">Q20+2*S20</f>
-        <v>1.83</v>
-      </c>
-      <c r="S20" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T20" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U20" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V20" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3">
-        <v>3</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E21" s="3">
-        <v>341.76</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>528.96</v>
-      </c>
-      <c r="H21" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J21" s="3">
-        <v>1</v>
-      </c>
-      <c r="K21" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L21" s="3">
-        <v>0</v>
-      </c>
-      <c r="M21" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N21" s="3">
-        <v>8.7083333333333339</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="Q21" s="3">
-        <v>1.85</v>
-      </c>
-      <c r="R21" s="3">
-        <f t="shared" si="0"/>
-        <v>1.87</v>
-      </c>
-      <c r="S21" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T21" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U21" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V21" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E22" s="3">
-        <v>345.6</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0</v>
-      </c>
-      <c r="G22" s="3">
-        <v>480</v>
-      </c>
-      <c r="H22" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J22" s="3">
-        <v>1</v>
-      </c>
-      <c r="K22" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L22" s="3">
-        <v>0</v>
-      </c>
-      <c r="M22" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N22" s="3">
-        <v>8.3263888888888893</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>1.78</v>
-      </c>
-      <c r="R22" s="3">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="S22" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T22" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U22" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V22" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3">
-        <v>5</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E23" s="3">
-        <v>384</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0</v>
-      </c>
-      <c r="G23" s="3">
-        <v>537.6</v>
-      </c>
-      <c r="H23" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J23" s="3">
-        <v>1</v>
-      </c>
-      <c r="K23" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L23" s="3">
-        <v>0</v>
-      </c>
-      <c r="M23" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N23" s="3">
-        <v>8.4791666666666661</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="Q23" s="3">
-        <v>1.95</v>
-      </c>
-      <c r="R23" s="3">
-        <f t="shared" si="0"/>
-        <v>1.97</v>
-      </c>
-      <c r="S23" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T23" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U23" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V23" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3">
-        <v>6</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E24" s="3">
-        <v>384</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0</v>
-      </c>
-      <c r="G24" s="3">
-        <v>528</v>
-      </c>
-      <c r="H24" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I24" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J24" s="3">
-        <v>1</v>
-      </c>
-      <c r="K24" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L24" s="3">
-        <v>0</v>
-      </c>
-      <c r="M24" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N24" s="3">
-        <v>8.5555555555555554</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="Q24" s="3">
-        <v>1.92</v>
-      </c>
-      <c r="R24" s="3">
-        <f t="shared" si="0"/>
-        <v>1.94</v>
-      </c>
-      <c r="S24" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T24" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U24" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V24" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3">
-        <v>7</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E25" s="3">
-        <v>345.6</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0</v>
-      </c>
-      <c r="G25" s="3">
-        <v>480</v>
-      </c>
-      <c r="H25" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J25" s="3">
-        <v>1</v>
-      </c>
-      <c r="K25" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L25" s="3">
-        <v>0</v>
-      </c>
-      <c r="M25" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N25" s="3">
-        <v>8.25</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q25" s="3">
-        <v>1.87</v>
-      </c>
-      <c r="R25" s="3">
-        <f t="shared" si="0"/>
-        <v>1.8900000000000001</v>
-      </c>
-      <c r="S25" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T25" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U25" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V25" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
-        <v>8</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E26" s="3">
-        <v>384</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0</v>
-      </c>
-      <c r="G26" s="3">
-        <v>499.2</v>
-      </c>
-      <c r="H26" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I26" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J26" s="3">
-        <v>1</v>
-      </c>
-      <c r="K26" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L26" s="3">
-        <v>0</v>
-      </c>
-      <c r="M26" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N26" s="3">
-        <v>8.25</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P26" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q26" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="R26" s="3">
-        <f t="shared" si="0"/>
-        <v>1.77</v>
-      </c>
-      <c r="S26" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T26" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U26" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V26" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3">
-        <v>9</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E27" s="3">
-        <v>361.92</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0</v>
-      </c>
-      <c r="G27" s="3">
-        <v>504</v>
-      </c>
-      <c r="H27" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I27" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J27" s="3">
-        <v>1</v>
-      </c>
-      <c r="K27" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L27" s="3">
-        <v>0</v>
-      </c>
-      <c r="M27" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N27" s="3">
-        <v>8.6472222222222221</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="Q27" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="R27" s="3">
-        <f t="shared" si="0"/>
-        <v>1.82</v>
-      </c>
-      <c r="S27" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U27" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V27" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3">
-        <v>10</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E28" s="3">
-        <v>384</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0</v>
-      </c>
-      <c r="G28" s="3">
-        <v>537.6</v>
-      </c>
-      <c r="H28" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I28" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J28" s="3">
-        <v>1</v>
-      </c>
-      <c r="K28" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L28" s="3">
-        <v>0</v>
-      </c>
-      <c r="M28" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N28" s="3">
-        <v>8.7083333333333339</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P28" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="Q28" s="3">
-        <v>1.69</v>
-      </c>
-      <c r="R28" s="3">
-        <f t="shared" si="0"/>
-        <v>1.71</v>
-      </c>
-      <c r="S28" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U28" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V28" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3">
-        <v>11</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E29" s="3">
-        <v>288</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3">
-        <v>441.6</v>
-      </c>
-      <c r="H29" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I29" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J29" s="3">
-        <v>1</v>
-      </c>
-      <c r="K29" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L29" s="3">
-        <v>0</v>
-      </c>
-      <c r="M29" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N29" s="3">
-        <v>8.5250000000000004</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="Q29" s="3">
-        <v>1.84</v>
-      </c>
-      <c r="R29" s="3">
-        <f t="shared" si="0"/>
-        <v>1.86</v>
-      </c>
-      <c r="S29" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U29" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V29" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B30" s="3">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3">
-        <v>12</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E30" s="3">
-        <v>355.2</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0</v>
-      </c>
-      <c r="G30" s="3">
-        <v>537.6</v>
-      </c>
-      <c r="H30" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I30" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J30" s="3">
-        <v>1</v>
-      </c>
-      <c r="K30" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L30" s="3">
-        <v>0</v>
-      </c>
-      <c r="M30" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N30" s="3">
-        <v>8.4027777777777786</v>
-      </c>
-      <c r="O30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q30" s="3">
-        <v>1.85</v>
-      </c>
-      <c r="R30" s="3">
-        <f t="shared" si="0"/>
-        <v>1.87</v>
-      </c>
-      <c r="S30" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T30" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U30" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V30" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>13</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E31" s="3">
-        <v>326.39999999999998</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0</v>
-      </c>
-      <c r="G31" s="3">
-        <v>489.6</v>
-      </c>
-      <c r="H31" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I31" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J31" s="3">
-        <v>1</v>
-      </c>
-      <c r="K31" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L31" s="3">
-        <v>0</v>
-      </c>
-      <c r="M31" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N31" s="3">
-        <v>8.4027777777777786</v>
-      </c>
-      <c r="O31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P31" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="Q31" s="3">
-        <v>1.58</v>
-      </c>
-      <c r="R31" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6</v>
-      </c>
-      <c r="S31" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T31" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U31" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V31" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>14</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E32" s="3">
-        <v>345.6</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0</v>
-      </c>
-      <c r="G32" s="3">
-        <v>537.6</v>
-      </c>
-      <c r="H32" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I32" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J32" s="3">
-        <v>1</v>
-      </c>
-      <c r="K32" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L32" s="3">
-        <v>0</v>
-      </c>
-      <c r="M32" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N32" s="3">
-        <v>8.4791666666666661</v>
-      </c>
-      <c r="O32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P32" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="Q32" s="3">
-        <v>1.87</v>
-      </c>
-      <c r="R32" s="3">
-        <f t="shared" si="0"/>
-        <v>1.8900000000000001</v>
-      </c>
-      <c r="S32" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T32" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U32" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V32" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3">
-        <v>15</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E33" s="3">
-        <v>364.8</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0</v>
-      </c>
-      <c r="G33" s="3">
-        <v>528</v>
-      </c>
-      <c r="H33" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I33" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J33" s="3">
-        <v>1</v>
-      </c>
-      <c r="K33" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L33" s="3">
-        <v>0</v>
-      </c>
-      <c r="M33" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N33" s="3">
-        <v>8.6319444444444446</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P33" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="Q33" s="3">
-        <v>1.93</v>
-      </c>
-      <c r="R33" s="3">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
-      </c>
-      <c r="S33" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T33" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U33" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V33" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3">
-        <v>16</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E34" s="3">
-        <v>366.72</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0</v>
-      </c>
-      <c r="G34" s="3">
-        <v>464.64</v>
-      </c>
-      <c r="H34" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I34" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="J34" s="3">
-        <v>1</v>
-      </c>
-      <c r="K34" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L34" s="3">
-        <v>0</v>
-      </c>
-      <c r="M34" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N34" s="3">
-        <v>8.3263888888888893</v>
-      </c>
-      <c r="O34" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P34" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="Q34" s="3">
-        <v>1.76</v>
-      </c>
-      <c r="R34" s="3">
-        <f t="shared" si="0"/>
-        <v>1.78</v>
-      </c>
-      <c r="S34" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T34" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="U34" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="V34" s="3">
-        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -8521,10 +6296,10 @@
   <sheetPr codeName="Planilha3">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F17"/>
+      <selection activeCell="A4" sqref="A4:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8563,16 +6338,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>385</v>
+        <v>340</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>386</v>
+        <v>341</v>
       </c>
       <c r="D2" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3">
         <v>0</v>
@@ -8583,299 +6358,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>385</v>
+        <v>340</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>386</v>
+        <v>341</v>
       </c>
       <c r="D3" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3">
-        <v>4</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D6" s="3">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>5</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D7" s="3">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3">
-        <v>6</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D8" s="3">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D9" s="3">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3">
-        <v>8</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D10" s="3">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3">
-        <v>9</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D11" s="3">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D12" s="3">
-        <v>11</v>
-      </c>
-      <c r="E12" s="3">
-        <v>11</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D13" s="3">
-        <v>12</v>
-      </c>
-      <c r="E13" s="3">
-        <v>12</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D14" s="3">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3">
-        <v>13</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D15" s="3">
-        <v>14</v>
-      </c>
-      <c r="E15" s="3">
-        <v>14</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D16" s="3">
-        <v>15</v>
-      </c>
-      <c r="E16" s="3">
-        <v>15</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D17" s="3">
-        <v>16</v>
-      </c>
-      <c r="E17" s="3">
-        <v>16</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update search reduced costs
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Documents\GitHub\EMB_MaxProfitDiet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966AA7B5-B736-4274-87F4-E83C0D3B7E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6864AD9C-1EE4-435B-BBAA-04DFEC8583E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="340">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -969,18 +969,12 @@
     <t>Citrus Pulp - BR</t>
   </si>
   <si>
-    <t>Corn, grain - BR</t>
-  </si>
-  <si>
     <t>Cottonseed Meal 38% - BR</t>
   </si>
   <si>
     <t>Cottonseed Whole - BR</t>
   </si>
   <si>
-    <t>Sorghum, grain or Milo - BR</t>
-  </si>
-  <si>
     <t>Soybean Hulls - BR</t>
   </si>
   <si>
@@ -1026,9 +1020,6 @@
     <t>Sorghum Silage</t>
   </si>
   <si>
-    <t>Tifton 85, hay</t>
-  </si>
-  <si>
     <t>Rice Bran</t>
   </si>
   <si>
@@ -1038,31 +1029,34 @@
     <t>F1 Nelore x Britânicas</t>
   </si>
   <si>
-    <t>MinCost</t>
-  </si>
-  <si>
     <t>DMI Equation</t>
   </si>
   <si>
     <t>NRC2016</t>
   </si>
   <si>
-    <t>Ingredient Lower</t>
-  </si>
-  <si>
-    <t>Ingredient Upper</t>
-  </si>
-  <si>
     <t>Teste1</t>
   </si>
   <si>
-    <t>Teste2</t>
-  </si>
-  <si>
     <t>Batch_02.csv</t>
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>Corn grain - BR</t>
+  </si>
+  <si>
+    <t>Sorghum grain or Milo - BR</t>
+  </si>
+  <si>
+    <t>Tifton 85 hay</t>
+  </si>
+  <si>
+    <t>Ingredient Level</t>
+  </si>
+  <si>
+    <t>citrus_pulp</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1332,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1366,22 +1360,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4797,7 +4775,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4846,7 +4824,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4900,7 +4878,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4954,7 +4932,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5008,7 +4986,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5062,7 +5040,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5116,7 +5094,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5179,9 +5157,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scenario" displayName="Scenario" ref="A1:X3" totalsRowShown="0">
-  <autoFilter ref="A1:X3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scenario" displayName="Scenario" ref="A1:W2" totalsRowShown="0">
+  <autoFilter ref="A1:W2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Feed Scenario"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Batch"/>
@@ -5206,8 +5184,7 @@
     <tableColumn id="13" xr3:uid="{A53F67F4-C308-48B0-8F56-0EAE9F733C72}" name="DMI Equation"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Obj"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Find Reduced Cost"/>
-    <tableColumn id="23" xr3:uid="{2EB88023-A01D-4F2A-891A-411E6B928938}" name="Ingredient Lower"/>
-    <tableColumn id="24" xr3:uid="{E4EFE318-D5E2-4D25-9645-0936290C9B8C}" name="Ingredient Upper"/>
+    <tableColumn id="23" xr3:uid="{2EB88023-A01D-4F2A-891A-411E6B928938}" name="Ingredient Level"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5524,8 +5501,8 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5573,7 +5550,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="3">
-        <v>1</v>
+        <v>0.19131799999999999</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5656,8 +5633,8 @@
       <c r="D6" s="3">
         <v>100</v>
       </c>
-      <c r="E6" s="25">
-        <v>1</v>
+      <c r="E6" s="25" t="s">
+        <v>339</v>
       </c>
       <c r="F6" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -5682,7 +5659,7 @@
       </c>
       <c r="F7" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
-        <v>Corn, grain - BR</v>
+        <v>Corn grain - BR</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -5745,7 +5722,7 @@
       </c>
       <c r="F10" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
-        <v>Sorghum, grain or Milo - BR</v>
+        <v>Sorghum grain or Milo - BR</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -5955,7 +5932,7 @@
       </c>
       <c r="F20" s="25" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
-        <v>Tifton 85, hay</v>
+        <v>Tifton 85 hay</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -6023,10 +6000,10 @@
   <sheetPr codeName="Planilha2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6054,11 +6031,10 @@
     <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="1027" width="8.7109375" customWidth="1"/>
+    <col min="24" max="1026" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6075,10 +6051,10 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>
@@ -6117,7 +6093,7 @@
         <v>20</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>21</v>
@@ -6126,13 +6102,10 @@
         <v>303</v>
       </c>
       <c r="W1" t="s">
-        <v>336</v>
-      </c>
-      <c r="X1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -6140,10 +6113,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E2" s="3">
         <v>350</v>
@@ -6179,7 +6152,7 @@
         <v>22</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="Q2" s="3">
         <v>0.8</v>
@@ -6191,93 +6164,16 @@
         <v>0.01</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="V2" s="3">
-        <v>-1</v>
+        <v>900</v>
       </c>
       <c r="W2" s="1">
         <v>0.1</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="E3" s="3">
-        <v>350</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>550</v>
-      </c>
-      <c r="H3" s="3">
-        <v>4</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3">
-        <v>1</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N3" s="3">
-        <v>8</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="R3" s="3">
-        <v>3</v>
-      </c>
-      <c r="S3" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="V3" s="3">
-        <v>-1</v>
-      </c>
-      <c r="W3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="X3" s="3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6330,7 +6226,7 @@
         <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -6338,10 +6234,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D2" s="3">
         <v>5</v>
@@ -6358,10 +6254,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D3" s="3">
         <v>4</v>
@@ -6389,8 +6285,8 @@
   </sheetPr>
   <dimension ref="A1:S243"/>
   <sheetViews>
-    <sheetView topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B229" sqref="B229"/>
+    <sheetView topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B238" sqref="B238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19696,7 +19592,7 @@
         <v>906</v>
       </c>
       <c r="B226" s="16" t="s">
-        <v>310</v>
+        <v>335</v>
       </c>
       <c r="C226" s="17">
         <v>0</v>
@@ -19755,7 +19651,7 @@
         <v>907</v>
       </c>
       <c r="B227" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C227" s="17">
         <v>0</v>
@@ -19814,7 +19710,7 @@
         <v>908</v>
       </c>
       <c r="B228" s="16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C228" s="17">
         <v>0</v>
@@ -19873,7 +19769,7 @@
         <v>909</v>
       </c>
       <c r="B229" s="16" t="s">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="C229" s="17">
         <v>0</v>
@@ -19932,7 +19828,7 @@
         <v>910</v>
       </c>
       <c r="B230" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C230" s="17">
         <v>0</v>
@@ -19991,7 +19887,7 @@
         <v>911</v>
       </c>
       <c r="B231" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C231" s="17">
         <v>0</v>
@@ -20050,7 +19946,7 @@
         <v>912</v>
       </c>
       <c r="B232" s="16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C232" s="17">
         <v>0</v>
@@ -20109,7 +20005,7 @@
         <v>913</v>
       </c>
       <c r="B233" s="16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C233" s="17">
         <v>0</v>
@@ -20168,7 +20064,7 @@
         <v>914</v>
       </c>
       <c r="B234" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C234" s="17">
         <v>0</v>
@@ -20227,7 +20123,7 @@
         <v>915</v>
       </c>
       <c r="B235" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C235" s="24">
         <v>0</v>
@@ -20278,7 +20174,7 @@
         <v>916</v>
       </c>
       <c r="B236" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C236" s="24">
         <v>0</v>
@@ -20329,7 +20225,7 @@
         <v>917</v>
       </c>
       <c r="B237" s="23" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C237" s="24">
         <v>25</v>
@@ -20380,7 +20276,7 @@
         <v>918</v>
       </c>
       <c r="B238" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C238" s="24">
         <v>0</v>
@@ -20431,7 +20327,7 @@
         <v>919</v>
       </c>
       <c r="B239" s="23" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C239" s="24">
         <v>100</v>
@@ -20482,7 +20378,7 @@
         <v>920</v>
       </c>
       <c r="B240" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C240" s="24">
         <v>40</v>
@@ -20533,7 +20429,7 @@
         <v>921</v>
       </c>
       <c r="B241" s="23" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="C241" s="24">
         <v>100</v>
@@ -20580,7 +20476,7 @@
         <v>922</v>
       </c>
       <c r="B242" s="23" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C242" s="24">
         <v>0</v>
@@ -20629,7 +20525,7 @@
         <v>923</v>
       </c>
       <c r="B243" s="30" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C243" s="31">
         <v>0</v>

</xml_diff>

<commit_message>
Merge with working develop
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="14490" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="14496" windowHeight="11160" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -509,7 +509,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="142">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -932,6 +932,9 @@
   </si>
   <si>
     <t>GSS-MAX_BIS</t>
+  </si>
+  <si>
+    <t>NPN, %DM</t>
   </si>
 </sst>
 </file>
@@ -941,7 +944,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1044,6 +1047,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1187,7 +1196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1265,12 +1274,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="56">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1377,6 +1389,27 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -6165,10 +6198,10 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Feed Scenario"/>
-    <tableColumn id="2" name="ID" dataDxfId="50"/>
-    <tableColumn id="3" name="Min %DM" dataDxfId="49"/>
-    <tableColumn id="4" name="Max %DM" dataDxfId="48"/>
-    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="47"/>
+    <tableColumn id="2" name="ID" dataDxfId="53"/>
+    <tableColumn id="3" name="Min %DM" dataDxfId="52"/>
+    <tableColumn id="4" name="Max %DM" dataDxfId="51"/>
+    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="50"/>
     <tableColumn id="6" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6176,33 +6209,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47">
   <autoFilter ref="A1:X7"/>
   <tableColumns count="24">
-    <tableColumn id="1" name="ID" dataDxfId="43"/>
-    <tableColumn id="2" name="Feed Scenario" dataDxfId="42"/>
-    <tableColumn id="3" name="Batch" dataDxfId="41"/>
-    <tableColumn id="4" name="Breed" dataDxfId="40"/>
-    <tableColumn id="5" name="SBW" dataDxfId="39"/>
-    <tableColumn id="6" name="Feeding Time" dataDxfId="38"/>
-    <tableColumn id="7" name="Target Weight" dataDxfId="37"/>
-    <tableColumn id="8" name="BCS" dataDxfId="36"/>
-    <tableColumn id="9" name="BE" dataDxfId="35"/>
-    <tableColumn id="10" name="L" dataDxfId="34"/>
-    <tableColumn id="11" name="SEX" dataDxfId="33"/>
-    <tableColumn id="12" name="a2" dataDxfId="32"/>
-    <tableColumn id="13" name="PH" dataDxfId="31"/>
-    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="30"/>
-    <tableColumn id="15" name="Algorithm" dataDxfId="29"/>
-    <tableColumn id="16" name="Identifier" dataDxfId="28"/>
-    <tableColumn id="17" name="LB" dataDxfId="27"/>
-    <tableColumn id="18" name="UB" dataDxfId="26"/>
-    <tableColumn id="19" name="Tol" dataDxfId="25"/>
-    <tableColumn id="20" name="DMI Equation" dataDxfId="24"/>
-    <tableColumn id="21" name="Obj" dataDxfId="23"/>
-    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="22"/>
-    <tableColumn id="23" name="Ingredient Level" dataDxfId="21"/>
-    <tableColumn id="24" name="LCA ID" dataDxfId="20"/>
+    <tableColumn id="1" name="ID" dataDxfId="46"/>
+    <tableColumn id="2" name="Feed Scenario" dataDxfId="45"/>
+    <tableColumn id="3" name="Batch" dataDxfId="44"/>
+    <tableColumn id="4" name="Breed" dataDxfId="43"/>
+    <tableColumn id="5" name="SBW" dataDxfId="42"/>
+    <tableColumn id="6" name="Feeding Time" dataDxfId="41"/>
+    <tableColumn id="7" name="Target Weight" dataDxfId="40"/>
+    <tableColumn id="8" name="BCS" dataDxfId="39"/>
+    <tableColumn id="9" name="BE" dataDxfId="38"/>
+    <tableColumn id="10" name="L" dataDxfId="37"/>
+    <tableColumn id="11" name="SEX" dataDxfId="36"/>
+    <tableColumn id="12" name="a2" dataDxfId="35"/>
+    <tableColumn id="13" name="PH" dataDxfId="34"/>
+    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="33"/>
+    <tableColumn id="15" name="Algorithm" dataDxfId="32"/>
+    <tableColumn id="16" name="Identifier" dataDxfId="31"/>
+    <tableColumn id="17" name="LB" dataDxfId="30"/>
+    <tableColumn id="18" name="UB" dataDxfId="29"/>
+    <tableColumn id="19" name="Tol" dataDxfId="28"/>
+    <tableColumn id="20" name="DMI Equation" dataDxfId="27"/>
+    <tableColumn id="21" name="Obj" dataDxfId="26"/>
+    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="25"/>
+    <tableColumn id="23" name="Ingredient Level" dataDxfId="24"/>
+    <tableColumn id="24" name="LCA ID" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6224,12 +6257,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:S22" totalsRowShown="0">
-  <autoFilter ref="A1:S22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:T22" totalsRowShown="0">
+  <autoFilter ref="A1:T22"/>
   <sortState ref="A2:S22">
     <sortCondition ref="A1:A22"/>
   </sortState>
-  <tableColumns count="19">
+  <tableColumns count="20">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Feed"/>
     <tableColumn id="5" name="Forage, %DM"/>
@@ -6249,6 +6282,7 @@
     <tableColumn id="20" name="NEga, Mcal/kg"/>
     <tableColumn id="21" name="RUP, %CP"/>
     <tableColumn id="29" name="pef, %NDF"/>
+    <tableColumn id="3" name="NPN, %DM" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6565,18 +6599,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="6" width="29.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6596,7 +6630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -6617,7 +6651,7 @@
         <v>UREA</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -6638,7 +6672,7 @@
         <v>Sugar beet pulp dehydrated</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -6659,7 +6693,7 @@
         <v>Corn gluten feed</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>1</v>
       </c>
@@ -6680,7 +6714,7 @@
         <v>Corn gluten meal (gluten 60)</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>1</v>
       </c>
@@ -6701,7 +6735,7 @@
         <v>Faba bean dehulled</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -6722,7 +6756,7 @@
         <v>Molasses</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>1</v>
       </c>
@@ -6743,7 +6777,7 @@
         <v>Rapeseed meal</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>1</v>
       </c>
@@ -6764,7 +6798,7 @@
         <v>Rapeseed oil</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>1</v>
       </c>
@@ -6785,7 +6819,7 @@
         <v>Soybean extruded</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>1</v>
       </c>
@@ -6806,7 +6840,7 @@
         <v>Sunflower meal low dehulling</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>1</v>
       </c>
@@ -6827,7 +6861,7 @@
         <v>Sunflower meal without dehulling</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>1</v>
       </c>
@@ -6848,7 +6882,7 @@
         <v>Sunflower meal high dehulling</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>1</v>
       </c>
@@ -6869,7 +6903,7 @@
         <v>Sunflower meal</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>1</v>
       </c>
@@ -6890,7 +6924,7 @@
         <v>Sunflower oil without dehulling</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>1</v>
       </c>
@@ -6911,7 +6945,7 @@
         <v>Wheat bran</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>1</v>
       </c>
@@ -6932,7 +6966,7 @@
         <v>DDGS Wheat</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>1</v>
       </c>
@@ -6953,7 +6987,7 @@
         <v>Wheat feed flour</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>1</v>
       </c>
@@ -6974,7 +7008,7 @@
         <v>Wheat gluten feed</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17">
         <v>1</v>
       </c>
@@ -6995,7 +7029,7 @@
         <v>Wheat middlings</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
         <v>1</v>
       </c>
@@ -7016,7 +7050,7 @@
         <v>Grass silage, horizontal silo, temporary meadow, with clover, Northwestern region, at farm/FR S</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>1</v>
       </c>
@@ -7039,10 +7073,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B20:B22 B2:B17">
-    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="1" stopIfTrue="1">
       <formula>ROW(B2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="2" stopIfTrue="1">
       <formula>COLUMN(B2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7062,39 +7096,39 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.28515625" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.33203125" customWidth="1"/>
+    <col min="17" max="17" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
@@ -7168,9 +7202,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="32">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B2" s="32">
         <v>1</v>
@@ -7242,7 +7276,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="32">
         <v>-1</v>
       </c>
@@ -7316,7 +7350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="32">
         <v>-1</v>
       </c>
@@ -7390,7 +7424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="32">
         <v>-1</v>
       </c>
@@ -7464,9 +7498,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="32">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B6" s="35">
         <v>1</v>
@@ -7538,7 +7572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="32">
         <v>-1</v>
       </c>
@@ -7633,18 +7667,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="7" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -7664,7 +7698,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -7684,7 +7718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -7718,36 +7752,36 @@
   <sheetPr codeName="Planilha4">
     <tabColor rgb="FFE7E6E6"/>
   </sheetPr>
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125"/>
-    <col min="19" max="19" width="11.85546875" customWidth="1"/>
-    <col min="20" max="986" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625"/>
+    <col min="19" max="19" width="11.88671875" customWidth="1"/>
+    <col min="20" max="986" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -7805,8 +7839,11 @@
       <c r="S1" s="14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -7864,8 +7901,11 @@
       <c r="S2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="5">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>4</v>
       </c>
@@ -7923,8 +7963,11 @@
       <c r="S3" s="5">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" s="5">
+        <v>0.79379999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>5</v>
       </c>
@@ -7982,8 +8025,11 @@
       <c r="S4" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="5">
+        <v>5.1840000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <v>6</v>
       </c>
@@ -8041,8 +8087,11 @@
       <c r="S5" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="5">
+        <v>0.20960000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>7</v>
       </c>
@@ -8100,8 +8149,11 @@
       <c r="S6" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="5">
+        <v>0.23250000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>8</v>
       </c>
@@ -8159,8 +8211,11 @@
       <c r="S7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="5">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>9</v>
       </c>
@@ -8218,8 +8273,11 @@
       <c r="S8" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="5">
+        <v>4.3574999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>10</v>
       </c>
@@ -8277,8 +8335,11 @@
       <c r="S9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>11</v>
       </c>
@@ -8336,8 +8397,11 @@
       <c r="S10" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="5">
+        <v>0.41078399999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>12</v>
       </c>
@@ -8395,8 +8459,11 @@
       <c r="S11" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="5">
+        <v>3.1954500000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>13</v>
       </c>
@@ -8454,8 +8521,11 @@
       <c r="S12" s="5">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="5">
+        <v>1.7570870000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>14</v>
       </c>
@@ -8513,8 +8583,11 @@
       <c r="S13" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="5">
+        <v>2.0746440000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>15</v>
       </c>
@@ -8572,8 +8645,11 @@
       <c r="S14" s="5">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" s="5">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>16</v>
       </c>
@@ -8631,8 +8707,11 @@
       <c r="S15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>17</v>
       </c>
@@ -8690,8 +8769,11 @@
       <c r="S16" s="5">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="5">
+        <v>2.0910000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>18</v>
       </c>
@@ -8749,8 +8831,11 @@
       <c r="S17" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="5">
+        <v>0.45674999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>19</v>
       </c>
@@ -8808,8 +8893,11 @@
       <c r="S18" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>20</v>
       </c>
@@ -8867,8 +8955,11 @@
       <c r="S19" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="5">
+        <v>2.6532</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>21</v>
       </c>
@@ -8926,8 +9017,11 @@
       <c r="S20" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="5">
+        <v>2.2067999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="28">
         <v>24</v>
       </c>
@@ -8985,8 +9079,11 @@
       <c r="S21" s="5">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="5">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="28">
         <v>25</v>
       </c>
@@ -9044,38 +9141,58 @@
       <c r="S22" s="22">
         <v>95</v>
       </c>
+      <c r="T22" s="5">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="K27" s="51"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="K29" s="51"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="K30" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B18:S19 B20 A20:A22 A2:S17">
-    <cfRule type="expression" dxfId="19" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="3" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="4" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:R20">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
       <formula>ROW(N20)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
       <formula>COLUMN(N20)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20">
-    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="7" stopIfTrue="1">
       <formula>ROW(S20)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="8" stopIfTrue="1">
       <formula>COLUMN(S20)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
       <formula>COLUMN(C20)=$F$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
       <formula>ROW(C20)=$E$1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2:T22">
+    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
+      <formula>ROW(T2)=$C$1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="2" stopIfTrue="1">
+      <formula>COLUMN(T2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -9097,17 +9214,17 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="25.42578125" style="37" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" style="37" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="37" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="37"/>
+    <col min="2" max="7" width="25.44140625" style="37" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" style="37" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="37" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9139,7 +9256,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9171,7 +9288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9209,7 +9326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9247,7 +9364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9279,7 +9396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9329,16 +9446,16 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="21.7109375" style="38"/>
-    <col min="10" max="11" width="21.7109375" style="38" customWidth="1"/>
-    <col min="12" max="16384" width="21.7109375" style="38"/>
+    <col min="2" max="2" width="39.109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="21.6640625" style="38"/>
+    <col min="10" max="11" width="21.6640625" style="38" customWidth="1"/>
+    <col min="12" max="16384" width="21.6640625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
@@ -9364,7 +9481,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -9390,7 +9507,7 @@
         <v>0.29275619000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>4</v>
       </c>
@@ -9416,7 +9533,7 @@
         <v>0.55197054999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>5</v>
       </c>
@@ -9442,7 +9559,7 @@
         <v>0.43937693999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <v>6</v>
       </c>
@@ -9468,7 +9585,7 @@
         <v>2.0767392</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>7</v>
       </c>
@@ -9494,7 +9611,7 @@
         <v>2.4169052999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>8</v>
       </c>
@@ -9520,7 +9637,7 @@
         <v>0.25908868000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>9</v>
       </c>
@@ -9546,7 +9663,7 @@
         <v>1.2147266999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>10</v>
       </c>
@@ -9572,7 +9689,7 @@
         <v>5.7683147000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>11</v>
       </c>
@@ -9598,7 +9715,7 @@
         <v>3.8084742</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>12</v>
       </c>
@@ -9624,7 +9741,7 @@
         <v>1.9759963</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>13</v>
       </c>
@@ -9650,7 +9767,7 @@
         <v>1.6645894999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>14</v>
       </c>
@@ -9676,7 +9793,7 @@
         <v>1.9759963</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>15</v>
       </c>
@@ -9702,7 +9819,7 @@
         <v>1.6645894999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>16</v>
       </c>
@@ -9728,7 +9845,7 @@
         <v>8.7067530000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>17</v>
       </c>
@@ -9754,7 +9871,7 @@
         <v>0.62333822000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>18</v>
       </c>
@@ -9780,7 +9897,7 @@
         <v>0.97791181999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>19</v>
       </c>
@@ -9806,7 +9923,7 @@
         <v>0.33293109999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>20</v>
       </c>
@@ -9832,7 +9949,7 @@
         <v>0.86067262</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>21</v>
       </c>
@@ -9858,7 +9975,7 @@
         <v>0.29167724</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="28">
         <v>24</v>
       </c>
@@ -9884,7 +10001,7 @@
         <v>1.1594272000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28">
         <v>25</v>
       </c>
@@ -9910,7 +10027,7 @@
         <v>1.448909</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="37"/>
       <c r="D23" s="37"/>
       <c r="E23" s="37"/>
@@ -9919,7 +10036,7 @@
       <c r="H23" s="37"/>
       <c r="I23" s="37"/>
     </row>
-    <row r="24" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="37"/>
       <c r="D24" s="37"/>
       <c r="E24" s="37"/>
@@ -9928,7 +10045,7 @@
       <c r="H24" s="37"/>
       <c r="I24" s="37"/>
     </row>
-    <row r="25" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="37"/>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>
@@ -9937,7 +10054,7 @@
       <c r="H25" s="37"/>
       <c r="I25" s="37"/>
     </row>
-    <row r="26" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="37"/>
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
@@ -9946,7 +10063,7 @@
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>
     </row>
-    <row r="27" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="37"/>
       <c r="D27" s="37"/>
       <c r="E27" s="37"/>
@@ -9955,7 +10072,7 @@
       <c r="H27" s="37"/>
       <c r="I27" s="37"/>
     </row>
-    <row r="28" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="37"/>
       <c r="D28" s="37"/>
       <c r="E28" s="37"/>
@@ -9964,7 +10081,7 @@
       <c r="H28" s="37"/>
       <c r="I28" s="37"/>
     </row>
-    <row r="29" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="37"/>
       <c r="E29" s="37"/>
       <c r="F29" s="37"/>
@@ -9972,7 +10089,7 @@
       <c r="H29" s="37"/>
       <c r="I29" s="37"/>
     </row>
-    <row r="30" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="37"/>
       <c r="E30" s="37"/>
       <c r="F30" s="37"/>
@@ -9980,7 +10097,7 @@
       <c r="H30" s="37"/>
       <c r="I30" s="37"/>
     </row>
-    <row r="31" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="37"/>
       <c r="D31" s="37"/>
       <c r="E31" s="37"/>
@@ -10015,298 +10132,298 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Input commit before merge
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="14496" windowHeight="11160" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="14490" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -509,7 +509,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -932,9 +932,6 @@
   </si>
   <si>
     <t>GSS-MAX_BIS</t>
-  </si>
-  <si>
-    <t>NPN, %DM</t>
   </si>
 </sst>
 </file>
@@ -944,7 +941,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1047,12 +1044,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1196,7 +1187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1229,7 +1220,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1274,15 +1264,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="53">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1389,27 +1377,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -6198,10 +6165,10 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Feed Scenario"/>
-    <tableColumn id="2" name="ID" dataDxfId="53"/>
-    <tableColumn id="3" name="Min %DM" dataDxfId="52"/>
-    <tableColumn id="4" name="Max %DM" dataDxfId="51"/>
-    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="50"/>
+    <tableColumn id="2" name="ID" dataDxfId="50"/>
+    <tableColumn id="3" name="Min %DM" dataDxfId="49"/>
+    <tableColumn id="4" name="Max %DM" dataDxfId="48"/>
+    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="47"/>
     <tableColumn id="6" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6209,33 +6176,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
   <autoFilter ref="A1:X7"/>
   <tableColumns count="24">
-    <tableColumn id="1" name="ID" dataDxfId="46"/>
-    <tableColumn id="2" name="Feed Scenario" dataDxfId="45"/>
-    <tableColumn id="3" name="Batch" dataDxfId="44"/>
-    <tableColumn id="4" name="Breed" dataDxfId="43"/>
-    <tableColumn id="5" name="SBW" dataDxfId="42"/>
-    <tableColumn id="6" name="Feeding Time" dataDxfId="41"/>
-    <tableColumn id="7" name="Target Weight" dataDxfId="40"/>
-    <tableColumn id="8" name="BCS" dataDxfId="39"/>
-    <tableColumn id="9" name="BE" dataDxfId="38"/>
-    <tableColumn id="10" name="L" dataDxfId="37"/>
-    <tableColumn id="11" name="SEX" dataDxfId="36"/>
-    <tableColumn id="12" name="a2" dataDxfId="35"/>
-    <tableColumn id="13" name="PH" dataDxfId="34"/>
-    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="33"/>
-    <tableColumn id="15" name="Algorithm" dataDxfId="32"/>
-    <tableColumn id="16" name="Identifier" dataDxfId="31"/>
-    <tableColumn id="17" name="LB" dataDxfId="30"/>
-    <tableColumn id="18" name="UB" dataDxfId="29"/>
-    <tableColumn id="19" name="Tol" dataDxfId="28"/>
-    <tableColumn id="20" name="DMI Equation" dataDxfId="27"/>
-    <tableColumn id="21" name="Obj" dataDxfId="26"/>
-    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="25"/>
-    <tableColumn id="23" name="Ingredient Level" dataDxfId="24"/>
-    <tableColumn id="24" name="LCA ID" dataDxfId="23"/>
+    <tableColumn id="1" name="ID" dataDxfId="43"/>
+    <tableColumn id="2" name="Feed Scenario" dataDxfId="42"/>
+    <tableColumn id="3" name="Batch" dataDxfId="41"/>
+    <tableColumn id="4" name="Breed" dataDxfId="40"/>
+    <tableColumn id="5" name="SBW" dataDxfId="39"/>
+    <tableColumn id="6" name="Feeding Time" dataDxfId="38"/>
+    <tableColumn id="7" name="Target Weight" dataDxfId="37"/>
+    <tableColumn id="8" name="BCS" dataDxfId="36"/>
+    <tableColumn id="9" name="BE" dataDxfId="35"/>
+    <tableColumn id="10" name="L" dataDxfId="34"/>
+    <tableColumn id="11" name="SEX" dataDxfId="33"/>
+    <tableColumn id="12" name="a2" dataDxfId="32"/>
+    <tableColumn id="13" name="PH" dataDxfId="31"/>
+    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="30"/>
+    <tableColumn id="15" name="Algorithm" dataDxfId="29"/>
+    <tableColumn id="16" name="Identifier" dataDxfId="28"/>
+    <tableColumn id="17" name="LB" dataDxfId="27"/>
+    <tableColumn id="18" name="UB" dataDxfId="26"/>
+    <tableColumn id="19" name="Tol" dataDxfId="25"/>
+    <tableColumn id="20" name="DMI Equation" dataDxfId="24"/>
+    <tableColumn id="21" name="Obj" dataDxfId="23"/>
+    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="22"/>
+    <tableColumn id="23" name="Ingredient Level" dataDxfId="21"/>
+    <tableColumn id="24" name="LCA ID" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6257,12 +6224,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:T22" totalsRowShown="0">
-  <autoFilter ref="A1:T22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:S22" totalsRowShown="0">
+  <autoFilter ref="A1:S22"/>
   <sortState ref="A2:S22">
     <sortCondition ref="A1:A22"/>
   </sortState>
-  <tableColumns count="20">
+  <tableColumns count="19">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Feed"/>
     <tableColumn id="5" name="Forage, %DM"/>
@@ -6282,7 +6249,6 @@
     <tableColumn id="20" name="NEga, Mcal/kg"/>
     <tableColumn id="21" name="RUP, %CP"/>
     <tableColumn id="29" name="pef, %NDF"/>
-    <tableColumn id="3" name="NPN, %DM" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6595,22 +6561,22 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="6" width="29.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
-    <col min="8" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6630,28 +6596,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="26">
-        <v>0</v>
-      </c>
-      <c r="D2" s="26">
+      <c r="C2" s="19">
+        <v>0</v>
+      </c>
+      <c r="D2" s="19">
         <v>4</v>
       </c>
-      <c r="E2" s="27">
-        <v>0.4</v>
+      <c r="E2" s="50">
+        <v>0.39</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>UREA</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -6672,7 +6638,7 @@
         <v>Sugar beet pulp dehydrated</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -6693,7 +6659,7 @@
         <v>Corn gluten feed</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>1</v>
       </c>
@@ -6714,7 +6680,7 @@
         <v>Corn gluten meal (gluten 60)</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>1</v>
       </c>
@@ -6735,7 +6701,7 @@
         <v>Faba bean dehulled</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -6756,7 +6722,7 @@
         <v>Molasses</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>1</v>
       </c>
@@ -6777,7 +6743,7 @@
         <v>Rapeseed meal</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>1</v>
       </c>
@@ -6798,7 +6764,7 @@
         <v>Rapeseed oil</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>1</v>
       </c>
@@ -6819,7 +6785,7 @@
         <v>Soybean extruded</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>1</v>
       </c>
@@ -6840,7 +6806,7 @@
         <v>Sunflower meal low dehulling</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>1</v>
       </c>
@@ -6861,7 +6827,7 @@
         <v>Sunflower meal without dehulling</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>1</v>
       </c>
@@ -6882,7 +6848,7 @@
         <v>Sunflower meal high dehulling</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>1</v>
       </c>
@@ -6903,7 +6869,7 @@
         <v>Sunflower meal</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>1</v>
       </c>
@@ -6924,7 +6890,7 @@
         <v>Sunflower oil without dehulling</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>1</v>
       </c>
@@ -6945,7 +6911,7 @@
         <v>Wheat bran</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>1</v>
       </c>
@@ -6966,7 +6932,7 @@
         <v>DDGS Wheat</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>1</v>
       </c>
@@ -6987,7 +6953,7 @@
         <v>Wheat feed flour</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>1</v>
       </c>
@@ -7008,7 +6974,7 @@
         <v>Wheat gluten feed</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>1</v>
       </c>
@@ -7029,11 +6995,11 @@
         <v>Wheat middlings</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>1</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="27">
         <v>24</v>
       </c>
       <c r="C21" s="20">
@@ -7042,7 +7008,7 @@
       <c r="D21" s="20">
         <v>100</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="26">
         <v>0.3</v>
       </c>
       <c r="F21" s="17" t="str">
@@ -7050,11 +7016,11 @@
         <v>Grass silage, horizontal silo, temporary meadow, with clover, Northwestern region, at farm/FR S</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>1</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="27">
         <v>25</v>
       </c>
       <c r="C22" s="20">
@@ -7063,7 +7029,7 @@
       <c r="D22" s="20">
         <v>100</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="26">
         <v>0.3</v>
       </c>
       <c r="F22" s="17" t="str">
@@ -7073,10 +7039,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B20:B22 B2:B17">
-    <cfRule type="expression" dxfId="55" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
       <formula>ROW(B2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
       <formula>COLUMN(B2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7097,552 +7063,552 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.33203125" customWidth="1"/>
-    <col min="17" max="17" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.28515625" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="X1" s="44" t="s">
+      <c r="X1" s="43" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="32">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="31">
         <v>1</v>
       </c>
-      <c r="C2" s="32">
-        <v>0</v>
-      </c>
-      <c r="D2" s="32" t="s">
+      <c r="C2" s="31">
+        <v>0</v>
+      </c>
+      <c r="D2" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="31">
         <v>375</v>
       </c>
-      <c r="F2" s="32">
-        <v>0</v>
-      </c>
-      <c r="G2" s="31">
+      <c r="F2" s="31">
+        <v>0</v>
+      </c>
+      <c r="G2" s="30">
         <v>620</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H2" s="31">
         <v>5</v>
       </c>
-      <c r="I2" s="32">
+      <c r="I2" s="31">
         <v>1</v>
       </c>
-      <c r="J2" s="32">
+      <c r="J2" s="31">
         <v>1</v>
       </c>
-      <c r="K2" s="32">
+      <c r="K2" s="31">
         <v>1</v>
       </c>
-      <c r="L2" s="32">
-        <v>0</v>
-      </c>
-      <c r="M2" s="32">
+      <c r="L2" s="31">
+        <v>0</v>
+      </c>
+      <c r="M2" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N2" s="33">
+      <c r="N2" s="32">
         <v>2.02</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="P2" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="Q2" s="32">
+      <c r="Q2" s="31">
         <v>0.8</v>
       </c>
-      <c r="R2" s="32">
+      <c r="R2" s="31">
         <v>3</v>
       </c>
-      <c r="S2" s="32">
+      <c r="S2" s="31">
         <v>0.01</v>
       </c>
-      <c r="T2" s="32" t="s">
+      <c r="T2" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="U2" s="32" t="s">
+      <c r="U2" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="V2" s="32">
-        <v>0</v>
-      </c>
-      <c r="W2" s="32">
+      <c r="V2" s="31">
+        <v>0</v>
+      </c>
+      <c r="W2" s="31">
         <v>0.1</v>
       </c>
-      <c r="X2" s="31">
+      <c r="X2" s="30">
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3" s="32">
-        <v>-1</v>
-      </c>
-      <c r="B3" s="35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="31">
+        <v>2</v>
+      </c>
+      <c r="B3" s="34">
         <v>1</v>
       </c>
-      <c r="C3" s="32">
-        <v>0</v>
-      </c>
-      <c r="D3" s="35" t="s">
+      <c r="C3" s="31">
+        <v>0</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="34">
         <v>375</v>
       </c>
-      <c r="F3" s="32">
-        <v>0</v>
-      </c>
-      <c r="G3" s="34">
+      <c r="F3" s="31">
+        <v>0</v>
+      </c>
+      <c r="G3" s="33">
         <v>620</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="34">
         <v>5</v>
       </c>
-      <c r="I3" s="35">
+      <c r="I3" s="34">
         <v>1</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="34">
         <v>1</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3" s="34">
         <v>1</v>
       </c>
-      <c r="L3" s="35">
-        <v>0</v>
-      </c>
-      <c r="M3" s="32">
+      <c r="L3" s="34">
+        <v>0</v>
+      </c>
+      <c r="M3" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N3" s="33">
+      <c r="N3" s="32">
         <v>2.02</v>
       </c>
-      <c r="O3" s="35" t="s">
+      <c r="O3" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="P3" s="35" t="s">
+      <c r="P3" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="Q3" s="32">
+      <c r="Q3" s="31">
         <v>1.6</v>
       </c>
-      <c r="R3" s="35">
+      <c r="R3" s="34">
         <v>1.9990000000000001</v>
       </c>
-      <c r="S3" s="35">
+      <c r="S3" s="34">
         <v>0.01</v>
       </c>
-      <c r="T3" s="35" t="s">
+      <c r="T3" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="35" t="s">
+      <c r="U3" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="V3" s="35">
-        <v>0</v>
-      </c>
-      <c r="W3" s="35">
+      <c r="V3" s="34">
+        <v>0</v>
+      </c>
+      <c r="W3" s="34">
         <v>0.1</v>
       </c>
-      <c r="X3" s="34">
+      <c r="X3" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="32">
-        <v>-1</v>
-      </c>
-      <c r="B4" s="35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34">
         <v>1</v>
       </c>
-      <c r="C4" s="32">
-        <v>0</v>
-      </c>
-      <c r="D4" s="35" t="s">
+      <c r="C4" s="31">
+        <v>0</v>
+      </c>
+      <c r="D4" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="34">
         <v>375</v>
       </c>
-      <c r="F4" s="32">
-        <v>0</v>
-      </c>
-      <c r="G4" s="34">
+      <c r="F4" s="31">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
         <v>620</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="34">
         <v>5</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="34">
         <v>1</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="34">
         <v>1</v>
       </c>
-      <c r="K4" s="35">
+      <c r="K4" s="34">
         <v>1</v>
       </c>
-      <c r="L4" s="35">
-        <v>0</v>
-      </c>
-      <c r="M4" s="32">
+      <c r="L4" s="34">
+        <v>0</v>
+      </c>
+      <c r="M4" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="32">
         <v>2.02</v>
       </c>
-      <c r="O4" s="35" t="s">
+      <c r="O4" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="P4" s="35" t="s">
+      <c r="P4" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="Q4" s="32">
+      <c r="Q4" s="31">
         <v>1.6</v>
       </c>
-      <c r="R4" s="35">
+      <c r="R4" s="34">
         <v>1.9990000000000001</v>
       </c>
-      <c r="S4" s="35">
+      <c r="S4" s="34">
         <v>0.01</v>
       </c>
-      <c r="T4" s="35" t="s">
+      <c r="T4" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="U4" s="35" t="s">
+      <c r="U4" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="V4" s="35">
-        <v>0</v>
-      </c>
-      <c r="W4" s="35">
+      <c r="V4" s="34">
+        <v>0</v>
+      </c>
+      <c r="W4" s="34">
         <v>0.1</v>
       </c>
-      <c r="X4" s="34">
+      <c r="X4" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="32">
-        <v>-1</v>
-      </c>
-      <c r="B5" s="32">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>4</v>
+      </c>
+      <c r="B5" s="31">
         <v>1</v>
       </c>
-      <c r="C5" s="32">
-        <v>0</v>
-      </c>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="31">
+        <v>0</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <v>375</v>
       </c>
-      <c r="F5" s="32">
-        <v>0</v>
-      </c>
-      <c r="G5" s="31">
+      <c r="F5" s="31">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
         <v>620</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="31">
         <v>5</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="31">
         <v>1</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="31">
         <v>1</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="31">
         <v>1</v>
       </c>
-      <c r="L5" s="32">
-        <v>0</v>
-      </c>
-      <c r="M5" s="32">
+      <c r="L5" s="31">
+        <v>0</v>
+      </c>
+      <c r="M5" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="32">
         <v>2.02</v>
       </c>
-      <c r="O5" s="32" t="s">
+      <c r="O5" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="P5" s="32" t="s">
+      <c r="P5" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="Q5" s="32">
+      <c r="Q5" s="31">
         <v>1.6</v>
       </c>
-      <c r="R5" s="35">
+      <c r="R5" s="34">
         <v>1.9990000000000001</v>
       </c>
-      <c r="S5" s="35">
+      <c r="S5" s="34">
         <v>0.01</v>
       </c>
-      <c r="T5" s="32" t="s">
+      <c r="T5" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="U5" s="32" t="s">
+      <c r="U5" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="V5" s="32">
-        <v>0</v>
-      </c>
-      <c r="W5" s="32">
+      <c r="V5" s="31">
+        <v>0</v>
+      </c>
+      <c r="W5" s="31">
         <v>0.1</v>
       </c>
-      <c r="X5" s="31">
+      <c r="X5" s="30">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="32">
-        <v>-1</v>
-      </c>
-      <c r="B6" s="35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
+        <v>5</v>
+      </c>
+      <c r="B6" s="34">
         <v>1</v>
       </c>
-      <c r="C6" s="32">
-        <v>0</v>
-      </c>
-      <c r="D6" s="35" t="s">
+      <c r="C6" s="31">
+        <v>0</v>
+      </c>
+      <c r="D6" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="34">
         <v>375</v>
       </c>
-      <c r="F6" s="32">
-        <v>0</v>
-      </c>
-      <c r="G6" s="34">
+      <c r="F6" s="31">
+        <v>0</v>
+      </c>
+      <c r="G6" s="33">
         <v>620</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="34">
         <v>5</v>
       </c>
-      <c r="I6" s="35">
+      <c r="I6" s="34">
         <v>1</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="34">
         <v>1</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="34">
         <v>1</v>
       </c>
-      <c r="L6" s="35">
-        <v>0</v>
-      </c>
-      <c r="M6" s="32">
+      <c r="L6" s="34">
+        <v>0</v>
+      </c>
+      <c r="M6" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N6" s="33">
+      <c r="N6" s="32">
         <v>2.02</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="Q6" s="32">
+      <c r="Q6" s="31">
         <v>1.6</v>
       </c>
-      <c r="R6" s="35">
+      <c r="R6" s="34">
         <v>1.9990000000000001</v>
       </c>
-      <c r="S6" s="35">
+      <c r="S6" s="34">
         <v>0.01</v>
       </c>
-      <c r="T6" s="35" t="s">
+      <c r="T6" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="U6" s="35" t="s">
+      <c r="U6" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="V6" s="35">
-        <v>0</v>
-      </c>
-      <c r="W6" s="35">
+      <c r="V6" s="34">
+        <v>0</v>
+      </c>
+      <c r="W6" s="34">
         <v>0.1</v>
       </c>
-      <c r="X6" s="34">
+      <c r="X6" s="33">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="32">
-        <v>-1</v>
-      </c>
-      <c r="B7" s="30">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>6</v>
+      </c>
+      <c r="B7" s="29">
         <v>1</v>
       </c>
-      <c r="C7" s="32">
-        <v>0</v>
-      </c>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="31">
+        <v>0</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>375</v>
       </c>
-      <c r="F7" s="32">
-        <v>0</v>
-      </c>
-      <c r="G7" s="29">
+      <c r="F7" s="31">
+        <v>0</v>
+      </c>
+      <c r="G7" s="28">
         <v>620</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="29">
         <v>5</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="29">
         <v>1</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="29">
         <v>1</v>
       </c>
-      <c r="K7" s="30">
+      <c r="K7" s="29">
         <v>1</v>
       </c>
-      <c r="L7" s="30">
-        <v>0</v>
-      </c>
-      <c r="M7" s="32">
+      <c r="L7" s="29">
+        <v>0</v>
+      </c>
+      <c r="M7" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="32">
         <v>2.02</v>
       </c>
-      <c r="O7" s="30" t="s">
+      <c r="O7" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="P7" s="30" t="s">
+      <c r="P7" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="Q7" s="32">
+      <c r="Q7" s="31">
         <v>1.6</v>
       </c>
-      <c r="R7" s="35">
+      <c r="R7" s="34">
         <v>1.9990000000000001</v>
       </c>
-      <c r="S7" s="35">
+      <c r="S7" s="34">
         <v>0.01</v>
       </c>
-      <c r="T7" s="30" t="s">
+      <c r="T7" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="U7" s="30" t="s">
+      <c r="U7" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="V7" s="30">
-        <v>0</v>
-      </c>
-      <c r="W7" s="30">
+      <c r="V7" s="29">
+        <v>0</v>
+      </c>
+      <c r="W7" s="29">
         <v>0.1</v>
       </c>
-      <c r="X7" s="29">
+      <c r="X7" s="28">
         <v>5</v>
       </c>
     </row>
@@ -7667,18 +7633,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="7" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -7698,7 +7664,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -7718,7 +7684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -7752,36 +7718,36 @@
   <sheetPr codeName="Planilha4">
     <tabColor rgb="FFE7E6E6"/>
   </sheetPr>
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
-    <col min="9" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625"/>
-    <col min="19" max="19" width="11.88671875" customWidth="1"/>
-    <col min="20" max="986" width="8.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125"/>
+    <col min="19" max="19" width="11.85546875" customWidth="1"/>
+    <col min="20" max="986" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -7839,11 +7805,8 @@
       <c r="S1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="T1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -7901,11 +7864,8 @@
       <c r="S2" s="5">
         <v>0</v>
       </c>
-      <c r="T2" s="5">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>4</v>
       </c>
@@ -7963,11 +7923,8 @@
       <c r="S3" s="5">
         <v>60</v>
       </c>
-      <c r="T3" s="5">
-        <v>0.79379999999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>5</v>
       </c>
@@ -8025,11 +7982,8 @@
       <c r="S4" s="5">
         <v>40</v>
       </c>
-      <c r="T4" s="5">
-        <v>5.1840000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>6</v>
       </c>
@@ -8087,11 +8041,8 @@
       <c r="S5" s="5">
         <v>40</v>
       </c>
-      <c r="T5" s="5">
-        <v>0.20960000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>7</v>
       </c>
@@ -8149,11 +8100,8 @@
       <c r="S6" s="5">
         <v>25</v>
       </c>
-      <c r="T6" s="5">
-        <v>0.23250000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>8</v>
       </c>
@@ -8211,11 +8159,8 @@
       <c r="S7" s="5">
         <v>0</v>
       </c>
-      <c r="T7" s="5">
-        <v>4.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>9</v>
       </c>
@@ -8273,11 +8218,8 @@
       <c r="S8" s="5">
         <v>40</v>
       </c>
-      <c r="T8" s="5">
-        <v>4.3574999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>10</v>
       </c>
@@ -8335,11 +8277,8 @@
       <c r="S9" s="5">
         <v>0</v>
       </c>
-      <c r="T9" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>11</v>
       </c>
@@ -8397,11 +8336,8 @@
       <c r="S10" s="5">
         <v>50</v>
       </c>
-      <c r="T10" s="5">
-        <v>0.41078399999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>12</v>
       </c>
@@ -8459,11 +8395,8 @@
       <c r="S11" s="5">
         <v>50</v>
       </c>
-      <c r="T11" s="5">
-        <v>3.1954500000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>13</v>
       </c>
@@ -8521,11 +8454,8 @@
       <c r="S12" s="5">
         <v>48</v>
       </c>
-      <c r="T12" s="5">
-        <v>1.7570870000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>14</v>
       </c>
@@ -8583,11 +8513,8 @@
       <c r="S13" s="5">
         <v>40</v>
       </c>
-      <c r="T13" s="5">
-        <v>2.0746440000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>15</v>
       </c>
@@ -8645,11 +8572,8 @@
       <c r="S14" s="5">
         <v>70</v>
       </c>
-      <c r="T14" s="5">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>16</v>
       </c>
@@ -8707,11 +8631,8 @@
       <c r="S15" s="5">
         <v>0</v>
       </c>
-      <c r="T15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>17</v>
       </c>
@@ -8769,11 +8690,8 @@
       <c r="S16" s="5">
         <v>45</v>
       </c>
-      <c r="T16" s="5">
-        <v>2.0910000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>18</v>
       </c>
@@ -8831,11 +8749,8 @@
       <c r="S17" s="5">
         <v>40</v>
       </c>
-      <c r="T17" s="5">
-        <v>0.45674999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>19</v>
       </c>
@@ -8893,11 +8808,8 @@
       <c r="S18" s="5">
         <v>5</v>
       </c>
-      <c r="T18" s="5">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>20</v>
       </c>
@@ -8955,11 +8867,8 @@
       <c r="S19" s="5">
         <v>10</v>
       </c>
-      <c r="T19" s="5">
-        <v>2.6532</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>21</v>
       </c>
@@ -9017,12 +8926,9 @@
       <c r="S20" s="5">
         <v>15</v>
       </c>
-      <c r="T20" s="5">
-        <v>2.2067999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="28">
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="27">
         <v>24</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -9079,12 +8985,9 @@
       <c r="S21" s="5">
         <v>85</v>
       </c>
-      <c r="T21" s="5">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="28">
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="27">
         <v>25</v>
       </c>
       <c r="B22" s="24" t="s">
@@ -9141,58 +9044,38 @@
       <c r="S22" s="22">
         <v>95</v>
       </c>
-      <c r="T22" s="5">
-        <v>2.4700000000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="K27" s="51"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="K29" s="51"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="K30" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B18:S19 B20 A20:A22 A2:S17">
-    <cfRule type="expression" dxfId="22" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:R20">
-    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
       <formula>ROW(N20)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
       <formula>COLUMN(N20)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20">
-    <cfRule type="expression" dxfId="18" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
       <formula>ROW(S20)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="6" stopIfTrue="1">
       <formula>COLUMN(S20)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>COLUMN(C20)=$F$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
       <formula>ROW(C20)=$E$1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T22">
-    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
-      <formula>ROW(T2)=$C$1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2" stopIfTrue="1">
-      <formula>COLUMN(T2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -9214,17 +9097,17 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="25.44140625" style="37" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" style="37" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="37" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="37"/>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="25.42578125" style="36" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="36" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="36" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9256,7 +9139,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9288,7 +9171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9326,7 +9209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9364,7 +9247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9396,7 +9279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9443,75 +9326,75 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="21.6640625" style="38"/>
-    <col min="10" max="11" width="21.6640625" style="38" customWidth="1"/>
-    <col min="12" max="16384" width="21.6640625" style="38"/>
+    <col min="1" max="1" width="5" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="21.7109375" style="37"/>
+    <col min="10" max="11" width="21.7109375" style="37" customWidth="1"/>
+    <col min="12" max="16384" width="21.7109375" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="50">
-        <v>9.0412228999999997E-4</v>
-      </c>
-      <c r="D2" s="50">
-        <v>0.86349785000000001</v>
-      </c>
-      <c r="E2" s="50">
-        <v>9.7451250000000003E-2</v>
-      </c>
-      <c r="F2" s="50">
-        <v>2.3592281000000001E-3</v>
-      </c>
-      <c r="G2" s="50">
-        <v>8.2270957000000003E-4</v>
-      </c>
-      <c r="H2" s="50">
-        <v>0.29275619000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="49">
+        <v>1.1524281000000001E-2</v>
+      </c>
+      <c r="D2" s="49">
+        <v>16.341711</v>
+      </c>
+      <c r="E2" s="49">
+        <v>1.7986842999999999</v>
+      </c>
+      <c r="F2" s="49">
+        <v>3.8502213E-2</v>
+      </c>
+      <c r="G2" s="49">
+        <v>1.7095398000000001E-2</v>
+      </c>
+      <c r="H2" s="49">
+        <v>8.7067530000000009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>4</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>98</v>
       </c>
       <c r="C3" s="2">
@@ -9533,11 +9416,11 @@
         <v>0.55197054999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>5</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>99</v>
       </c>
       <c r="C4" s="2">
@@ -9559,11 +9442,11 @@
         <v>0.43937693999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>6</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>100</v>
       </c>
       <c r="C5" s="2">
@@ -9585,11 +9468,11 @@
         <v>2.0767392</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>7</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="39" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="2">
@@ -9611,11 +9494,11 @@
         <v>2.4169052999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>8</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="40" t="s">
         <v>102</v>
       </c>
       <c r="C7" s="2">
@@ -9637,11 +9520,11 @@
         <v>0.25908868000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>9</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="40" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="2">
@@ -9663,63 +9546,63 @@
         <v>1.2147266999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>10</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="48">
         <v>1.1524281000000001E-2</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="48">
         <v>13.064581</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="48">
         <v>1.7986842999999999</v>
       </c>
-      <c r="F9" s="49">
+      <c r="F9" s="48">
         <v>3.8502213E-2</v>
       </c>
-      <c r="G9" s="49">
+      <c r="G9" s="48">
         <v>1.4339836999999999E-2</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="48">
         <v>5.7683147000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>11</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="48">
         <v>3.8977495E-3</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D10" s="48">
         <v>6.6378231000000003</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="48">
         <v>0.33354636999999998</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="48">
         <v>3.6638446000000001E-3</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G10" s="48">
         <v>6.3452205000000001E-3</v>
       </c>
-      <c r="H10" s="49">
+      <c r="H10" s="48">
         <v>3.8084742</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>12</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="40" t="s">
         <v>106</v>
       </c>
       <c r="C11" s="2">
@@ -9741,63 +9624,63 @@
         <v>1.9759963</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>13</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C12" s="48">
         <v>1.8296865E-3</v>
       </c>
-      <c r="D12" s="49">
+      <c r="D12" s="48">
         <v>2.1376919999999999</v>
       </c>
-      <c r="E12" s="49">
+      <c r="E12" s="48">
         <v>0.21715095000000001</v>
       </c>
-      <c r="F12" s="49">
+      <c r="F12" s="48">
         <v>3.8183357999999998E-3</v>
       </c>
-      <c r="G12" s="49">
+      <c r="G12" s="48">
         <v>3.2683618999999999E-3</v>
       </c>
-      <c r="H12" s="49">
+      <c r="H12" s="48">
         <v>1.6645894999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>14</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="48">
         <v>2.1675339E-3</v>
       </c>
-      <c r="D13" s="49">
+      <c r="D13" s="48">
         <v>2.3852028000000001</v>
       </c>
-      <c r="E13" s="49">
+      <c r="E13" s="48">
         <v>0.24039757</v>
       </c>
-      <c r="F13" s="49">
+      <c r="F13" s="48">
         <v>4.5559939999999998E-3</v>
       </c>
-      <c r="G13" s="49">
+      <c r="G13" s="48">
         <v>3.8858629999999998E-3</v>
       </c>
-      <c r="H13" s="49">
+      <c r="H13" s="48">
         <v>1.9759963</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>15</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="40" t="s">
         <v>84</v>
       </c>
       <c r="C14" s="2">
@@ -9819,292 +9702,292 @@
         <v>1.6645894999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>16</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="48">
         <v>9.5703047000000006E-3</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D15" s="48">
         <v>11.181349000000001</v>
       </c>
-      <c r="E15" s="49">
+      <c r="E15" s="48">
         <v>1.1358234</v>
       </c>
-      <c r="F15" s="49">
+      <c r="F15" s="48">
         <v>1.9972074999999999E-2</v>
       </c>
-      <c r="G15" s="49">
+      <c r="G15" s="48">
         <v>1.7095398000000001E-2</v>
       </c>
-      <c r="H15" s="49">
+      <c r="H15" s="48">
         <v>8.7067530000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>17</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="48">
         <v>1.2856242E-3</v>
       </c>
-      <c r="D16" s="49">
+      <c r="D16" s="48">
         <v>5.4884582999999996</v>
       </c>
-      <c r="E16" s="49">
+      <c r="E16" s="48">
         <v>0.33457320000000002</v>
       </c>
-      <c r="F16" s="49">
+      <c r="F16" s="48">
         <v>5.0812655999999999E-3</v>
       </c>
-      <c r="G16" s="49">
+      <c r="G16" s="48">
         <v>2.1954254000000001E-3</v>
       </c>
-      <c r="H16" s="49">
+      <c r="H16" s="48">
         <v>0.62333822000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>18</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="48">
         <v>2.0170432000000001E-3</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="48">
         <v>9.4737010999999995</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E17" s="48">
         <v>0.57584038999999998</v>
       </c>
-      <c r="F17" s="49">
+      <c r="F17" s="48">
         <v>7.9888571999999995E-3</v>
       </c>
-      <c r="G17" s="49">
+      <c r="G17" s="48">
         <v>6.0113188999999997E-3</v>
       </c>
-      <c r="H17" s="49">
+      <c r="H17" s="48">
         <v>0.97791181999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>19</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="49">
+      <c r="C18" s="48">
         <v>6.8793711999999996E-4</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="48">
         <v>0.93976550999999997</v>
       </c>
-      <c r="E18" s="49">
+      <c r="E18" s="48">
         <v>0.10546989</v>
       </c>
-      <c r="F18" s="49">
+      <c r="F18" s="48">
         <v>2.5927768E-3</v>
       </c>
-      <c r="G18" s="49">
+      <c r="G18" s="48">
         <v>1.0021024000000001E-3</v>
       </c>
-      <c r="H18" s="49">
+      <c r="H18" s="48">
         <v>0.33293109999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>20</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="49">
+      <c r="C19" s="48">
         <v>1.7751223E-3</v>
       </c>
-      <c r="D19" s="49">
+      <c r="D19" s="48">
         <v>7.5781744</v>
       </c>
-      <c r="E19" s="49">
+      <c r="E19" s="48">
         <v>0.46196108000000002</v>
       </c>
-      <c r="F19" s="49">
+      <c r="F19" s="48">
         <v>7.0159441999999997E-3</v>
       </c>
-      <c r="G19" s="49">
+      <c r="G19" s="48">
         <v>3.0313279000000002E-3</v>
       </c>
-      <c r="H19" s="49">
+      <c r="H19" s="48">
         <v>0.86067262</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>21</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="49">
+      <c r="C20" s="48">
         <v>6.0269407000000002E-4</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="48">
         <v>0.82331812000000004</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E20" s="48">
         <v>9.2401000999999996E-2</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F20" s="48">
         <v>2.2715029999999998E-3</v>
       </c>
-      <c r="G20" s="49">
+      <c r="G20" s="48">
         <v>8.7793080999999998E-4</v>
       </c>
-      <c r="H20" s="49">
+      <c r="H20" s="48">
         <v>0.29167724</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28">
+    <row r="21" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27">
         <v>24</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="46">
+      <c r="C21" s="45">
         <v>1.398646E-5</v>
       </c>
-      <c r="D21" s="47">
+      <c r="D21" s="46">
         <v>1.0869945000000001</v>
       </c>
-      <c r="E21" s="47">
+      <c r="E21" s="46">
         <v>0.18026732000000001</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="46">
         <v>7.1452427000000002E-3</v>
       </c>
-      <c r="G21" s="47">
+      <c r="G21" s="46">
         <v>1.8322938999999999E-3</v>
       </c>
-      <c r="H21" s="47">
+      <c r="H21" s="46">
         <v>1.1594272000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28">
+    <row r="22" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27">
         <v>25</v>
       </c>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="46">
+      <c r="C22" s="45">
         <v>7.2338821999999997E-3</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="46">
         <v>2.1388340000000001</v>
       </c>
-      <c r="E22" s="47">
+      <c r="E22" s="46">
         <v>0.31076082999999999</v>
       </c>
-      <c r="F22" s="47">
+      <c r="F22" s="46">
         <v>3.6478406000000001E-3</v>
       </c>
-      <c r="G22" s="47">
+      <c r="G22" s="46">
         <v>9.9511690999999993E-4</v>
       </c>
-      <c r="H22" s="47">
+      <c r="H22" s="46">
         <v>1.448909</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-    </row>
-    <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-    </row>
-    <row r="25" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-    </row>
-    <row r="26" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-    </row>
-    <row r="27" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-    </row>
-    <row r="28" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-    </row>
-    <row r="29" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-    </row>
-    <row r="30" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-    </row>
-    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
+    <row r="23" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+    </row>
+    <row r="24" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+    </row>
+    <row r="25" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+    </row>
+    <row r="26" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+    </row>
+    <row r="27" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+    </row>
+    <row r="28" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+    </row>
+    <row r="29" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+    </row>
+    <row r="30" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+    </row>
+    <row r="31" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A20:A22 A2:A17">
@@ -10132,298 +10015,298 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Revert "Input commit before merge"
This reverts commit 2386156e
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="14490" windowHeight="11160" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="14496" windowHeight="11160" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -509,7 +509,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="142">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -932,6 +932,9 @@
   </si>
   <si>
     <t>GSS-MAX_BIS</t>
+  </si>
+  <si>
+    <t>NPN, %DM</t>
   </si>
 </sst>
 </file>
@@ -941,7 +944,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1044,6 +1047,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1187,7 +1196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1220,6 +1229,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1264,13 +1274,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="56">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1377,6 +1389,27 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -6165,10 +6198,10 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Feed Scenario"/>
-    <tableColumn id="2" name="ID" dataDxfId="50"/>
-    <tableColumn id="3" name="Min %DM" dataDxfId="49"/>
-    <tableColumn id="4" name="Max %DM" dataDxfId="48"/>
-    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="47"/>
+    <tableColumn id="2" name="ID" dataDxfId="53"/>
+    <tableColumn id="3" name="Min %DM" dataDxfId="52"/>
+    <tableColumn id="4" name="Max %DM" dataDxfId="51"/>
+    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="50"/>
     <tableColumn id="6" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6176,33 +6209,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47">
   <autoFilter ref="A1:X7"/>
   <tableColumns count="24">
-    <tableColumn id="1" name="ID" dataDxfId="43"/>
-    <tableColumn id="2" name="Feed Scenario" dataDxfId="42"/>
-    <tableColumn id="3" name="Batch" dataDxfId="41"/>
-    <tableColumn id="4" name="Breed" dataDxfId="40"/>
-    <tableColumn id="5" name="SBW" dataDxfId="39"/>
-    <tableColumn id="6" name="Feeding Time" dataDxfId="38"/>
-    <tableColumn id="7" name="Target Weight" dataDxfId="37"/>
-    <tableColumn id="8" name="BCS" dataDxfId="36"/>
-    <tableColumn id="9" name="BE" dataDxfId="35"/>
-    <tableColumn id="10" name="L" dataDxfId="34"/>
-    <tableColumn id="11" name="SEX" dataDxfId="33"/>
-    <tableColumn id="12" name="a2" dataDxfId="32"/>
-    <tableColumn id="13" name="PH" dataDxfId="31"/>
-    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="30"/>
-    <tableColumn id="15" name="Algorithm" dataDxfId="29"/>
-    <tableColumn id="16" name="Identifier" dataDxfId="28"/>
-    <tableColumn id="17" name="LB" dataDxfId="27"/>
-    <tableColumn id="18" name="UB" dataDxfId="26"/>
-    <tableColumn id="19" name="Tol" dataDxfId="25"/>
-    <tableColumn id="20" name="DMI Equation" dataDxfId="24"/>
-    <tableColumn id="21" name="Obj" dataDxfId="23"/>
-    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="22"/>
-    <tableColumn id="23" name="Ingredient Level" dataDxfId="21"/>
-    <tableColumn id="24" name="LCA ID" dataDxfId="20"/>
+    <tableColumn id="1" name="ID" dataDxfId="46"/>
+    <tableColumn id="2" name="Feed Scenario" dataDxfId="45"/>
+    <tableColumn id="3" name="Batch" dataDxfId="44"/>
+    <tableColumn id="4" name="Breed" dataDxfId="43"/>
+    <tableColumn id="5" name="SBW" dataDxfId="42"/>
+    <tableColumn id="6" name="Feeding Time" dataDxfId="41"/>
+    <tableColumn id="7" name="Target Weight" dataDxfId="40"/>
+    <tableColumn id="8" name="BCS" dataDxfId="39"/>
+    <tableColumn id="9" name="BE" dataDxfId="38"/>
+    <tableColumn id="10" name="L" dataDxfId="37"/>
+    <tableColumn id="11" name="SEX" dataDxfId="36"/>
+    <tableColumn id="12" name="a2" dataDxfId="35"/>
+    <tableColumn id="13" name="PH" dataDxfId="34"/>
+    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="33"/>
+    <tableColumn id="15" name="Algorithm" dataDxfId="32"/>
+    <tableColumn id="16" name="Identifier" dataDxfId="31"/>
+    <tableColumn id="17" name="LB" dataDxfId="30"/>
+    <tableColumn id="18" name="UB" dataDxfId="29"/>
+    <tableColumn id="19" name="Tol" dataDxfId="28"/>
+    <tableColumn id="20" name="DMI Equation" dataDxfId="27"/>
+    <tableColumn id="21" name="Obj" dataDxfId="26"/>
+    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="25"/>
+    <tableColumn id="23" name="Ingredient Level" dataDxfId="24"/>
+    <tableColumn id="24" name="LCA ID" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6224,12 +6257,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:S22" totalsRowShown="0">
-  <autoFilter ref="A1:S22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:T22" totalsRowShown="0">
+  <autoFilter ref="A1:T22"/>
   <sortState ref="A2:S22">
     <sortCondition ref="A1:A22"/>
   </sortState>
-  <tableColumns count="19">
+  <tableColumns count="20">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Feed"/>
     <tableColumn id="5" name="Forage, %DM"/>
@@ -6249,6 +6282,7 @@
     <tableColumn id="20" name="NEga, Mcal/kg"/>
     <tableColumn id="21" name="RUP, %CP"/>
     <tableColumn id="29" name="pef, %NDF"/>
+    <tableColumn id="3" name="NPN, %DM" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6561,22 +6595,22 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="6" width="29.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6596,28 +6630,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="19">
-        <v>0</v>
-      </c>
-      <c r="D2" s="19">
+      <c r="C2" s="26">
+        <v>0</v>
+      </c>
+      <c r="D2" s="26">
         <v>4</v>
       </c>
-      <c r="E2" s="50">
-        <v>0.39</v>
+      <c r="E2" s="27">
+        <v>0.4</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>UREA</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -6638,7 +6672,7 @@
         <v>Sugar beet pulp dehydrated</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -6659,7 +6693,7 @@
         <v>Corn gluten feed</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>1</v>
       </c>
@@ -6680,7 +6714,7 @@
         <v>Corn gluten meal (gluten 60)</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>1</v>
       </c>
@@ -6701,7 +6735,7 @@
         <v>Faba bean dehulled</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -6722,7 +6756,7 @@
         <v>Molasses</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>1</v>
       </c>
@@ -6743,7 +6777,7 @@
         <v>Rapeseed meal</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>1</v>
       </c>
@@ -6764,7 +6798,7 @@
         <v>Rapeseed oil</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>1</v>
       </c>
@@ -6785,7 +6819,7 @@
         <v>Soybean extruded</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>1</v>
       </c>
@@ -6806,7 +6840,7 @@
         <v>Sunflower meal low dehulling</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>1</v>
       </c>
@@ -6827,7 +6861,7 @@
         <v>Sunflower meal without dehulling</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>1</v>
       </c>
@@ -6848,7 +6882,7 @@
         <v>Sunflower meal high dehulling</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>1</v>
       </c>
@@ -6869,7 +6903,7 @@
         <v>Sunflower meal</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>1</v>
       </c>
@@ -6890,7 +6924,7 @@
         <v>Sunflower oil without dehulling</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>1</v>
       </c>
@@ -6911,7 +6945,7 @@
         <v>Wheat bran</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>1</v>
       </c>
@@ -6932,7 +6966,7 @@
         <v>DDGS Wheat</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>1</v>
       </c>
@@ -6953,7 +6987,7 @@
         <v>Wheat feed flour</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>1</v>
       </c>
@@ -6974,7 +7008,7 @@
         <v>Wheat gluten feed</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17">
         <v>1</v>
       </c>
@@ -6995,11 +7029,11 @@
         <v>Wheat middlings</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
         <v>1</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="28">
         <v>24</v>
       </c>
       <c r="C21" s="20">
@@ -7008,7 +7042,7 @@
       <c r="D21" s="20">
         <v>100</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="27">
         <v>0.3</v>
       </c>
       <c r="F21" s="17" t="str">
@@ -7016,11 +7050,11 @@
         <v>Grass silage, horizontal silo, temporary meadow, with clover, Northwestern region, at farm/FR S</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>1</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="28">
         <v>25</v>
       </c>
       <c r="C22" s="20">
@@ -7029,7 +7063,7 @@
       <c r="D22" s="20">
         <v>100</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="27">
         <v>0.3</v>
       </c>
       <c r="F22" s="17" t="str">
@@ -7039,10 +7073,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B20:B22 B2:B17">
-    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="1" stopIfTrue="1">
       <formula>ROW(B2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="2" stopIfTrue="1">
       <formula>COLUMN(B2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7063,552 +7097,552 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.28515625" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.33203125" customWidth="1"/>
+    <col min="17" max="17" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="S1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="W1" s="35" t="s">
+      <c r="W1" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="X1" s="43" t="s">
+      <c r="X1" s="44" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="32">
         <v>1</v>
       </c>
-      <c r="C2" s="31">
-        <v>0</v>
-      </c>
-      <c r="D2" s="31" t="s">
+      <c r="C2" s="32">
+        <v>0</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="32">
         <v>375</v>
       </c>
-      <c r="F2" s="31">
-        <v>0</v>
-      </c>
-      <c r="G2" s="30">
+      <c r="F2" s="32">
+        <v>0</v>
+      </c>
+      <c r="G2" s="31">
         <v>620</v>
       </c>
-      <c r="H2" s="31">
+      <c r="H2" s="32">
         <v>5</v>
       </c>
-      <c r="I2" s="31">
+      <c r="I2" s="32">
         <v>1</v>
       </c>
-      <c r="J2" s="31">
+      <c r="J2" s="32">
         <v>1</v>
       </c>
-      <c r="K2" s="31">
+      <c r="K2" s="32">
         <v>1</v>
       </c>
-      <c r="L2" s="31">
-        <v>0</v>
-      </c>
-      <c r="M2" s="31">
+      <c r="L2" s="32">
+        <v>0</v>
+      </c>
+      <c r="M2" s="32">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N2" s="32">
+      <c r="N2" s="33">
         <v>2.02</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="O2" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="Q2" s="31">
+      <c r="Q2" s="32">
         <v>0.8</v>
       </c>
-      <c r="R2" s="31">
+      <c r="R2" s="32">
         <v>3</v>
       </c>
-      <c r="S2" s="31">
+      <c r="S2" s="32">
         <v>0.01</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="U2" s="31" t="s">
+      <c r="U2" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="V2" s="31">
-        <v>0</v>
-      </c>
-      <c r="W2" s="31">
+      <c r="V2" s="32">
+        <v>0</v>
+      </c>
+      <c r="W2" s="32">
         <v>0.1</v>
       </c>
-      <c r="X2" s="30">
+      <c r="X2" s="31">
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="31">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="32">
+        <v>-1</v>
+      </c>
+      <c r="B3" s="35">
+        <v>1</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="35">
+        <v>375</v>
+      </c>
+      <c r="F3" s="32">
+        <v>0</v>
+      </c>
+      <c r="G3" s="34">
+        <v>620</v>
+      </c>
+      <c r="H3" s="35">
+        <v>5</v>
+      </c>
+      <c r="I3" s="35">
+        <v>1</v>
+      </c>
+      <c r="J3" s="35">
+        <v>1</v>
+      </c>
+      <c r="K3" s="35">
+        <v>1</v>
+      </c>
+      <c r="L3" s="35">
+        <v>0</v>
+      </c>
+      <c r="M3" s="32">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N3" s="33">
+        <v>2.02</v>
+      </c>
+      <c r="O3" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="P3" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q3" s="32">
+        <v>1.6</v>
+      </c>
+      <c r="R3" s="35">
+        <v>1.9990000000000001</v>
+      </c>
+      <c r="S3" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="T3" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="U3" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="V3" s="35">
+        <v>0</v>
+      </c>
+      <c r="W3" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="X3" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="32">
+        <v>-1</v>
+      </c>
+      <c r="B4" s="35">
+        <v>1</v>
+      </c>
+      <c r="C4" s="32">
+        <v>0</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="35">
+        <v>375</v>
+      </c>
+      <c r="F4" s="32">
+        <v>0</v>
+      </c>
+      <c r="G4" s="34">
+        <v>620</v>
+      </c>
+      <c r="H4" s="35">
+        <v>5</v>
+      </c>
+      <c r="I4" s="35">
+        <v>1</v>
+      </c>
+      <c r="J4" s="35">
+        <v>1</v>
+      </c>
+      <c r="K4" s="35">
+        <v>1</v>
+      </c>
+      <c r="L4" s="35">
+        <v>0</v>
+      </c>
+      <c r="M4" s="32">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N4" s="33">
+        <v>2.02</v>
+      </c>
+      <c r="O4" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="P4" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q4" s="32">
+        <v>1.6</v>
+      </c>
+      <c r="R4" s="35">
+        <v>1.9990000000000001</v>
+      </c>
+      <c r="S4" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="T4" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="U4" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="V4" s="35">
+        <v>0</v>
+      </c>
+      <c r="W4" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="X4" s="34">
         <v>2</v>
       </c>
-      <c r="B3" s="34">
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="32">
+        <v>-1</v>
+      </c>
+      <c r="B5" s="32">
         <v>1</v>
       </c>
-      <c r="C3" s="31">
-        <v>0</v>
-      </c>
-      <c r="D3" s="34" t="s">
+      <c r="C5" s="32">
+        <v>0</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="34">
+      <c r="E5" s="32">
         <v>375</v>
       </c>
-      <c r="F3" s="31">
-        <v>0</v>
-      </c>
-      <c r="G3" s="33">
+      <c r="F5" s="32">
+        <v>0</v>
+      </c>
+      <c r="G5" s="31">
         <v>620</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H5" s="32">
         <v>5</v>
       </c>
-      <c r="I3" s="34">
+      <c r="I5" s="32">
         <v>1</v>
       </c>
-      <c r="J3" s="34">
+      <c r="J5" s="32">
         <v>1</v>
       </c>
-      <c r="K3" s="34">
+      <c r="K5" s="32">
         <v>1</v>
       </c>
-      <c r="L3" s="34">
-        <v>0</v>
-      </c>
-      <c r="M3" s="31">
+      <c r="L5" s="32">
+        <v>0</v>
+      </c>
+      <c r="M5" s="32">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N3" s="32">
+      <c r="N5" s="33">
         <v>2.02</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="O5" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="P3" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q3" s="31">
+      <c r="P5" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q5" s="32">
         <v>1.6</v>
       </c>
-      <c r="R3" s="34">
+      <c r="R5" s="35">
         <v>1.9990000000000001</v>
       </c>
-      <c r="S3" s="34">
+      <c r="S5" s="35">
         <v>0.01</v>
       </c>
-      <c r="T3" s="34" t="s">
+      <c r="T5" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="34" t="s">
+      <c r="U5" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="V3" s="34">
-        <v>0</v>
-      </c>
-      <c r="W3" s="34">
+      <c r="V5" s="32">
+        <v>0</v>
+      </c>
+      <c r="W5" s="32">
         <v>0.1</v>
       </c>
-      <c r="X3" s="33">
+      <c r="X5" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="32">
+        <v>-1</v>
+      </c>
+      <c r="B6" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="31">
-        <v>3</v>
-      </c>
-      <c r="B4" s="34">
+      <c r="C6" s="32">
+        <v>0</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="35">
+        <v>375</v>
+      </c>
+      <c r="F6" s="32">
+        <v>0</v>
+      </c>
+      <c r="G6" s="34">
+        <v>620</v>
+      </c>
+      <c r="H6" s="35">
+        <v>5</v>
+      </c>
+      <c r="I6" s="35">
         <v>1</v>
       </c>
-      <c r="C4" s="31">
-        <v>0</v>
-      </c>
-      <c r="D4" s="34" t="s">
+      <c r="J6" s="35">
+        <v>1</v>
+      </c>
+      <c r="K6" s="35">
+        <v>1</v>
+      </c>
+      <c r="L6" s="35">
+        <v>0</v>
+      </c>
+      <c r="M6" s="32">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N6" s="33">
+        <v>2.02</v>
+      </c>
+      <c r="O6" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="P6" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q6" s="32">
+        <v>1.6</v>
+      </c>
+      <c r="R6" s="35">
+        <v>1.9990000000000001</v>
+      </c>
+      <c r="S6" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="T6" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="U6" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="V6" s="35">
+        <v>0</v>
+      </c>
+      <c r="W6" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="X6" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="32">
+        <v>-1</v>
+      </c>
+      <c r="B7" s="30">
+        <v>1</v>
+      </c>
+      <c r="C7" s="32">
+        <v>0</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E7" s="30">
         <v>375</v>
       </c>
-      <c r="F4" s="31">
-        <v>0</v>
-      </c>
-      <c r="G4" s="33">
+      <c r="F7" s="32">
+        <v>0</v>
+      </c>
+      <c r="G7" s="29">
         <v>620</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H7" s="30">
         <v>5</v>
       </c>
-      <c r="I4" s="34">
+      <c r="I7" s="30">
         <v>1</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J7" s="30">
         <v>1</v>
       </c>
-      <c r="K4" s="34">
+      <c r="K7" s="30">
         <v>1</v>
       </c>
-      <c r="L4" s="34">
-        <v>0</v>
-      </c>
-      <c r="M4" s="31">
+      <c r="L7" s="30">
+        <v>0</v>
+      </c>
+      <c r="M7" s="32">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N7" s="33">
         <v>2.02</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="O7" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="P4" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q4" s="31">
+      <c r="P7" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q7" s="32">
         <v>1.6</v>
       </c>
-      <c r="R4" s="34">
+      <c r="R7" s="35">
         <v>1.9990000000000001</v>
       </c>
-      <c r="S4" s="34">
+      <c r="S7" s="35">
         <v>0.01</v>
       </c>
-      <c r="T4" s="34" t="s">
+      <c r="T7" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="U4" s="34" t="s">
+      <c r="U7" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="V4" s="34">
-        <v>0</v>
-      </c>
-      <c r="W4" s="34">
+      <c r="V7" s="30">
+        <v>0</v>
+      </c>
+      <c r="W7" s="30">
         <v>0.1</v>
       </c>
-      <c r="X4" s="33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
-        <v>4</v>
-      </c>
-      <c r="B5" s="31">
-        <v>1</v>
-      </c>
-      <c r="C5" s="31">
-        <v>0</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" s="31">
-        <v>375</v>
-      </c>
-      <c r="F5" s="31">
-        <v>0</v>
-      </c>
-      <c r="G5" s="30">
-        <v>620</v>
-      </c>
-      <c r="H5" s="31">
-        <v>5</v>
-      </c>
-      <c r="I5" s="31">
-        <v>1</v>
-      </c>
-      <c r="J5" s="31">
-        <v>1</v>
-      </c>
-      <c r="K5" s="31">
-        <v>1</v>
-      </c>
-      <c r="L5" s="31">
-        <v>0</v>
-      </c>
-      <c r="M5" s="31">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="N5" s="32">
-        <v>2.02</v>
-      </c>
-      <c r="O5" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="P5" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q5" s="31">
-        <v>1.6</v>
-      </c>
-      <c r="R5" s="34">
-        <v>1.9990000000000001</v>
-      </c>
-      <c r="S5" s="34">
-        <v>0.01</v>
-      </c>
-      <c r="T5" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="U5" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="V5" s="31">
-        <v>0</v>
-      </c>
-      <c r="W5" s="31">
-        <v>0.1</v>
-      </c>
-      <c r="X5" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
-        <v>5</v>
-      </c>
-      <c r="B6" s="34">
-        <v>1</v>
-      </c>
-      <c r="C6" s="31">
-        <v>0</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="34">
-        <v>375</v>
-      </c>
-      <c r="F6" s="31">
-        <v>0</v>
-      </c>
-      <c r="G6" s="33">
-        <v>620</v>
-      </c>
-      <c r="H6" s="34">
-        <v>5</v>
-      </c>
-      <c r="I6" s="34">
-        <v>1</v>
-      </c>
-      <c r="J6" s="34">
-        <v>1</v>
-      </c>
-      <c r="K6" s="34">
-        <v>1</v>
-      </c>
-      <c r="L6" s="34">
-        <v>0</v>
-      </c>
-      <c r="M6" s="31">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="N6" s="32">
-        <v>2.02</v>
-      </c>
-      <c r="O6" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="P6" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q6" s="31">
-        <v>1.6</v>
-      </c>
-      <c r="R6" s="34">
-        <v>1.9990000000000001</v>
-      </c>
-      <c r="S6" s="34">
-        <v>0.01</v>
-      </c>
-      <c r="T6" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="U6" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="V6" s="34">
-        <v>0</v>
-      </c>
-      <c r="W6" s="34">
-        <v>0.1</v>
-      </c>
-      <c r="X6" s="33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
-        <v>6</v>
-      </c>
-      <c r="B7" s="29">
-        <v>1</v>
-      </c>
-      <c r="C7" s="31">
-        <v>0</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="29">
-        <v>375</v>
-      </c>
-      <c r="F7" s="31">
-        <v>0</v>
-      </c>
-      <c r="G7" s="28">
-        <v>620</v>
-      </c>
-      <c r="H7" s="29">
-        <v>5</v>
-      </c>
-      <c r="I7" s="29">
-        <v>1</v>
-      </c>
-      <c r="J7" s="29">
-        <v>1</v>
-      </c>
-      <c r="K7" s="29">
-        <v>1</v>
-      </c>
-      <c r="L7" s="29">
-        <v>0</v>
-      </c>
-      <c r="M7" s="31">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="N7" s="32">
-        <v>2.02</v>
-      </c>
-      <c r="O7" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="P7" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q7" s="31">
-        <v>1.6</v>
-      </c>
-      <c r="R7" s="34">
-        <v>1.9990000000000001</v>
-      </c>
-      <c r="S7" s="34">
-        <v>0.01</v>
-      </c>
-      <c r="T7" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="U7" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="V7" s="29">
-        <v>0</v>
-      </c>
-      <c r="W7" s="29">
-        <v>0.1</v>
-      </c>
-      <c r="X7" s="28">
+      <c r="X7" s="29">
         <v>5</v>
       </c>
     </row>
@@ -7633,18 +7667,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="7" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -7664,7 +7698,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -7684,7 +7718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -7718,36 +7752,36 @@
   <sheetPr codeName="Planilha4">
     <tabColor rgb="FFE7E6E6"/>
   </sheetPr>
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125"/>
-    <col min="19" max="19" width="11.85546875" customWidth="1"/>
-    <col min="20" max="986" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625"/>
+    <col min="19" max="19" width="11.88671875" customWidth="1"/>
+    <col min="20" max="986" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -7805,8 +7839,11 @@
       <c r="S1" s="14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -7864,8 +7901,11 @@
       <c r="S2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="5">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>4</v>
       </c>
@@ -7923,8 +7963,11 @@
       <c r="S3" s="5">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" s="5">
+        <v>0.79379999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>5</v>
       </c>
@@ -7982,8 +8025,11 @@
       <c r="S4" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="5">
+        <v>5.1840000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <v>6</v>
       </c>
@@ -8041,8 +8087,11 @@
       <c r="S5" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="5">
+        <v>0.20960000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>7</v>
       </c>
@@ -8100,8 +8149,11 @@
       <c r="S6" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="5">
+        <v>0.23250000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>8</v>
       </c>
@@ -8159,8 +8211,11 @@
       <c r="S7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="5">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>9</v>
       </c>
@@ -8218,8 +8273,11 @@
       <c r="S8" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="5">
+        <v>4.3574999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>10</v>
       </c>
@@ -8277,8 +8335,11 @@
       <c r="S9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>11</v>
       </c>
@@ -8336,8 +8397,11 @@
       <c r="S10" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="5">
+        <v>0.41078399999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>12</v>
       </c>
@@ -8395,8 +8459,11 @@
       <c r="S11" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="5">
+        <v>3.1954500000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>13</v>
       </c>
@@ -8454,8 +8521,11 @@
       <c r="S12" s="5">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="5">
+        <v>1.7570870000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>14</v>
       </c>
@@ -8513,8 +8583,11 @@
       <c r="S13" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="5">
+        <v>2.0746440000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>15</v>
       </c>
@@ -8572,8 +8645,11 @@
       <c r="S14" s="5">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" s="5">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>16</v>
       </c>
@@ -8631,8 +8707,11 @@
       <c r="S15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>17</v>
       </c>
@@ -8690,8 +8769,11 @@
       <c r="S16" s="5">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="5">
+        <v>2.0910000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>18</v>
       </c>
@@ -8749,8 +8831,11 @@
       <c r="S17" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="5">
+        <v>0.45674999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>19</v>
       </c>
@@ -8808,8 +8893,11 @@
       <c r="S18" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>20</v>
       </c>
@@ -8867,8 +8955,11 @@
       <c r="S19" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="5">
+        <v>2.6532</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>21</v>
       </c>
@@ -8926,9 +9017,12 @@
       <c r="S20" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
+      <c r="T20" s="5">
+        <v>2.2067999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="28">
         <v>24</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -8985,9 +9079,12 @@
       <c r="S21" s="5">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
+      <c r="T21" s="5">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="28">
         <v>25</v>
       </c>
       <c r="B22" s="24" t="s">
@@ -9044,38 +9141,58 @@
       <c r="S22" s="22">
         <v>95</v>
       </c>
+      <c r="T22" s="5">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="K27" s="51"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="K29" s="51"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="K30" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B18:S19 B20 A20:A22 A2:S17">
-    <cfRule type="expression" dxfId="19" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="3" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="4" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:R20">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
       <formula>ROW(N20)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
       <formula>COLUMN(N20)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20">
-    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="7" stopIfTrue="1">
       <formula>ROW(S20)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="8" stopIfTrue="1">
       <formula>COLUMN(S20)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:M20">
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
       <formula>COLUMN(C20)=$F$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
       <formula>ROW(C20)=$E$1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2:T22">
+    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
+      <formula>ROW(T2)=$C$1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="2" stopIfTrue="1">
+      <formula>COLUMN(T2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -9097,17 +9214,17 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="25.42578125" style="36" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" style="36" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="36"/>
+    <col min="1" max="1" width="5" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="25.44140625" style="37" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" style="37" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="37" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9139,7 +9256,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9171,7 +9288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9209,7 +9326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9247,7 +9364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9279,7 +9396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9326,75 +9443,75 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="21.7109375" style="37"/>
-    <col min="10" max="11" width="21.7109375" style="37" customWidth="1"/>
-    <col min="12" max="16384" width="21.7109375" style="37"/>
+    <col min="1" max="1" width="5" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="21.6640625" style="38"/>
+    <col min="10" max="11" width="21.6640625" style="38" customWidth="1"/>
+    <col min="12" max="16384" width="21.6640625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="39" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>3</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="49">
-        <v>1.1524281000000001E-2</v>
-      </c>
-      <c r="D2" s="49">
-        <v>16.341711</v>
-      </c>
-      <c r="E2" s="49">
-        <v>1.7986842999999999</v>
-      </c>
-      <c r="F2" s="49">
-        <v>3.8502213E-2</v>
-      </c>
-      <c r="G2" s="49">
-        <v>1.7095398000000001E-2</v>
-      </c>
-      <c r="H2" s="49">
-        <v>8.7067530000000009</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="50">
+        <v>9.0412228999999997E-4</v>
+      </c>
+      <c r="D2" s="50">
+        <v>0.86349785000000001</v>
+      </c>
+      <c r="E2" s="50">
+        <v>9.7451250000000003E-2</v>
+      </c>
+      <c r="F2" s="50">
+        <v>2.3592281000000001E-3</v>
+      </c>
+      <c r="G2" s="50">
+        <v>8.2270957000000003E-4</v>
+      </c>
+      <c r="H2" s="50">
+        <v>0.29275619000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>4</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>98</v>
       </c>
       <c r="C3" s="2">
@@ -9416,11 +9533,11 @@
         <v>0.55197054999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>5</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="48" t="s">
         <v>99</v>
       </c>
       <c r="C4" s="2">
@@ -9442,11 +9559,11 @@
         <v>0.43937693999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <v>6</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="48" t="s">
         <v>100</v>
       </c>
       <c r="C5" s="2">
@@ -9468,11 +9585,11 @@
         <v>2.0767392</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>7</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="40" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="2">
@@ -9494,11 +9611,11 @@
         <v>2.4169052999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>8</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="41" t="s">
         <v>102</v>
       </c>
       <c r="C7" s="2">
@@ -9520,11 +9637,11 @@
         <v>0.25908868000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>9</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="41" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="2">
@@ -9546,63 +9663,63 @@
         <v>1.2147266999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>10</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="49">
         <v>1.1524281000000001E-2</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="49">
         <v>13.064581</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="49">
         <v>1.7986842999999999</v>
       </c>
-      <c r="F9" s="48">
+      <c r="F9" s="49">
         <v>3.8502213E-2</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="49">
         <v>1.4339836999999999E-2</v>
       </c>
-      <c r="H9" s="48">
+      <c r="H9" s="49">
         <v>5.7683147000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>11</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C10" s="49">
         <v>3.8977495E-3</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="49">
         <v>6.6378231000000003</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="49">
         <v>0.33354636999999998</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F10" s="49">
         <v>3.6638446000000001E-3</v>
       </c>
-      <c r="G10" s="48">
+      <c r="G10" s="49">
         <v>6.3452205000000001E-3</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="49">
         <v>3.8084742</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>12</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="41" t="s">
         <v>106</v>
       </c>
       <c r="C11" s="2">
@@ -9624,63 +9741,63 @@
         <v>1.9759963</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>13</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="49">
         <v>1.8296865E-3</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="49">
         <v>2.1376919999999999</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="49">
         <v>0.21715095000000001</v>
       </c>
-      <c r="F12" s="48">
+      <c r="F12" s="49">
         <v>3.8183357999999998E-3</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="49">
         <v>3.2683618999999999E-3</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="49">
         <v>1.6645894999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>14</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="49">
         <v>2.1675339E-3</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="49">
         <v>2.3852028000000001</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E13" s="49">
         <v>0.24039757</v>
       </c>
-      <c r="F13" s="48">
+      <c r="F13" s="49">
         <v>4.5559939999999998E-3</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="49">
         <v>3.8858629999999998E-3</v>
       </c>
-      <c r="H13" s="48">
+      <c r="H13" s="49">
         <v>1.9759963</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>15</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C14" s="2">
@@ -9702,292 +9819,292 @@
         <v>1.6645894999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>16</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="49">
         <v>9.5703047000000006E-3</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="49">
         <v>11.181349000000001</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E15" s="49">
         <v>1.1358234</v>
       </c>
-      <c r="F15" s="48">
+      <c r="F15" s="49">
         <v>1.9972074999999999E-2</v>
       </c>
-      <c r="G15" s="48">
+      <c r="G15" s="49">
         <v>1.7095398000000001E-2</v>
       </c>
-      <c r="H15" s="48">
+      <c r="H15" s="49">
         <v>8.7067530000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>17</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="49">
         <v>1.2856242E-3</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="49">
         <v>5.4884582999999996</v>
       </c>
-      <c r="E16" s="48">
+      <c r="E16" s="49">
         <v>0.33457320000000002</v>
       </c>
-      <c r="F16" s="48">
+      <c r="F16" s="49">
         <v>5.0812655999999999E-3</v>
       </c>
-      <c r="G16" s="48">
+      <c r="G16" s="49">
         <v>2.1954254000000001E-3</v>
       </c>
-      <c r="H16" s="48">
+      <c r="H16" s="49">
         <v>0.62333822000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>18</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="49">
         <v>2.0170432000000001E-3</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="49">
         <v>9.4737010999999995</v>
       </c>
-      <c r="E17" s="48">
+      <c r="E17" s="49">
         <v>0.57584038999999998</v>
       </c>
-      <c r="F17" s="48">
+      <c r="F17" s="49">
         <v>7.9888571999999995E-3</v>
       </c>
-      <c r="G17" s="48">
+      <c r="G17" s="49">
         <v>6.0113188999999997E-3</v>
       </c>
-      <c r="H17" s="48">
+      <c r="H17" s="49">
         <v>0.97791181999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>19</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="49">
         <v>6.8793711999999996E-4</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="49">
         <v>0.93976550999999997</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E18" s="49">
         <v>0.10546989</v>
       </c>
-      <c r="F18" s="48">
+      <c r="F18" s="49">
         <v>2.5927768E-3</v>
       </c>
-      <c r="G18" s="48">
+      <c r="G18" s="49">
         <v>1.0021024000000001E-3</v>
       </c>
-      <c r="H18" s="48">
+      <c r="H18" s="49">
         <v>0.33293109999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>20</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="49">
         <v>1.7751223E-3</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="49">
         <v>7.5781744</v>
       </c>
-      <c r="E19" s="48">
+      <c r="E19" s="49">
         <v>0.46196108000000002</v>
       </c>
-      <c r="F19" s="48">
+      <c r="F19" s="49">
         <v>7.0159441999999997E-3</v>
       </c>
-      <c r="G19" s="48">
+      <c r="G19" s="49">
         <v>3.0313279000000002E-3</v>
       </c>
-      <c r="H19" s="48">
+      <c r="H19" s="49">
         <v>0.86067262</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>21</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="48">
+      <c r="C20" s="49">
         <v>6.0269407000000002E-4</v>
       </c>
-      <c r="D20" s="48">
+      <c r="D20" s="49">
         <v>0.82331812000000004</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="49">
         <v>9.2401000999999996E-2</v>
       </c>
-      <c r="F20" s="48">
+      <c r="F20" s="49">
         <v>2.2715029999999998E-3</v>
       </c>
-      <c r="G20" s="48">
+      <c r="G20" s="49">
         <v>8.7793080999999998E-4</v>
       </c>
-      <c r="H20" s="48">
+      <c r="H20" s="49">
         <v>0.29167724</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
+    <row r="21" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28">
         <v>24</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="46">
         <v>1.398646E-5</v>
       </c>
-      <c r="D21" s="46">
+      <c r="D21" s="47">
         <v>1.0869945000000001</v>
       </c>
-      <c r="E21" s="46">
+      <c r="E21" s="47">
         <v>0.18026732000000001</v>
       </c>
-      <c r="F21" s="46">
+      <c r="F21" s="47">
         <v>7.1452427000000002E-3</v>
       </c>
-      <c r="G21" s="46">
+      <c r="G21" s="47">
         <v>1.8322938999999999E-3</v>
       </c>
-      <c r="H21" s="46">
+      <c r="H21" s="47">
         <v>1.1594272000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
+    <row r="22" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28">
         <v>25</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="46">
         <v>7.2338821999999997E-3</v>
       </c>
-      <c r="D22" s="46">
+      <c r="D22" s="47">
         <v>2.1388340000000001</v>
       </c>
-      <c r="E22" s="46">
+      <c r="E22" s="47">
         <v>0.31076082999999999</v>
       </c>
-      <c r="F22" s="46">
+      <c r="F22" s="47">
         <v>3.6478406000000001E-3</v>
       </c>
-      <c r="G22" s="46">
+      <c r="G22" s="47">
         <v>9.9511690999999993E-4</v>
       </c>
-      <c r="H22" s="46">
+      <c r="H22" s="47">
         <v>1.448909</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-    </row>
-    <row r="24" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-    </row>
-    <row r="25" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-    </row>
-    <row r="26" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-    </row>
-    <row r="27" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-    </row>
-    <row r="28" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-    </row>
-    <row r="29" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-    </row>
-    <row r="30" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-    </row>
-    <row r="31" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
+    <row r="23" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+    </row>
+    <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+    </row>
+    <row r="25" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+    </row>
+    <row r="26" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+    </row>
+    <row r="27" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+    </row>
+    <row r="28" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+    </row>
+    <row r="29" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+    </row>
+    <row r="30" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+    </row>
+    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A20:A22 A2:A17">
@@ -10015,298 +10132,298 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
fix in reduced cost calculator
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -916,9 +916,6 @@
   </si>
   <si>
     <t>Corn Silage - BR</t>
-  </si>
-  <si>
-    <t>Sugarcane bagase - BR</t>
   </si>
   <si>
     <t>Peanut meal</t>
@@ -1315,7 +1312,23 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="70">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2609,34 +2622,34 @@
   </dxfs>
   <tableStyles count="6" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Feeds-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="67"/>
-      <tableStyleElement type="firstRowStripe" dxfId="66"/>
-      <tableStyleElement type="secondRowStripe" dxfId="65"/>
+      <tableStyleElement type="headerRow" dxfId="69"/>
+      <tableStyleElement type="firstRowStripe" dxfId="68"/>
+      <tableStyleElement type="secondRowStripe" dxfId="67"/>
     </tableStyle>
     <tableStyle name="Scenario-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="64"/>
-      <tableStyleElement type="firstRowStripe" dxfId="63"/>
-      <tableStyleElement type="secondRowStripe" dxfId="62"/>
+      <tableStyleElement type="headerRow" dxfId="66"/>
+      <tableStyleElement type="firstRowStripe" dxfId="65"/>
+      <tableStyleElement type="secondRowStripe" dxfId="64"/>
     </tableStyle>
     <tableStyle name="Batch-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="61"/>
-      <tableStyleElement type="firstRowStripe" dxfId="60"/>
-      <tableStyleElement type="secondRowStripe" dxfId="59"/>
+      <tableStyleElement type="headerRow" dxfId="63"/>
+      <tableStyleElement type="firstRowStripe" dxfId="62"/>
+      <tableStyleElement type="secondRowStripe" dxfId="61"/>
     </tableStyle>
     <tableStyle name="Feed Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="58"/>
-      <tableStyleElement type="firstRowStripe" dxfId="57"/>
-      <tableStyleElement type="secondRowStripe" dxfId="56"/>
+      <tableStyleElement type="headerRow" dxfId="60"/>
+      <tableStyleElement type="firstRowStripe" dxfId="59"/>
+      <tableStyleElement type="secondRowStripe" dxfId="58"/>
     </tableStyle>
     <tableStyle name="LCA-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="55"/>
-      <tableStyleElement type="firstRowStripe" dxfId="54"/>
-      <tableStyleElement type="secondRowStripe" dxfId="53"/>
+      <tableStyleElement type="headerRow" dxfId="57"/>
+      <tableStyleElement type="firstRowStripe" dxfId="56"/>
+      <tableStyleElement type="secondRowStripe" dxfId="55"/>
     </tableStyle>
     <tableStyle name="LCA Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="52"/>
-      <tableStyleElement type="firstRowStripe" dxfId="51"/>
-      <tableStyleElement type="secondRowStripe" dxfId="50"/>
+      <tableStyleElement type="headerRow" dxfId="54"/>
+      <tableStyleElement type="firstRowStripe" dxfId="53"/>
+      <tableStyleElement type="secondRowStripe" dxfId="52"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -6407,10 +6420,10 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Feed Scenario"/>
-    <tableColumn id="2" name="ID" dataDxfId="49" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Min %DM" dataDxfId="48"/>
-    <tableColumn id="4" name="Max %DM" dataDxfId="47"/>
-    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="46"/>
+    <tableColumn id="2" name="ID" dataDxfId="51" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Min %DM" dataDxfId="50"/>
+    <tableColumn id="4" name="Max %DM" dataDxfId="49"/>
+    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="48"/>
     <tableColumn id="6" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6418,33 +6431,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="A1:X7"/>
   <tableColumns count="24">
-    <tableColumn id="1" name="ID" dataDxfId="42"/>
-    <tableColumn id="2" name="Feed Scenario" dataDxfId="41"/>
-    <tableColumn id="3" name="Batch" dataDxfId="40"/>
-    <tableColumn id="4" name="Breed" dataDxfId="39"/>
-    <tableColumn id="5" name="SBW" dataDxfId="38"/>
-    <tableColumn id="6" name="Feeding Time" dataDxfId="37"/>
-    <tableColumn id="7" name="Target Weight" dataDxfId="36"/>
-    <tableColumn id="8" name="BCS" dataDxfId="35"/>
-    <tableColumn id="9" name="BE" dataDxfId="34"/>
-    <tableColumn id="10" name="L" dataDxfId="33"/>
-    <tableColumn id="11" name="SEX" dataDxfId="32"/>
-    <tableColumn id="12" name="a2" dataDxfId="31"/>
-    <tableColumn id="13" name="PH" dataDxfId="30"/>
-    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="29"/>
-    <tableColumn id="15" name="Algorithm" dataDxfId="28"/>
-    <tableColumn id="16" name="Identifier" dataDxfId="27"/>
-    <tableColumn id="17" name="LB" dataDxfId="26"/>
-    <tableColumn id="18" name="UB" dataDxfId="25"/>
-    <tableColumn id="19" name="Tol" dataDxfId="24"/>
-    <tableColumn id="20" name="DMI Equation" dataDxfId="23"/>
-    <tableColumn id="21" name="Obj" dataDxfId="22"/>
-    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="21"/>
-    <tableColumn id="23" name="Ingredient Level" dataDxfId="20"/>
-    <tableColumn id="24" name="LCA ID" dataDxfId="19"/>
+    <tableColumn id="1" name="ID" dataDxfId="44"/>
+    <tableColumn id="2" name="Feed Scenario" dataDxfId="43"/>
+    <tableColumn id="3" name="Batch" dataDxfId="42"/>
+    <tableColumn id="4" name="Breed" dataDxfId="41"/>
+    <tableColumn id="5" name="SBW" dataDxfId="40"/>
+    <tableColumn id="6" name="Feeding Time" dataDxfId="39"/>
+    <tableColumn id="7" name="Target Weight" dataDxfId="38"/>
+    <tableColumn id="8" name="BCS" dataDxfId="37"/>
+    <tableColumn id="9" name="BE" dataDxfId="36"/>
+    <tableColumn id="10" name="L" dataDxfId="35"/>
+    <tableColumn id="11" name="SEX" dataDxfId="34"/>
+    <tableColumn id="12" name="a2" dataDxfId="33"/>
+    <tableColumn id="13" name="PH" dataDxfId="32"/>
+    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="31"/>
+    <tableColumn id="15" name="Algorithm" dataDxfId="30"/>
+    <tableColumn id="16" name="Identifier" dataDxfId="29"/>
+    <tableColumn id="17" name="LB" dataDxfId="28"/>
+    <tableColumn id="18" name="UB" dataDxfId="27"/>
+    <tableColumn id="19" name="Tol" dataDxfId="26"/>
+    <tableColumn id="20" name="DMI Equation" dataDxfId="25"/>
+    <tableColumn id="21" name="Obj" dataDxfId="24"/>
+    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="23"/>
+    <tableColumn id="23" name="Ingredient Level" dataDxfId="22"/>
+    <tableColumn id="24" name="LCA ID" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6491,7 +6504,7 @@
     <tableColumn id="20" name="NEga, Mcal/kg"/>
     <tableColumn id="21" name="RUP, %CP"/>
     <tableColumn id="29" name="pef, %NDF"/>
-    <tableColumn id="3" name="NPN, %DM" dataDxfId="18"/>
+    <tableColumn id="3" name="NPN, %DM" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6517,20 +6530,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela26" displayName="Tabela26" ref="A1:H15" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela26" displayName="Tabela26" ref="A1:H15" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:H15"/>
   <sortState ref="A2:H22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="ID" dataDxfId="15" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Name" dataDxfId="14" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="LCA_Phosphorous consumption (kg P)" dataDxfId="13"/>
-    <tableColumn id="3" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="12"/>
-    <tableColumn id="4" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="11"/>
-    <tableColumn id="7" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="10"/>
-    <tableColumn id="8" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="9"/>
-    <tableColumn id="9" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="8"/>
+    <tableColumn id="1" name="ID" dataDxfId="17" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Name" dataDxfId="16" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="LCA_Phosphorous consumption (kg P)" dataDxfId="15"/>
+    <tableColumn id="3" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="14"/>
+    <tableColumn id="4" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="13"/>
+    <tableColumn id="7" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="12"/>
+    <tableColumn id="8" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="11"/>
+    <tableColumn id="9" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6916,7 +6929,7 @@
         <v>80</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7148,7 +7161,7 @@
       </c>
       <c r="E16" s="41">
         <f t="shared" ref="E16:E29" ca="1" si="0">RAND()*2</f>
-        <v>1.3932568803424463</v>
+        <v>1.5569419878419242</v>
       </c>
       <c r="F16" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7170,7 +7183,7 @@
       </c>
       <c r="E17" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43171249278968515</v>
+        <v>1.9229526651116182</v>
       </c>
       <c r="F17" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7192,7 +7205,7 @@
       </c>
       <c r="E18" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8114269651053374</v>
+        <v>1.4225666477993428</v>
       </c>
       <c r="F18" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7214,7 +7227,7 @@
       </c>
       <c r="E19" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96547796936655095</v>
+        <v>0.64773709652756062</v>
       </c>
       <c r="F19" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7236,7 +7249,7 @@
       </c>
       <c r="E20" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7912489733929426</v>
+        <v>1.2964837846565127</v>
       </c>
       <c r="F20" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7258,7 +7271,7 @@
       </c>
       <c r="E21" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4416800872228794E-2</v>
+        <v>1.4001439866647205</v>
       </c>
       <c r="F21" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7280,7 +7293,7 @@
       </c>
       <c r="E22" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7661177192288293</v>
+        <v>0.391965053529163</v>
       </c>
       <c r="F22" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7302,7 +7315,7 @@
       </c>
       <c r="E23" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0160761883155986</v>
+        <v>1.7619020947656918</v>
       </c>
       <c r="F23" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7324,7 +7337,7 @@
       </c>
       <c r="E24" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21318347742222632</v>
+        <v>1.1435129250360481</v>
       </c>
       <c r="F24" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7346,7 +7359,7 @@
       </c>
       <c r="E25" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0739854703010134</v>
+        <v>1.3026632541537453</v>
       </c>
       <c r="F25" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7368,7 +7381,7 @@
       </c>
       <c r="E26" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18356115705444509</v>
+        <v>1.5482370405177421</v>
       </c>
       <c r="F26" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7390,7 +7403,7 @@
       </c>
       <c r="E27" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15353718989514431</v>
+        <v>1.0700050925339362</v>
       </c>
       <c r="F27" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7412,7 +7425,7 @@
       </c>
       <c r="E28" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55007910005474425</v>
+        <v>1.7537369869260859</v>
       </c>
       <c r="F28" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7434,7 +7447,7 @@
       </c>
       <c r="E29" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8308515258198526</v>
+        <v>0.4937244448109126</v>
       </c>
       <c r="F29" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7443,18 +7456,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
       <formula>ROW(B2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>COLUMN(B2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B29">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>ROW(B16)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>COLUMN(B16)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7474,8 +7487,8 @@
   </sheetPr>
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R31" sqref="P31:R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7582,7 +7595,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B2" s="21">
         <v>1</v>
@@ -7645,7 +7658,7 @@
         <v>88</v>
       </c>
       <c r="V2" s="21">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="W2" s="21">
         <v>0.1</v>
@@ -7656,7 +7669,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B3" s="24">
         <v>2</v>
@@ -7698,7 +7711,7 @@
         <v>2.02</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P3" s="24" t="s">
         <v>92</v>
@@ -8198,7 +8211,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8787,7 +8800,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C10" s="36">
         <v>0</v>
@@ -8849,7 +8862,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C11" s="36">
         <v>0</v>
@@ -8973,7 +8986,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" s="2">
         <v>100</v>
@@ -9035,7 +9048,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -9097,7 +9110,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C15" s="36">
         <v>100</v>
@@ -9165,10 +9178,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A15 C2:T15">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9419,8 +9432,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9463,7 +9476,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C2" s="30">
         <v>0</v>
@@ -9489,7 +9502,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C3" s="30">
         <v>0</v>
@@ -9515,7 +9528,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C4" s="30">
         <v>0</v>
@@ -9541,7 +9554,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C5" s="30">
         <v>0</v>
@@ -9566,8 +9579,8 @@
       <c r="A6" s="37">
         <v>27</v>
       </c>
-      <c r="B6" s="38" t="s">
-        <v>139</v>
+      <c r="B6" s="37" t="s">
+        <v>133</v>
       </c>
       <c r="C6" s="30">
         <v>0</v>
@@ -9592,8 +9605,8 @@
       <c r="A7" s="37">
         <v>28</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>132</v>
+      <c r="B7" s="37" t="s">
+        <v>134</v>
       </c>
       <c r="C7" s="30">
         <v>0</v>
@@ -9618,8 +9631,8 @@
       <c r="A8" s="37">
         <v>29</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>133</v>
+      <c r="B8" s="48" t="s">
+        <v>135</v>
       </c>
       <c r="C8" s="30">
         <v>0</v>
@@ -9644,8 +9657,8 @@
       <c r="A9" s="37">
         <v>30</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>134</v>
+      <c r="B9" s="49" t="s">
+        <v>136</v>
       </c>
       <c r="C9" s="30">
         <v>0</v>
@@ -9670,8 +9683,8 @@
       <c r="A10" s="38">
         <v>31</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>135</v>
+      <c r="B10" s="38" t="s">
+        <v>140</v>
       </c>
       <c r="C10" s="30">
         <v>0</v>
@@ -9696,8 +9709,8 @@
       <c r="A11" s="38">
         <v>32</v>
       </c>
-      <c r="B11" s="37" t="s">
-        <v>136</v>
+      <c r="B11" s="38" t="s">
+        <v>141</v>
       </c>
       <c r="C11" s="30">
         <v>0</v>
@@ -9748,8 +9761,8 @@
       <c r="A13" s="2">
         <v>35</v>
       </c>
-      <c r="B13" s="38" t="s">
-        <v>138</v>
+      <c r="B13" s="40" t="s">
+        <v>143</v>
       </c>
       <c r="C13" s="30">
         <v>0</v>
@@ -9800,8 +9813,8 @@
       <c r="A15" s="38">
         <v>37</v>
       </c>
-      <c r="B15" s="40" t="s">
-        <v>145</v>
+      <c r="B15" s="38" t="s">
+        <v>146</v>
       </c>
       <c r="C15" s="30">
         <v>0</v>
@@ -9878,10 +9891,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A15">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix in input data and image.Rdata
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -1312,87 +1312,7 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="70">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="68">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1549,9 +1469,41 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="0.0;0.0;0;@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2478,6 +2430,38 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFDEEAF6"/>
           <bgColor rgb="FFDEEAF6"/>
         </patternFill>
@@ -2622,34 +2606,34 @@
   </dxfs>
   <tableStyles count="6" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Feeds-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="69"/>
-      <tableStyleElement type="firstRowStripe" dxfId="68"/>
-      <tableStyleElement type="secondRowStripe" dxfId="67"/>
+      <tableStyleElement type="headerRow" dxfId="67"/>
+      <tableStyleElement type="firstRowStripe" dxfId="66"/>
+      <tableStyleElement type="secondRowStripe" dxfId="65"/>
     </tableStyle>
     <tableStyle name="Scenario-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="66"/>
-      <tableStyleElement type="firstRowStripe" dxfId="65"/>
-      <tableStyleElement type="secondRowStripe" dxfId="64"/>
+      <tableStyleElement type="headerRow" dxfId="64"/>
+      <tableStyleElement type="firstRowStripe" dxfId="63"/>
+      <tableStyleElement type="secondRowStripe" dxfId="62"/>
     </tableStyle>
     <tableStyle name="Batch-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="63"/>
-      <tableStyleElement type="firstRowStripe" dxfId="62"/>
-      <tableStyleElement type="secondRowStripe" dxfId="61"/>
+      <tableStyleElement type="headerRow" dxfId="61"/>
+      <tableStyleElement type="firstRowStripe" dxfId="60"/>
+      <tableStyleElement type="secondRowStripe" dxfId="59"/>
     </tableStyle>
     <tableStyle name="Feed Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="60"/>
-      <tableStyleElement type="firstRowStripe" dxfId="59"/>
-      <tableStyleElement type="secondRowStripe" dxfId="58"/>
+      <tableStyleElement type="headerRow" dxfId="58"/>
+      <tableStyleElement type="firstRowStripe" dxfId="57"/>
+      <tableStyleElement type="secondRowStripe" dxfId="56"/>
     </tableStyle>
     <tableStyle name="LCA-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="57"/>
-      <tableStyleElement type="firstRowStripe" dxfId="56"/>
-      <tableStyleElement type="secondRowStripe" dxfId="55"/>
+      <tableStyleElement type="headerRow" dxfId="55"/>
+      <tableStyleElement type="firstRowStripe" dxfId="54"/>
+      <tableStyleElement type="secondRowStripe" dxfId="53"/>
     </tableStyle>
     <tableStyle name="LCA Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="54"/>
-      <tableStyleElement type="firstRowStripe" dxfId="53"/>
-      <tableStyleElement type="secondRowStripe" dxfId="52"/>
+      <tableStyleElement type="headerRow" dxfId="52"/>
+      <tableStyleElement type="firstRowStripe" dxfId="51"/>
+      <tableStyleElement type="secondRowStripe" dxfId="50"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -6420,10 +6404,10 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Feed Scenario"/>
-    <tableColumn id="2" name="ID" dataDxfId="51" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Min %DM" dataDxfId="50"/>
-    <tableColumn id="4" name="Max %DM" dataDxfId="49"/>
-    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="48"/>
+    <tableColumn id="2" name="ID" dataDxfId="45" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Min %DM" dataDxfId="44"/>
+    <tableColumn id="4" name="Max %DM" dataDxfId="43"/>
+    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="42"/>
     <tableColumn id="6" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6431,33 +6415,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X7" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
   <autoFilter ref="A1:X7"/>
   <tableColumns count="24">
-    <tableColumn id="1" name="ID" dataDxfId="44"/>
-    <tableColumn id="2" name="Feed Scenario" dataDxfId="43"/>
-    <tableColumn id="3" name="Batch" dataDxfId="42"/>
-    <tableColumn id="4" name="Breed" dataDxfId="41"/>
-    <tableColumn id="5" name="SBW" dataDxfId="40"/>
-    <tableColumn id="6" name="Feeding Time" dataDxfId="39"/>
-    <tableColumn id="7" name="Target Weight" dataDxfId="38"/>
-    <tableColumn id="8" name="BCS" dataDxfId="37"/>
-    <tableColumn id="9" name="BE" dataDxfId="36"/>
-    <tableColumn id="10" name="L" dataDxfId="35"/>
-    <tableColumn id="11" name="SEX" dataDxfId="34"/>
-    <tableColumn id="12" name="a2" dataDxfId="33"/>
-    <tableColumn id="13" name="PH" dataDxfId="32"/>
-    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="31"/>
-    <tableColumn id="15" name="Algorithm" dataDxfId="30"/>
-    <tableColumn id="16" name="Identifier" dataDxfId="29"/>
-    <tableColumn id="17" name="LB" dataDxfId="28"/>
-    <tableColumn id="18" name="UB" dataDxfId="27"/>
-    <tableColumn id="19" name="Tol" dataDxfId="26"/>
-    <tableColumn id="20" name="DMI Equation" dataDxfId="25"/>
-    <tableColumn id="21" name="Obj" dataDxfId="24"/>
-    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="23"/>
-    <tableColumn id="23" name="Ingredient Level" dataDxfId="22"/>
-    <tableColumn id="24" name="LCA ID" dataDxfId="21"/>
+    <tableColumn id="1" name="ID" dataDxfId="38"/>
+    <tableColumn id="2" name="Feed Scenario" dataDxfId="37"/>
+    <tableColumn id="3" name="Batch" dataDxfId="36"/>
+    <tableColumn id="4" name="Breed" dataDxfId="35"/>
+    <tableColumn id="5" name="SBW" dataDxfId="34"/>
+    <tableColumn id="6" name="Feeding Time" dataDxfId="33"/>
+    <tableColumn id="7" name="Target Weight" dataDxfId="32"/>
+    <tableColumn id="8" name="BCS" dataDxfId="31"/>
+    <tableColumn id="9" name="BE" dataDxfId="30"/>
+    <tableColumn id="10" name="L" dataDxfId="29"/>
+    <tableColumn id="11" name="SEX" dataDxfId="28"/>
+    <tableColumn id="12" name="a2" dataDxfId="27"/>
+    <tableColumn id="13" name="PH" dataDxfId="26"/>
+    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="25"/>
+    <tableColumn id="15" name="Algorithm" dataDxfId="24"/>
+    <tableColumn id="16" name="Identifier" dataDxfId="23"/>
+    <tableColumn id="17" name="LB" dataDxfId="22"/>
+    <tableColumn id="18" name="UB" dataDxfId="21"/>
+    <tableColumn id="19" name="Tol" dataDxfId="20"/>
+    <tableColumn id="20" name="DMI Equation" dataDxfId="19"/>
+    <tableColumn id="21" name="Obj" dataDxfId="18"/>
+    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="17"/>
+    <tableColumn id="23" name="Ingredient Level" dataDxfId="16"/>
+    <tableColumn id="24" name="LCA ID" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6504,7 +6488,7 @@
     <tableColumn id="20" name="NEga, Mcal/kg"/>
     <tableColumn id="21" name="RUP, %CP"/>
     <tableColumn id="29" name="pef, %NDF"/>
-    <tableColumn id="3" name="NPN, %DM" dataDxfId="20"/>
+    <tableColumn id="3" name="NPN, %DM" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6530,20 +6514,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela26" displayName="Tabela26" ref="A1:H15" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela26" displayName="Tabela26" ref="A1:H15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H15"/>
   <sortState ref="A2:H22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="ID" dataDxfId="17" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Name" dataDxfId="16" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="LCA_Phosphorous consumption (kg P)" dataDxfId="15"/>
-    <tableColumn id="3" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="14"/>
-    <tableColumn id="4" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="13"/>
-    <tableColumn id="7" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="12"/>
-    <tableColumn id="8" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="11"/>
-    <tableColumn id="9" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="10"/>
+    <tableColumn id="1" name="ID" dataDxfId="7" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Name" dataDxfId="6" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="LCA_Phosphorous consumption (kg P)" dataDxfId="5"/>
+    <tableColumn id="3" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="4"/>
+    <tableColumn id="4" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="3"/>
+    <tableColumn id="7" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="2"/>
+    <tableColumn id="8" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="1"/>
+    <tableColumn id="9" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7161,7 +7145,7 @@
       </c>
       <c r="E16" s="41">
         <f t="shared" ref="E16:E29" ca="1" si="0">RAND()*2</f>
-        <v>1.5569419878419242</v>
+        <v>1.6940438308210688</v>
       </c>
       <c r="F16" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7183,7 +7167,7 @@
       </c>
       <c r="E17" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9229526651116182</v>
+        <v>0.35431906373659983</v>
       </c>
       <c r="F17" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7205,7 +7189,7 @@
       </c>
       <c r="E18" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4225666477993428</v>
+        <v>1.6453173610361571</v>
       </c>
       <c r="F18" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7227,7 +7211,7 @@
       </c>
       <c r="E19" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64773709652756062</v>
+        <v>1.1837686315602622</v>
       </c>
       <c r="F19" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7249,7 +7233,7 @@
       </c>
       <c r="E20" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2964837846565127</v>
+        <v>1.8700080495882252</v>
       </c>
       <c r="F20" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7271,7 +7255,7 @@
       </c>
       <c r="E21" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4001439866647205</v>
+        <v>0.33710567324159912</v>
       </c>
       <c r="F21" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7293,7 +7277,7 @@
       </c>
       <c r="E22" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.391965053529163</v>
+        <v>1.7105058712146695</v>
       </c>
       <c r="F22" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7315,7 +7299,7 @@
       </c>
       <c r="E23" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7619020947656918</v>
+        <v>0.40751567889959994</v>
       </c>
       <c r="F23" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7337,7 +7321,7 @@
       </c>
       <c r="E24" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1435129250360481</v>
+        <v>1.2852557000916958</v>
       </c>
       <c r="F24" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7359,7 +7343,7 @@
       </c>
       <c r="E25" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3026632541537453</v>
+        <v>1.2216006706599818</v>
       </c>
       <c r="F25" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7381,7 +7365,7 @@
       </c>
       <c r="E26" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5482370405177421</v>
+        <v>0.67415519115287914</v>
       </c>
       <c r="F26" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7403,7 +7387,7 @@
       </c>
       <c r="E27" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0700050925339362</v>
+        <v>0.87226334150872642</v>
       </c>
       <c r="F27" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7425,7 +7409,7 @@
       </c>
       <c r="E28" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7537369869260859</v>
+        <v>1.5329226524185682</v>
       </c>
       <c r="F28" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7447,7 +7431,7 @@
       </c>
       <c r="E29" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4937244448109126</v>
+        <v>0.53369191249986492</v>
       </c>
       <c r="F29" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7456,18 +7440,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="3" stopIfTrue="1">
       <formula>ROW(B2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="4" stopIfTrue="1">
       <formula>COLUMN(B2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B29">
-    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="1" stopIfTrue="1">
       <formula>ROW(B16)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="2" stopIfTrue="1">
       <formula>COLUMN(B16)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7487,8 +7471,8 @@
   </sheetPr>
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R31" sqref="P31:R33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7607,13 +7591,13 @@
         <v>129</v>
       </c>
       <c r="E2" s="21">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="F2" s="21">
         <v>0</v>
       </c>
       <c r="G2" s="20">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="H2" s="21">
         <v>4</v>
@@ -7681,13 +7665,13 @@
         <v>129</v>
       </c>
       <c r="E3" s="21">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="F3" s="21">
         <v>0</v>
       </c>
       <c r="G3" s="20">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="H3" s="21">
         <v>4</v>
@@ -7755,13 +7739,13 @@
         <v>129</v>
       </c>
       <c r="E4" s="21">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="F4" s="21">
         <v>0</v>
       </c>
       <c r="G4" s="20">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="H4" s="21">
         <v>4</v>
@@ -7829,13 +7813,13 @@
         <v>129</v>
       </c>
       <c r="E5" s="21">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="F5" s="21">
         <v>0</v>
       </c>
       <c r="G5" s="20">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="H5" s="21">
         <v>4</v>
@@ -7903,13 +7887,13 @@
         <v>129</v>
       </c>
       <c r="E6" s="21">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="F6" s="21">
         <v>0</v>
       </c>
       <c r="G6" s="20">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="H6" s="21">
         <v>4</v>
@@ -7977,13 +7961,13 @@
         <v>129</v>
       </c>
       <c r="E7" s="21">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="F7" s="21">
         <v>0</v>
       </c>
       <c r="G7" s="20">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="H7" s="21">
         <v>4</v>
@@ -9178,10 +9162,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A15 C2:T15">
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9891,10 +9875,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A15">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
DMI calculation fixed: averaged instead of from RData
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="147">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -933,10 +933,10 @@
     <t>Corn Dist Ethanol</t>
   </si>
   <si>
-    <t>BF</t>
-  </si>
-  <si>
     <t>Sugarcane Silage - BR</t>
+  </si>
+  <si>
+    <t>RC_Sugarcane</t>
   </si>
 </sst>
 </file>
@@ -6393,6 +6393,330 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9439275" cy="502920"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9439275" cy="502920"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9439275" cy="502920"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9439275" cy="381000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0666D43A-ADED-4D3B-AF69-A2474C82F50E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9439275" cy="381000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E7DC4C3-566A-49F6-9A8F-B7812E354531}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9439275" cy="381000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7145,7 +7469,7 @@
       </c>
       <c r="E16" s="41">
         <f t="shared" ref="E16:E29" ca="1" si="0">RAND()*2</f>
-        <v>1.6940438308210688</v>
+        <v>3.0090777697150406E-2</v>
       </c>
       <c r="F16" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7167,7 +7491,7 @@
       </c>
       <c r="E17" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35431906373659983</v>
+        <v>0.98398253298434502</v>
       </c>
       <c r="F17" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7189,7 +7513,7 @@
       </c>
       <c r="E18" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6453173610361571</v>
+        <v>1.0250384740856502</v>
       </c>
       <c r="F18" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7211,7 +7535,7 @@
       </c>
       <c r="E19" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1837686315602622</v>
+        <v>1.785552835209298</v>
       </c>
       <c r="F19" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7233,7 +7557,7 @@
       </c>
       <c r="E20" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8700080495882252</v>
+        <v>0.6302588903304851</v>
       </c>
       <c r="F20" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7255,7 +7579,7 @@
       </c>
       <c r="E21" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33710567324159912</v>
+        <v>0.87928823044778448</v>
       </c>
       <c r="F21" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7277,7 +7601,7 @@
       </c>
       <c r="E22" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7105058712146695</v>
+        <v>1.7980603442782361</v>
       </c>
       <c r="F22" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7299,7 +7623,7 @@
       </c>
       <c r="E23" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40751567889959994</v>
+        <v>1.2440121310702519</v>
       </c>
       <c r="F23" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7321,7 +7645,7 @@
       </c>
       <c r="E24" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2852557000916958</v>
+        <v>0.50115360236887185</v>
       </c>
       <c r="F24" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7343,7 +7667,7 @@
       </c>
       <c r="E25" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2216006706599818</v>
+        <v>0.19232468952752635</v>
       </c>
       <c r="F25" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7365,7 +7689,7 @@
       </c>
       <c r="E26" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67415519115287914</v>
+        <v>1.5006227508412389</v>
       </c>
       <c r="F26" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7387,7 +7711,7 @@
       </c>
       <c r="E27" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87226334150872642</v>
+        <v>1.834642213237524</v>
       </c>
       <c r="F27" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7409,7 +7733,7 @@
       </c>
       <c r="E28" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5329226524185682</v>
+        <v>1.7225592945713657</v>
       </c>
       <c r="F28" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7431,7 +7755,7 @@
       </c>
       <c r="E29" s="41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53369191249986492</v>
+        <v>0.28291533422733561</v>
       </c>
       <c r="F29" s="43" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -7471,8 +7795,8 @@
   </sheetPr>
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7624,7 +7948,7 @@
         <v>94</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="Q2" s="21">
         <v>0.8</v>
@@ -7642,7 +7966,7 @@
         <v>88</v>
       </c>
       <c r="V2" s="21">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W2" s="21">
         <v>0.1</v>
@@ -7655,7 +7979,7 @@
       <c r="A3" s="21">
         <v>-1</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="21">
         <v>2</v>
       </c>
       <c r="C3" s="21">
@@ -7676,52 +8000,52 @@
       <c r="H3" s="21">
         <v>4</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="21">
         <v>1</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="21">
         <v>1</v>
       </c>
       <c r="K3" s="21">
         <v>1.2</v>
       </c>
-      <c r="L3" s="24">
+      <c r="L3" s="21">
         <v>0</v>
       </c>
       <c r="M3" s="21">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N3" s="22">
-        <v>2.02</v>
-      </c>
-      <c r="O3" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="P3" s="24" t="s">
+      <c r="N3" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="P3" s="21" t="s">
         <v>92</v>
       </c>
       <c r="Q3" s="21">
         <v>0.8</v>
       </c>
-      <c r="R3" s="24">
+      <c r="R3" s="21">
         <v>3</v>
       </c>
-      <c r="S3" s="24">
+      <c r="S3" s="21">
         <v>0.01</v>
       </c>
-      <c r="T3" s="24" t="s">
+      <c r="T3" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="U3" s="24" t="s">
+      <c r="U3" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="V3" s="24">
-        <v>0</v>
-      </c>
-      <c r="W3" s="24">
+      <c r="V3" s="21">
+        <v>35</v>
+      </c>
+      <c r="W3" s="21">
         <v>0.1</v>
       </c>
-      <c r="X3" s="23">
+      <c r="X3" s="20">
         <v>-1</v>
       </c>
     </row>
@@ -8121,7 +8445,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E22:E23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8166,7 +8490,7 @@
         <v>117</v>
       </c>
       <c r="D2" s="2">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2">
         <v>73</v>
@@ -9094,7 +9418,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C15" s="36">
         <v>100</v>
@@ -9798,7 +10122,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C15" s="30">
         <v>0</v>

</xml_diff>

<commit_message>
RDP <= 12.5 TDN & other fixes
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="14490" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="148">
   <si>
     <t>Feed Scenario</t>
   </si>
@@ -937,6 +937,9 @@
   </si>
   <si>
     <t>RC_Sugarcane</t>
+  </si>
+  <si>
+    <t>BF</t>
   </si>
 </sst>
 </file>
@@ -1056,13 +1059,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
@@ -1079,8 +1075,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1121,6 +1124,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1232,7 +1241,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1289,22 +1298,27 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="18" fillId="7" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="17" fillId="7" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1312,7 +1326,7 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="66">
     <dxf>
       <font>
         <strike val="0"/>
@@ -2446,22 +2460,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFDEEAF6"/>
           <bgColor rgb="FFDEEAF6"/>
         </patternFill>
@@ -2606,34 +2604,34 @@
   </dxfs>
   <tableStyles count="6" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Feeds-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="67"/>
-      <tableStyleElement type="firstRowStripe" dxfId="66"/>
-      <tableStyleElement type="secondRowStripe" dxfId="65"/>
+      <tableStyleElement type="headerRow" dxfId="65"/>
+      <tableStyleElement type="firstRowStripe" dxfId="64"/>
+      <tableStyleElement type="secondRowStripe" dxfId="63"/>
     </tableStyle>
     <tableStyle name="Scenario-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="64"/>
-      <tableStyleElement type="firstRowStripe" dxfId="63"/>
-      <tableStyleElement type="secondRowStripe" dxfId="62"/>
+      <tableStyleElement type="headerRow" dxfId="62"/>
+      <tableStyleElement type="firstRowStripe" dxfId="61"/>
+      <tableStyleElement type="secondRowStripe" dxfId="60"/>
     </tableStyle>
     <tableStyle name="Batch-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="61"/>
-      <tableStyleElement type="firstRowStripe" dxfId="60"/>
-      <tableStyleElement type="secondRowStripe" dxfId="59"/>
+      <tableStyleElement type="headerRow" dxfId="59"/>
+      <tableStyleElement type="firstRowStripe" dxfId="58"/>
+      <tableStyleElement type="secondRowStripe" dxfId="57"/>
     </tableStyle>
     <tableStyle name="Feed Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="58"/>
-      <tableStyleElement type="firstRowStripe" dxfId="57"/>
-      <tableStyleElement type="secondRowStripe" dxfId="56"/>
+      <tableStyleElement type="headerRow" dxfId="56"/>
+      <tableStyleElement type="firstRowStripe" dxfId="55"/>
+      <tableStyleElement type="secondRowStripe" dxfId="54"/>
     </tableStyle>
     <tableStyle name="LCA-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="55"/>
-      <tableStyleElement type="firstRowStripe" dxfId="54"/>
-      <tableStyleElement type="secondRowStripe" dxfId="53"/>
+      <tableStyleElement type="headerRow" dxfId="53"/>
+      <tableStyleElement type="firstRowStripe" dxfId="52"/>
+      <tableStyleElement type="secondRowStripe" dxfId="51"/>
     </tableStyle>
     <tableStyle name="LCA Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="52"/>
-      <tableStyleElement type="firstRowStripe" dxfId="51"/>
-      <tableStyleElement type="secondRowStripe" dxfId="50"/>
+      <tableStyleElement type="headerRow" dxfId="50"/>
+      <tableStyleElement type="firstRowStripe" dxfId="49"/>
+      <tableStyleElement type="secondRowStripe" dxfId="48"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -6721,8 +6719,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="feeds" displayName="feeds" ref="A1:F29" totalsRowShown="0">
-  <autoFilter ref="A1:F29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="feeds" displayName="feeds" ref="A1:F27" totalsRowShown="0">
+  <autoFilter ref="A1:F27"/>
   <sortState ref="A2:F29">
     <sortCondition ref="A1:A29"/>
   </sortState>
@@ -7123,10 +7121,10 @@
   <sheetPr codeName="Planilha1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7140,7 +7138,7 @@
     <col min="8" max="1021" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7160,7 +7158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -7171,9 +7169,9 @@
         <v>0</v>
       </c>
       <c r="D2" s="37">
-        <v>1.5</v>
-      </c>
-      <c r="E2" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="47" t="s">
         <v>124</v>
       </c>
       <c r="F2" s="16" t="str">
@@ -7181,7 +7179,7 @@
         <v>Urea - BR</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -7194,7 +7192,7 @@
       <c r="D3" s="38">
         <v>50</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="48" t="s">
         <v>126</v>
       </c>
       <c r="F3" s="16" t="str">
@@ -7202,7 +7200,7 @@
         <v>Citrus pulp, dry</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>1</v>
       </c>
@@ -7215,7 +7213,7 @@
       <c r="D4" s="38">
         <v>60</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="47" t="s">
         <v>127</v>
       </c>
       <c r="F4" s="16" t="str">
@@ -7223,7 +7221,7 @@
         <v>Corn Silage - BR</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -7236,7 +7234,7 @@
       <c r="D5" s="38">
         <v>80</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="48" t="s">
         <v>142</v>
       </c>
       <c r="F5" s="2" t="str">
@@ -7244,7 +7242,7 @@
         <v>Corn grain - BR</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>1</v>
       </c>
@@ -7257,7 +7255,7 @@
       <c r="D6" s="37">
         <v>30</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="47" t="s">
         <v>120</v>
       </c>
       <c r="F6" s="16" t="str">
@@ -7265,7 +7263,7 @@
         <v>Cottonseed Meal 38% - BR</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>1</v>
       </c>
@@ -7278,7 +7276,7 @@
       <c r="D7" s="38">
         <v>18</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="48" t="s">
         <v>119</v>
       </c>
       <c r="F7" s="16" t="str">
@@ -7286,7 +7284,7 @@
         <v>Cottonseed Whole - BR</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>1</v>
       </c>
@@ -7299,7 +7297,7 @@
       <c r="D8" s="38">
         <v>30</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="48" t="s">
         <v>118</v>
       </c>
       <c r="F8" s="16" t="str">
@@ -7307,7 +7305,7 @@
         <v>Soybean Hulls - BR</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>1</v>
       </c>
@@ -7320,15 +7318,28 @@
       <c r="D9" s="37">
         <v>30</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="41" t="s">
         <v>125</v>
       </c>
       <c r="F9" s="16" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Soybean Meal 49% - BR</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+    </row>
+    <row r="10" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -7341,15 +7352,30 @@
       <c r="D10" s="37">
         <v>100</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="47" t="s">
         <v>121</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Peanut meal</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+    </row>
+    <row r="11" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>1</v>
       </c>
@@ -7362,20 +7388,33 @@
       <c r="D11" s="37">
         <v>50</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="48" t="s">
         <v>122</v>
       </c>
       <c r="F11" s="16" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Rice bran</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+    </row>
+    <row r="12" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>1</v>
       </c>
       <c r="B12" s="37">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C12" s="17">
         <v>0</v>
@@ -7383,15 +7422,28 @@
       <c r="D12" s="37">
         <v>50</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="47" t="s">
         <v>123</v>
       </c>
       <c r="F12" s="16" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Wheat Meal - BR</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+    </row>
+    <row r="13" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>1</v>
       </c>
@@ -7404,15 +7456,30 @@
       <c r="D13" s="38">
         <v>100</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="49">
         <v>10</v>
       </c>
       <c r="F13" s="16" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Sugarcane (S. officinarum) Bagasse Brazil Medium Chop</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -7425,15 +7492,30 @@
       <c r="D14" s="39">
         <v>0</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="49">
         <v>10</v>
       </c>
       <c r="F14" s="16" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Corn Dist Ethanol</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -7446,337 +7528,373 @@
       <c r="D15" s="39">
         <v>100</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="50" t="s">
         <v>128</v>
       </c>
       <c r="F15" s="16" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Sugarcane Silage - BR</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="42">
         <v>2</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="44">
         <v>3</v>
       </c>
-      <c r="C16" s="45">
-        <v>0</v>
-      </c>
-      <c r="D16" s="44">
-        <v>50</v>
-      </c>
-      <c r="E16" s="41">
-        <f t="shared" ref="E16:E29" ca="1" si="0">RAND()*2</f>
-        <v>3.0090777697150406E-2</v>
-      </c>
-      <c r="F16" s="43" t="str">
+      <c r="C16" s="43">
+        <v>0</v>
+      </c>
+      <c r="D16" s="37">
+        <v>100</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2.08</v>
+      </c>
+      <c r="F16" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Urea - BR</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="43">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
         <v>2</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B17" s="44">
         <v>24</v>
       </c>
-      <c r="C17" s="45">
-        <v>0</v>
-      </c>
-      <c r="D17" s="44">
+      <c r="C17" s="43">
+        <v>0</v>
+      </c>
+      <c r="D17" s="38">
         <v>50</v>
       </c>
-      <c r="E17" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.98398253298434502</v>
-      </c>
-      <c r="F17" s="43" t="str">
+      <c r="E17" s="2">
+        <v>0.34583000000000003</v>
+      </c>
+      <c r="F17" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Citrus pulp, dry</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="43">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="42">
         <v>2</v>
       </c>
-      <c r="B18" s="47">
+      <c r="B18" s="44">
         <v>25</v>
       </c>
-      <c r="C18" s="45">
-        <v>0</v>
-      </c>
-      <c r="D18" s="44">
+      <c r="C18" s="43">
+        <v>0</v>
+      </c>
+      <c r="D18" s="38">
         <v>60</v>
       </c>
-      <c r="E18" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0250384740856502</v>
-      </c>
-      <c r="F18" s="43" t="str">
+      <c r="E18" s="2">
+        <v>0.44566666700000002</v>
+      </c>
+      <c r="F18" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Corn Silage - BR</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="43">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="42">
         <v>2</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="44">
         <v>26</v>
       </c>
-      <c r="C19" s="45">
-        <v>0</v>
-      </c>
-      <c r="D19" s="44">
+      <c r="C19" s="43">
+        <v>0</v>
+      </c>
+      <c r="D19" s="38">
         <v>80</v>
       </c>
-      <c r="E19" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.785552835209298</v>
-      </c>
-      <c r="F19" s="43" t="str">
+      <c r="E19" s="2">
+        <v>0.44566666700000002</v>
+      </c>
+      <c r="F19" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Corn grain - BR</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="43">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="42">
         <v>2</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20" s="44">
         <v>27</v>
       </c>
-      <c r="C20" s="45">
-        <v>0</v>
-      </c>
-      <c r="D20" s="44">
+      <c r="C20" s="43">
+        <v>0</v>
+      </c>
+      <c r="D20" s="37">
         <v>30</v>
       </c>
-      <c r="E20" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.6302588903304851</v>
-      </c>
-      <c r="F20" s="43" t="str">
+      <c r="E20" s="2">
+        <v>0.79444000000000004</v>
+      </c>
+      <c r="F20" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Cottonseed Meal 38% - BR</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="43">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="42">
         <v>2</v>
       </c>
-      <c r="B21" s="47">
+      <c r="B21" s="44">
         <v>28</v>
       </c>
-      <c r="C21" s="45">
-        <v>0</v>
-      </c>
-      <c r="D21" s="44">
+      <c r="C21" s="43">
+        <v>0</v>
+      </c>
+      <c r="D21" s="38">
         <v>18</v>
       </c>
-      <c r="E21" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.87928823044778448</v>
-      </c>
-      <c r="F21" s="43" t="str">
+      <c r="E21" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="F21" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Cottonseed Whole - BR</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" s="42">
         <v>2</v>
       </c>
-      <c r="B22" s="47">
+      <c r="B22" s="44">
         <v>29</v>
       </c>
-      <c r="C22" s="45">
-        <v>0</v>
-      </c>
-      <c r="D22" s="44">
+      <c r="C22" s="43">
+        <v>0</v>
+      </c>
+      <c r="D22" s="38">
         <v>30</v>
       </c>
-      <c r="E22" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7980603442782361</v>
-      </c>
-      <c r="F22" s="43" t="str">
+      <c r="E22" s="2">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="F22" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Soybean Hulls - BR</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="43">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="42">
         <v>2</v>
       </c>
-      <c r="B23" s="47">
+      <c r="B23" s="44">
         <v>30</v>
       </c>
-      <c r="C23" s="45">
-        <v>0</v>
-      </c>
-      <c r="D23" s="44">
+      <c r="C23" s="43">
+        <v>0</v>
+      </c>
+      <c r="D23" s="37">
         <v>30</v>
       </c>
-      <c r="E23" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.2440121310702519</v>
-      </c>
-      <c r="F23" s="43" t="str">
+      <c r="E23" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="F23" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Soybean Meal 49% - BR</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="43">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="42">
         <v>2</v>
       </c>
-      <c r="B24" s="47">
+      <c r="B24" s="44">
         <v>31</v>
       </c>
-      <c r="C24" s="45">
-        <v>0</v>
-      </c>
-      <c r="D24" s="44">
+      <c r="C24" s="43">
+        <v>0</v>
+      </c>
+      <c r="D24" s="37">
         <v>100</v>
       </c>
-      <c r="E24" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.50115360236887185</v>
-      </c>
-      <c r="F24" s="43" t="str">
+      <c r="E24" s="2">
+        <v>0.88749999999999996</v>
+      </c>
+      <c r="F24" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Peanut meal</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="43">
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="42">
         <v>2</v>
       </c>
-      <c r="B25" s="47">
+      <c r="B25" s="44">
         <v>32</v>
       </c>
-      <c r="C25" s="45">
-        <v>0</v>
-      </c>
-      <c r="D25" s="44">
+      <c r="C25" s="43">
+        <v>0</v>
+      </c>
+      <c r="D25" s="37">
         <v>50</v>
       </c>
-      <c r="E25" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.19232468952752635</v>
-      </c>
-      <c r="F25" s="43" t="str">
+      <c r="E25" s="2">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="F25" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Rice bran</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="43">
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="42">
         <v>2</v>
       </c>
-      <c r="B26" s="47">
-        <v>33</v>
-      </c>
-      <c r="C26" s="45">
-        <v>0</v>
-      </c>
-      <c r="D26" s="44">
-        <v>1.5</v>
-      </c>
-      <c r="E26" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.5006227508412389</v>
-      </c>
-      <c r="F26" s="43" t="str">
+      <c r="B26" s="44">
+        <v>38</v>
+      </c>
+      <c r="C26" s="43">
+        <v>0</v>
+      </c>
+      <c r="D26" s="37">
+        <v>50</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.51204000000000005</v>
+      </c>
+      <c r="F26" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Wheat Meal - BR</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="43">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="42">
         <v>2</v>
       </c>
-      <c r="B27" s="43">
-        <v>35</v>
-      </c>
-      <c r="C27" s="45">
-        <v>0</v>
-      </c>
-      <c r="D27" s="44">
-        <v>100</v>
-      </c>
-      <c r="E27" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.834642213237524</v>
-      </c>
-      <c r="F27" s="43" t="str">
-        <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
-        <v>Sugarcane (S. officinarum) Bagasse Brazil Medium Chop</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
-        <v>2</v>
-      </c>
-      <c r="B28" s="43">
-        <v>36</v>
-      </c>
-      <c r="C28" s="45">
-        <v>0</v>
-      </c>
-      <c r="D28" s="46">
-        <v>100</v>
-      </c>
-      <c r="E28" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7225592945713657</v>
-      </c>
-      <c r="F28" s="43" t="str">
-        <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
-        <v>Corn Dist Ethanol</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="43">
-        <v>2</v>
-      </c>
-      <c r="B29" s="47">
+      <c r="B27" s="44">
         <v>37</v>
       </c>
-      <c r="C29" s="45">
-        <v>0</v>
-      </c>
-      <c r="D29" s="46">
-        <v>100</v>
-      </c>
-      <c r="E29" s="41">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.28291533422733561</v>
-      </c>
-      <c r="F29" s="43" t="str">
+      <c r="C27" s="43">
+        <v>0</v>
+      </c>
+      <c r="D27" s="39">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.222319286</v>
+      </c>
+      <c r="F27" s="42" t="str">
         <f>VLOOKUP(feeds[[#This Row],[ID]],FeedLib[],2,0)</f>
         <v>Sugarcane Silage - BR</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B15">
-    <cfRule type="expression" dxfId="49" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="B2:B27">
+    <cfRule type="expression" dxfId="47" priority="3" stopIfTrue="1">
       <formula>ROW(B2)=$C$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="4" stopIfTrue="1">
       <formula>COLUMN(B2)=$D$1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:B29">
-    <cfRule type="expression" dxfId="47" priority="1" stopIfTrue="1">
-      <formula>ROW(B16)=$C$1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="2" stopIfTrue="1">
-      <formula>COLUMN(B16)=$D$1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7795,8 +7913,8 @@
   </sheetPr>
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7903,7 +8021,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B2" s="21">
         <v>1</v>
@@ -7939,7 +8057,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="21">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
       <c r="N2" s="22" t="s">
         <v>130</v>
@@ -7966,7 +8084,7 @@
         <v>88</v>
       </c>
       <c r="V2" s="21">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="W2" s="21">
         <v>0.1</v>
@@ -7977,13 +8095,13 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B3" s="21">
         <v>2</v>
       </c>
       <c r="C3" s="21">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>129</v>
@@ -8013,19 +8131,19 @@
         <v>0</v>
       </c>
       <c r="M3" s="21">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="N3" s="22" t="s">
-        <v>130</v>
+        <v>6.5</v>
+      </c>
+      <c r="N3" s="22">
+        <v>5.29</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="P3" s="21" t="s">
         <v>92</v>
       </c>
       <c r="Q3" s="21">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="R3" s="21">
         <v>3</v>
@@ -8040,7 +8158,7 @@
         <v>88</v>
       </c>
       <c r="V3" s="21">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="W3" s="21">
         <v>0.1</v>
@@ -8087,7 +8205,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="21">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
       <c r="N4" s="22">
         <v>2.02</v>
@@ -8161,7 +8279,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="21">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
       <c r="N5" s="22">
         <v>2.02</v>
@@ -8235,7 +8353,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="21">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
       <c r="N6" s="22">
         <v>2.02</v>
@@ -8309,7 +8427,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="21">
-        <v>8.1999999999999993</v>
+        <v>6.5</v>
       </c>
       <c r="N7" s="22">
         <v>2.02</v>
@@ -8490,10 +8608,10 @@
         <v>117</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -8513,13 +8631,13 @@
   <sheetPr codeName="Planilha4">
     <tabColor rgb="FFE7E6E6"/>
   </sheetPr>
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:B15"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8576,7 +8694,7 @@
       <c r="J1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="51" t="s">
         <v>38</v>
       </c>
       <c r="L1" s="15" t="s">
@@ -8621,7 +8739,7 @@
         <v>99</v>
       </c>
       <c r="E2" s="36">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F2" s="36">
         <v>100</v>
@@ -8641,23 +8759,23 @@
       <c r="K2" s="36">
         <v>0</v>
       </c>
-      <c r="L2" s="36">
-        <v>0</v>
-      </c>
-      <c r="M2" s="36">
+      <c r="L2" s="31">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
         <v>0</v>
       </c>
       <c r="N2" s="36">
         <v>0</v>
       </c>
-      <c r="O2" s="36">
-        <v>0</v>
+      <c r="O2" s="2">
+        <v>96.6</v>
       </c>
       <c r="P2" s="36">
-        <v>0</v>
+        <v>2.42</v>
       </c>
       <c r="Q2" s="36">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="R2" s="36">
         <v>0</v>
@@ -8680,52 +8798,52 @@
         <v>0</v>
       </c>
       <c r="D3" s="36">
-        <v>87.687365400000004</v>
+        <v>86.9</v>
       </c>
       <c r="E3" s="36">
-        <v>6.9054801509999999</v>
+        <v>7.09</v>
       </c>
       <c r="F3" s="36">
-        <v>41.055999999999997</v>
+        <v>27</v>
       </c>
       <c r="G3" s="36">
-        <v>5.63</v>
+        <v>16.34</v>
       </c>
       <c r="H3" s="36">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I3" s="36">
         <v>0</v>
       </c>
       <c r="J3" s="36">
-        <v>2.4395544550000001</v>
+        <v>2</v>
       </c>
       <c r="K3" s="36">
         <v>7.420880682</v>
       </c>
-      <c r="L3" s="36">
-        <v>1.004126063</v>
-      </c>
-      <c r="M3" s="36">
-        <v>24.017840379999999</v>
+      <c r="L3" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="M3" s="2">
+        <v>18.190000000000001</v>
       </c>
       <c r="N3" s="36">
-        <v>2.4489999999999998</v>
-      </c>
-      <c r="O3" s="36">
-        <v>69.974000000000004</v>
+        <v>1.819</v>
+      </c>
+      <c r="O3" s="2">
+        <v>77.599999999999994</v>
       </c>
       <c r="P3" s="36">
-        <v>1.6326637450000001</v>
+        <v>1.87</v>
       </c>
       <c r="Q3" s="36">
-        <v>1.026278931</v>
+        <v>1.23</v>
       </c>
       <c r="R3" s="36">
-        <v>40.314</v>
+        <v>29</v>
       </c>
       <c r="S3" s="36">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="T3" s="40">
         <v>0.67000499999999996</v>
@@ -8739,119 +8857,119 @@
         <v>139</v>
       </c>
       <c r="C4" s="36">
-        <v>65</v>
+        <v>0.65</v>
       </c>
       <c r="D4" s="36">
-        <v>31.58</v>
+        <v>31.3</v>
       </c>
       <c r="E4" s="36">
-        <v>7.59</v>
+        <v>7.09</v>
       </c>
       <c r="F4" s="36">
-        <v>65.650000000000006</v>
+        <v>41.39</v>
       </c>
       <c r="G4" s="36">
-        <v>0.68</v>
+        <v>10.8</v>
       </c>
       <c r="H4" s="36">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="I4" s="36">
         <v>0</v>
       </c>
       <c r="J4" s="36">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="K4" s="36">
         <v>5.0199999999999996</v>
       </c>
-      <c r="L4" s="36">
-        <v>30.91</v>
-      </c>
-      <c r="M4" s="36">
-        <v>53.59</v>
+      <c r="L4" s="31">
+        <v>27.48</v>
+      </c>
+      <c r="M4" s="2">
+        <v>53.2</v>
       </c>
       <c r="N4" s="36">
-        <v>4.66</v>
-      </c>
-      <c r="O4" s="36">
-        <v>63.11</v>
+        <v>4.3038800000000004</v>
+      </c>
+      <c r="O4" s="2">
+        <v>65.8</v>
       </c>
       <c r="P4" s="36">
-        <v>1.42</v>
+        <v>1.5</v>
       </c>
       <c r="Q4" s="36">
-        <v>0.83</v>
+        <v>0.9</v>
       </c>
       <c r="R4" s="36">
-        <v>34.35</v>
+        <v>38</v>
       </c>
       <c r="S4" s="36">
-        <v>86.14</v>
+        <v>85</v>
       </c>
       <c r="T4" s="2">
         <v>1.9074580000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="38">
+    <row r="5" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="55">
         <v>26</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="36">
-        <v>0</v>
-      </c>
-      <c r="D5" s="36">
-        <v>88.65</v>
-      </c>
-      <c r="E5" s="36">
-        <v>9.08</v>
-      </c>
-      <c r="F5" s="36">
-        <v>43.93</v>
-      </c>
-      <c r="G5" s="36">
-        <v>0.54</v>
-      </c>
-      <c r="H5" s="36">
-        <v>0</v>
-      </c>
-      <c r="I5" s="36">
-        <v>0</v>
-      </c>
-      <c r="J5" s="36">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="K5" s="36">
+      <c r="C5" s="53">
+        <v>0</v>
+      </c>
+      <c r="D5" s="53">
+        <v>88</v>
+      </c>
+      <c r="E5" s="53">
+        <v>9.5</v>
+      </c>
+      <c r="F5" s="53">
+        <v>11</v>
+      </c>
+      <c r="G5" s="53">
+        <v>4</v>
+      </c>
+      <c r="H5" s="53">
+        <v>5.77</v>
+      </c>
+      <c r="I5" s="53">
+        <v>0</v>
+      </c>
+      <c r="J5" s="53">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K5" s="53">
         <v>1.43</v>
       </c>
-      <c r="L5" s="36">
-        <v>73.25</v>
-      </c>
-      <c r="M5" s="36">
-        <v>12.18</v>
-      </c>
-      <c r="N5" s="36">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="O5" s="36">
-        <v>87.24</v>
-      </c>
-      <c r="P5" s="36">
-        <v>2.15</v>
-      </c>
-      <c r="Q5" s="36">
-        <v>1.48</v>
-      </c>
-      <c r="R5" s="36">
-        <v>56.07</v>
-      </c>
-      <c r="S5" s="36">
-        <v>15.88</v>
-      </c>
-      <c r="T5" s="2">
+      <c r="L5" s="56">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="M5" s="54">
+        <v>13.4</v>
+      </c>
+      <c r="N5" s="53">
+        <v>0.37519999999999998</v>
+      </c>
+      <c r="O5" s="54">
+        <v>89</v>
+      </c>
+      <c r="P5" s="53">
+        <v>2.21</v>
+      </c>
+      <c r="Q5" s="53">
+        <v>1.52</v>
+      </c>
+      <c r="R5" s="53">
+        <v>25</v>
+      </c>
+      <c r="S5" s="53">
+        <v>80</v>
+      </c>
+      <c r="T5" s="54">
         <v>0.36575000000000002</v>
       </c>
     </row>
@@ -8866,52 +8984,52 @@
         <v>0</v>
       </c>
       <c r="D6" s="36">
-        <v>90.11</v>
+        <v>90</v>
       </c>
       <c r="E6" s="36">
-        <v>42.27</v>
+        <v>37.89</v>
       </c>
       <c r="F6" s="36">
-        <v>56.67</v>
+        <v>20</v>
       </c>
       <c r="G6" s="36">
-        <v>2.09</v>
+        <v>1.5</v>
       </c>
       <c r="H6" s="36">
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="I6" s="36">
         <v>0</v>
       </c>
       <c r="J6" s="36">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="K6" s="36">
         <v>6.6</v>
       </c>
-      <c r="L6" s="36">
-        <v>15.76</v>
-      </c>
-      <c r="M6" s="36">
-        <v>33.28</v>
+      <c r="L6" s="2">
+        <v>1.74</v>
+      </c>
+      <c r="M6" s="2">
+        <v>46.89</v>
       </c>
       <c r="N6" s="36">
-        <v>6.63</v>
-      </c>
-      <c r="O6" s="36">
-        <v>70.92</v>
+        <v>7.0757010000000005</v>
+      </c>
+      <c r="O6" s="2">
+        <v>62.2</v>
       </c>
       <c r="P6" s="36">
-        <v>1.66</v>
+        <v>1.38</v>
       </c>
       <c r="Q6" s="36">
-        <v>1.04</v>
+        <v>0.8</v>
       </c>
       <c r="R6" s="36">
-        <v>43.33</v>
+        <v>22</v>
       </c>
       <c r="S6" s="36">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="T6" s="2">
         <v>3.0312000000000001</v>
@@ -8928,52 +9046,52 @@
         <v>0</v>
       </c>
       <c r="D7" s="36">
-        <v>91.19</v>
+        <v>89.5</v>
       </c>
       <c r="E7" s="36">
-        <v>22.15</v>
+        <v>22.6</v>
       </c>
       <c r="F7" s="36">
-        <v>73.040000000000006</v>
+        <v>12.3</v>
       </c>
       <c r="G7" s="36">
-        <v>1.3</v>
+        <v>7.5</v>
       </c>
       <c r="H7" s="36">
-        <v>0</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I7" s="36">
         <v>0</v>
       </c>
       <c r="J7" s="36">
-        <v>19.07</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="K7" s="36">
         <v>4.2300000000000004</v>
       </c>
-      <c r="L7" s="36">
-        <v>9.0299999999999994</v>
-      </c>
-      <c r="M7" s="36">
-        <v>45.52</v>
+      <c r="L7" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="M7" s="2">
+        <v>44.1</v>
       </c>
       <c r="N7" s="36">
-        <v>8.2899999999999991</v>
-      </c>
-      <c r="O7" s="36">
-        <v>88.49</v>
+        <v>10.143000000000001</v>
+      </c>
+      <c r="O7" s="2">
+        <v>79.8</v>
       </c>
       <c r="P7" s="36">
-        <v>2.19</v>
+        <v>1.93</v>
       </c>
       <c r="Q7" s="36">
-        <v>1.51</v>
+        <v>1.29</v>
       </c>
       <c r="R7" s="36">
-        <v>26.96</v>
+        <v>28</v>
       </c>
       <c r="S7" s="36">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="T7" s="2">
         <v>1.603945</v>
@@ -8983,59 +9101,59 @@
       <c r="A8" s="34">
         <v>29</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="45" t="s">
         <v>135</v>
       </c>
       <c r="C8" s="36">
         <v>0</v>
       </c>
       <c r="D8" s="36">
-        <v>89.79</v>
+        <v>89.7</v>
       </c>
       <c r="E8" s="36">
-        <v>49.81</v>
+        <v>13.4</v>
       </c>
       <c r="F8" s="36">
-        <v>71.25</v>
+        <v>18</v>
       </c>
       <c r="G8" s="36">
-        <v>1.05</v>
+        <v>5.8</v>
       </c>
       <c r="H8" s="36">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="I8" s="36">
         <v>0</v>
       </c>
       <c r="J8" s="36">
-        <v>1.87</v>
+        <v>2</v>
       </c>
       <c r="K8" s="36">
         <v>6.68</v>
       </c>
-      <c r="L8" s="36">
-        <v>28.88</v>
-      </c>
-      <c r="M8" s="36">
-        <v>12.75</v>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>62.7</v>
       </c>
       <c r="N8" s="36">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="O8" s="36">
-        <v>77.52</v>
+        <v>2.0064000000000002</v>
+      </c>
+      <c r="O8" s="2">
+        <v>66.3</v>
       </c>
       <c r="P8" s="36">
-        <v>1.86</v>
+        <v>1.51</v>
       </c>
       <c r="Q8" s="36">
-        <v>1.22</v>
+        <v>0.92</v>
       </c>
       <c r="R8" s="36">
-        <v>28.76</v>
+        <v>31</v>
       </c>
       <c r="S8" s="36">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="T8" s="2">
         <v>0.84419999999999995</v>
@@ -9045,56 +9163,56 @@
       <c r="A9" s="37">
         <v>30</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="46" t="s">
         <v>136</v>
       </c>
       <c r="C9" s="36">
         <v>0</v>
       </c>
       <c r="D9" s="36">
-        <v>89.97</v>
+        <v>88.7</v>
       </c>
       <c r="E9" s="36">
-        <v>13.35</v>
+        <v>47</v>
       </c>
       <c r="F9" s="36">
-        <v>50.82</v>
+        <v>35.89</v>
       </c>
       <c r="G9" s="36">
-        <v>2.34</v>
+        <v>1.6</v>
       </c>
       <c r="H9" s="36">
-        <v>0</v>
+        <v>10.88</v>
       </c>
       <c r="I9" s="36">
         <v>0</v>
       </c>
       <c r="J9" s="36">
-        <v>2.31</v>
+        <v>5.5</v>
       </c>
       <c r="K9" s="36">
         <v>5.12</v>
       </c>
-      <c r="L9" s="36">
-        <v>14.58</v>
-      </c>
-      <c r="M9" s="36">
-        <v>64.64</v>
+      <c r="L9" s="2">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="M9" s="2">
+        <v>14.09</v>
       </c>
       <c r="N9" s="36">
-        <v>3.16</v>
-      </c>
-      <c r="O9" s="36">
-        <v>69.819999999999993</v>
+        <v>2.6770999999999998</v>
+      </c>
+      <c r="O9" s="2">
+        <v>82.8</v>
       </c>
       <c r="P9" s="36">
-        <v>1.62</v>
+        <v>2.02</v>
       </c>
       <c r="Q9" s="36">
-        <v>1.01</v>
+        <v>1.36</v>
       </c>
       <c r="R9" s="36">
-        <v>49.18</v>
+        <v>16</v>
       </c>
       <c r="S9" s="36">
         <v>30</v>
@@ -9114,52 +9232,52 @@
         <v>0</v>
       </c>
       <c r="D10" s="36">
-        <v>94.1</v>
+        <v>90</v>
       </c>
       <c r="E10" s="36">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F10" s="36">
-        <v>29.8</v>
+        <v>30</v>
       </c>
       <c r="G10" s="36">
-        <v>12.5</v>
+        <v>5</v>
       </c>
       <c r="H10" s="36">
-        <v>0</v>
+        <v>14.4</v>
       </c>
       <c r="I10" s="36">
         <v>0</v>
       </c>
       <c r="J10" s="36">
-        <v>7.7</v>
+        <v>7.5</v>
       </c>
       <c r="K10" s="36">
         <v>5.6</v>
       </c>
-      <c r="L10" s="36">
-        <v>6.9</v>
-      </c>
-      <c r="M10" s="36">
-        <v>19.899999999999999</v>
+      <c r="L10" s="2">
+        <v>11.84</v>
+      </c>
+      <c r="M10" s="2">
+        <v>16</v>
       </c>
       <c r="N10" s="36">
-        <v>3.3</v>
-      </c>
-      <c r="O10" s="36">
-        <v>80.8</v>
+        <v>1.6</v>
+      </c>
+      <c r="O10" s="2">
+        <v>91.9</v>
       </c>
       <c r="P10" s="36">
-        <v>2</v>
+        <v>2.29</v>
       </c>
       <c r="Q10" s="36">
-        <v>1.3</v>
+        <v>1.59</v>
       </c>
       <c r="R10" s="36">
-        <v>28.2</v>
+        <v>23</v>
       </c>
       <c r="S10" s="36">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="T10" s="2">
         <v>1.8</v>
@@ -9176,117 +9294,117 @@
         <v>0</v>
       </c>
       <c r="D11" s="36">
-        <v>91.8</v>
+        <v>90</v>
       </c>
       <c r="E11" s="36">
-        <v>14.7</v>
+        <v>16</v>
       </c>
       <c r="F11" s="36">
-        <v>25.8</v>
+        <v>29.68</v>
       </c>
       <c r="G11" s="36">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="H11" s="36">
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="I11" s="36">
         <v>0</v>
       </c>
       <c r="J11" s="36">
-        <v>17.600000000000001</v>
+        <v>13.4</v>
       </c>
       <c r="K11" s="36">
         <v>12.2</v>
       </c>
-      <c r="L11" s="36">
-        <v>20.2</v>
-      </c>
-      <c r="M11" s="36">
-        <v>26.6</v>
+      <c r="L11" s="2">
+        <v>30.21</v>
+      </c>
+      <c r="M11" s="2">
+        <v>30.19</v>
       </c>
       <c r="N11" s="36">
-        <v>5.3</v>
-      </c>
-      <c r="O11" s="36">
-        <v>83.4</v>
+        <v>6.5210400000000002</v>
+      </c>
+      <c r="O11" s="2">
+        <v>77.2</v>
       </c>
       <c r="P11" s="36">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="Q11" s="36">
-        <v>1.4</v>
+        <v>1.22</v>
       </c>
       <c r="R11" s="36">
-        <v>44.7</v>
+        <v>26</v>
       </c>
       <c r="S11" s="36">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="T11" s="2">
         <v>1.66208</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="37">
-        <v>33</v>
-      </c>
-      <c r="B12" s="37" t="s">
+    <row r="12" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="52">
+        <v>38</v>
+      </c>
+      <c r="B12" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="36">
-        <v>0</v>
-      </c>
-      <c r="D12" s="36">
-        <v>89.05</v>
-      </c>
-      <c r="E12" s="36">
-        <v>17.48</v>
-      </c>
-      <c r="F12" s="36">
-        <v>65.34</v>
-      </c>
-      <c r="G12" s="36">
-        <v>0.48</v>
-      </c>
-      <c r="H12" s="36">
-        <v>0</v>
-      </c>
-      <c r="I12" s="36">
-        <v>0</v>
-      </c>
-      <c r="J12" s="36">
-        <v>3.87</v>
-      </c>
-      <c r="K12" s="36">
-        <v>5.39</v>
-      </c>
-      <c r="L12" s="36">
-        <v>30.81</v>
-      </c>
-      <c r="M12" s="36">
-        <v>42.46</v>
-      </c>
-      <c r="N12" s="36">
-        <v>3.59</v>
-      </c>
-      <c r="O12" s="36">
-        <v>71.28</v>
-      </c>
-      <c r="P12" s="36">
-        <v>1.67</v>
-      </c>
-      <c r="Q12" s="36">
-        <v>1.05</v>
-      </c>
-      <c r="R12" s="36">
-        <v>34.659999999999997</v>
-      </c>
-      <c r="S12" s="36">
-        <v>22.5</v>
-      </c>
-      <c r="T12" s="2">
-        <v>2.625</v>
+      <c r="C12" s="53">
+        <v>0</v>
+      </c>
+      <c r="D12" s="53">
+        <v>88.7</v>
+      </c>
+      <c r="E12" s="53">
+        <v>17</v>
+      </c>
+      <c r="F12" s="53">
+        <v>41</v>
+      </c>
+      <c r="G12" s="53">
+        <v>4</v>
+      </c>
+      <c r="H12" s="53">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="I12" s="53">
+        <v>0</v>
+      </c>
+      <c r="J12" s="53">
+        <v>4.5</v>
+      </c>
+      <c r="K12" s="53">
+        <v>5.8</v>
+      </c>
+      <c r="L12" s="53">
+        <v>21.79</v>
+      </c>
+      <c r="M12" s="53">
+        <v>44</v>
+      </c>
+      <c r="N12" s="53">
+        <v>8</v>
+      </c>
+      <c r="O12" s="53">
+        <v>71.150000000000006</v>
+      </c>
+      <c r="P12" s="53">
+        <v>1.68</v>
+      </c>
+      <c r="Q12" s="53">
+        <v>1.06</v>
+      </c>
+      <c r="R12" s="53">
+        <v>23</v>
+      </c>
+      <c r="S12" s="53">
+        <v>45</v>
+      </c>
+      <c r="T12" s="53">
+        <v>2.0910000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -9329,8 +9447,8 @@
       <c r="M13" s="2">
         <v>75.59</v>
       </c>
-      <c r="N13" s="2">
-        <v>11.3</v>
+      <c r="N13" s="36">
+        <v>8.5416700000000017</v>
       </c>
       <c r="O13" s="2">
         <v>54.2</v>
@@ -9385,16 +9503,16 @@
       <c r="K14">
         <v>5.89</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="2">
         <v>12.16</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="2">
         <v>32.15</v>
       </c>
-      <c r="N14">
-        <v>14.42</v>
-      </c>
-      <c r="O14">
+      <c r="N14" s="36">
+        <v>4.6360299999999999</v>
+      </c>
+      <c r="O14" s="2">
         <v>87.7</v>
       </c>
       <c r="P14">
@@ -9424,68 +9542,65 @@
         <v>100</v>
       </c>
       <c r="D15" s="36">
-        <v>51.06</v>
+        <v>46.8</v>
       </c>
       <c r="E15" s="36">
-        <v>2.04</v>
+        <v>1.8</v>
       </c>
       <c r="F15" s="36">
-        <v>40.51</v>
+        <v>42</v>
       </c>
       <c r="G15" s="36">
-        <v>1.03</v>
+        <v>50.39</v>
       </c>
       <c r="H15" s="36">
-        <v>0</v>
+        <v>31.62</v>
       </c>
       <c r="I15" s="36">
         <v>0</v>
       </c>
       <c r="J15" s="36">
-        <v>1.0900000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="K15" s="36">
         <v>4.63</v>
       </c>
-      <c r="L15" s="36">
-        <v>12.47</v>
-      </c>
-      <c r="M15" s="36">
-        <v>79.78</v>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>61.39</v>
       </c>
       <c r="N15" s="36">
-        <v>12.75</v>
-      </c>
-      <c r="O15" s="36">
-        <v>41.47</v>
+        <v>9.6996200000000012</v>
+      </c>
+      <c r="O15" s="2">
+        <v>53.5</v>
       </c>
       <c r="P15" s="36">
-        <v>0.76</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="Q15" s="36">
-        <v>0.26</v>
+        <v>0.53</v>
       </c>
       <c r="R15" s="36">
-        <v>59.49</v>
+        <v>52</v>
       </c>
       <c r="S15" s="36">
-        <v>97.5</v>
+        <v>75</v>
       </c>
       <c r="T15" s="2">
         <v>3.78E-2</v>
       </c>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="31"/>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K20" s="31"/>
-    </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K21" s="31"/>
+    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="Q19" s="40"/>
+    </row>
+    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D20" s="40"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A15 C2:T15">
+  <conditionalFormatting sqref="A2:A15 C2:K11 N2:N11 P2:T11 P13:T15 N13:N15 C13:K15 C12:T12">
     <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>ROW(A2)=$C$1</formula>
     </cfRule>
@@ -9494,9 +9609,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -9939,7 +10054,7 @@
       <c r="A8" s="37">
         <v>29</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="45" t="s">
         <v>135</v>
       </c>
       <c r="C8" s="30">
@@ -9965,7 +10080,7 @@
       <c r="A9" s="37">
         <v>30</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="46" t="s">
         <v>136</v>
       </c>
       <c r="C9" s="30">

</xml_diff>

<commit_message>
Input Urea UB fixed
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\Downloads\17_12_EMBRAPA\Etanol-Agro\RESULTADOS\2021-03-31\03-RC-DDG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Gabriel\Models\EMB_MaxProfitDiet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2692F843-F96B-4DE3-AA78-D1E53F55F635}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="LCA Library" sheetId="8" r:id="rId6"/>
     <sheet name="Parameters List" sheetId="6" state="hidden" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>MARQUES Gabriel</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -164,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -260,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -308,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -332,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -357,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -381,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -429,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000012000000}">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -478,7 +477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000013000000}">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -966,7 +965,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0;0.0;0"/>
   </numFmts>
@@ -1343,9 +1342,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
   <dxfs count="66">
     <dxf>
@@ -2624,32 +2623,32 @@
     </dxf>
   </dxfs>
   <tableStyles count="6" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Feeds-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Feeds-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="65"/>
       <tableStyleElement type="firstRowStripe" dxfId="64"/>
       <tableStyleElement type="secondRowStripe" dxfId="63"/>
     </tableStyle>
-    <tableStyle name="Scenario-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Scenario-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="62"/>
       <tableStyleElement type="firstRowStripe" dxfId="61"/>
       <tableStyleElement type="secondRowStripe" dxfId="60"/>
     </tableStyle>
-    <tableStyle name="Batch-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
+    <tableStyle name="Batch-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="59"/>
       <tableStyleElement type="firstRowStripe" dxfId="58"/>
       <tableStyleElement type="secondRowStripe" dxfId="57"/>
     </tableStyle>
-    <tableStyle name="Feed Library-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
+    <tableStyle name="Feed Library-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="56"/>
       <tableStyleElement type="firstRowStripe" dxfId="55"/>
       <tableStyleElement type="secondRowStripe" dxfId="54"/>
     </tableStyle>
-    <tableStyle name="LCA-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
+    <tableStyle name="LCA-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="53"/>
       <tableStyleElement type="firstRowStripe" dxfId="52"/>
       <tableStyleElement type="secondRowStripe" dxfId="51"/>
     </tableStyle>
-    <tableStyle name="LCA Library-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
+    <tableStyle name="LCA Library-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="50"/>
       <tableStyleElement type="firstRowStripe" dxfId="49"/>
       <tableStyleElement type="secondRowStripe" dxfId="48"/>
@@ -7226,137 +7225,137 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="feeds" displayName="feeds" ref="A1:F27" totalsRowShown="0">
-  <autoFilter ref="A1:F27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="feeds" displayName="feeds" ref="A1:F27" totalsRowShown="0">
+  <autoFilter ref="A1:F27"/>
+  <sortState ref="A2:F29">
     <sortCondition ref="A1:A29"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Feed Scenario"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ID" dataDxfId="45" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Min %DM" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Max %DM" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Cost [US$/kg AF]" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Name"/>
+    <tableColumn id="1" name="Feed Scenario"/>
+    <tableColumn id="2" name="ID" dataDxfId="45" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Min %DM" dataDxfId="44"/>
+    <tableColumn id="4" name="Max %DM" dataDxfId="43"/>
+    <tableColumn id="5" name="Cost [US$/kg AF]" dataDxfId="42"/>
+    <tableColumn id="6" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="scenario" displayName="scenario" ref="A1:X10" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
-  <autoFilter ref="A1:X10" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="scenario" displayName="scenario" ref="A1:X10" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
+  <autoFilter ref="A1:X10"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Feed Scenario" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Batch" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Breed" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="SBW" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Feeding Time" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Target Weight" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="BCS" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BE" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="L" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="SEX" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="a2" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="PH" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Selling Price [US$]" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Algorithm" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Identifier" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="LB" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="UB" dataDxfId="21"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Tol" dataDxfId="20"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="DMI Equation" dataDxfId="19"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Obj" dataDxfId="18"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Find Reduced Cost" dataDxfId="17"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="Ingredient Level" dataDxfId="16"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="LCA ID" dataDxfId="15"/>
+    <tableColumn id="1" name="ID" dataDxfId="38"/>
+    <tableColumn id="2" name="Feed Scenario" dataDxfId="37"/>
+    <tableColumn id="3" name="Batch" dataDxfId="36"/>
+    <tableColumn id="4" name="Breed" dataDxfId="35"/>
+    <tableColumn id="5" name="SBW" dataDxfId="34"/>
+    <tableColumn id="6" name="Feeding Time" dataDxfId="33"/>
+    <tableColumn id="7" name="Target Weight" dataDxfId="32"/>
+    <tableColumn id="8" name="BCS" dataDxfId="31"/>
+    <tableColumn id="9" name="BE" dataDxfId="30"/>
+    <tableColumn id="10" name="L" dataDxfId="29"/>
+    <tableColumn id="11" name="SEX" dataDxfId="28"/>
+    <tableColumn id="12" name="a2" dataDxfId="27"/>
+    <tableColumn id="13" name="PH" dataDxfId="26"/>
+    <tableColumn id="14" name="Selling Price [US$]" dataDxfId="25"/>
+    <tableColumn id="15" name="Algorithm" dataDxfId="24"/>
+    <tableColumn id="16" name="Identifier" dataDxfId="23"/>
+    <tableColumn id="17" name="LB" dataDxfId="22"/>
+    <tableColumn id="18" name="UB" dataDxfId="21"/>
+    <tableColumn id="19" name="Tol" dataDxfId="20"/>
+    <tableColumn id="20" name="DMI Equation" dataDxfId="19"/>
+    <tableColumn id="21" name="Obj" dataDxfId="18"/>
+    <tableColumn id="22" name="Find Reduced Cost" dataDxfId="17"/>
+    <tableColumn id="23" name="Ingredient Level" dataDxfId="16"/>
+    <tableColumn id="24" name="LCA ID" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="batch" displayName="batch" ref="A1:F5" totalsRowShown="0">
-  <autoFilter ref="A1:F5" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="batch" displayName="batch" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Batch ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Filename"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Period col"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Initial Period"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Final Period"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Only Costs Batch"/>
+    <tableColumn id="1" name="Batch ID"/>
+    <tableColumn id="2" name="Filename"/>
+    <tableColumn id="3" name="Period col"/>
+    <tableColumn id="4" name="Initial Period"/>
+    <tableColumn id="5" name="Final Period"/>
+    <tableColumn id="6" name="Only Costs Batch"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="FeedLib" displayName="FeedLib" ref="A1:T15" totalsRowShown="0">
-  <autoFilter ref="A1:T15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:T15" totalsRowShown="0">
+  <autoFilter ref="A1:T15"/>
+  <sortState ref="A2:T15">
     <sortCondition ref="A1:A15"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Feed"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Forage, %DM"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="DM, %AF"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="CP, %DM"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="SP, %CP"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="ADICP, %CP"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="Sugars, %DM"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="OA, %DM"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Fat, %DM"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="Ash, %DM"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="Starch, %DM"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="NDF, %DM"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="Lignin, %DM"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="TDN, %DM"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="NEma, Mcal/kg"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0300-000014000000}" name="NEga, Mcal/kg"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0300-000015000000}" name="RUP, %CP"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0300-00001D000000}" name="pef, %NDF"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="NPN, %DM" dataDxfId="12"/>
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Feed"/>
+    <tableColumn id="5" name="Forage, %DM"/>
+    <tableColumn id="6" name="DM, %AF"/>
+    <tableColumn id="7" name="CP, %DM"/>
+    <tableColumn id="8" name="SP, %CP"/>
+    <tableColumn id="9" name="ADICP, %CP"/>
+    <tableColumn id="10" name="Sugars, %DM"/>
+    <tableColumn id="11" name="OA, %DM"/>
+    <tableColumn id="12" name="Fat, %DM"/>
+    <tableColumn id="13" name="Ash, %DM"/>
+    <tableColumn id="14" name="Starch, %DM"/>
+    <tableColumn id="15" name="NDF, %DM"/>
+    <tableColumn id="16" name="Lignin, %DM"/>
+    <tableColumn id="17" name="TDN, %DM"/>
+    <tableColumn id="19" name="NEma, Mcal/kg"/>
+    <tableColumn id="20" name="NEga, Mcal/kg"/>
+    <tableColumn id="21" name="RUP, %CP"/>
+    <tableColumn id="29" name="pef, %NDF"/>
+    <tableColumn id="3" name="NPN, %DM" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="lca" displayName="lca" ref="A1:J6" totalsRowShown="0">
-  <autoFilter ref="A1:J6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="lca" displayName="lca" ref="A1:J6" totalsRowShown="0">
+  <autoFilter ref="A1:J6"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="ID"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="weight_LCA_Phosphorous consumption (kg P)"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="weight_LCA_CED 1.8 non renewable fossil+nuclear (MJ)"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="weight_LCA_Climate change ILCD (kg CO2 eq)"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="weight_LCA_Acidification ILCD (molc H+ eq)"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="weight_LCA_Eutrophication CML baseline (kg PO4- eq)"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="weight_LCA_Land competition CML non baseline (m2a)"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="Methane_Equation"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="N2O_Equation"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Normalize"/>
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="3" name="weight_LCA_Phosphorous consumption (kg P)"/>
+    <tableColumn id="5" name="weight_LCA_CED 1.8 non renewable fossil+nuclear (MJ)"/>
+    <tableColumn id="9" name="weight_LCA_Climate change ILCD (kg CO2 eq)"/>
+    <tableColumn id="10" name="weight_LCA_Acidification ILCD (molc H+ eq)"/>
+    <tableColumn id="11" name="weight_LCA_Eutrophication CML baseline (kg PO4- eq)"/>
+    <tableColumn id="12" name="weight_LCA_Land competition CML non baseline (m2a)"/>
+    <tableColumn id="14" name="Methane_Equation"/>
+    <tableColumn id="7" name="N2O_Equation"/>
+    <tableColumn id="2" name="Normalize"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabela26" displayName="Tabela26" ref="A1:H15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H15" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela26" displayName="Tabela26" ref="A1:H15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H15"/>
+  <sortState ref="A2:H22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="ID" dataDxfId="7" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Name" dataDxfId="6" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="LCA_Phosphorous consumption (kg P)" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="7" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Name" dataDxfId="6" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="LCA_Phosphorous consumption (kg P)" dataDxfId="5"/>
+    <tableColumn id="3" name="LCA_CED 1.8 non renewable fossil+nuclear (MJ)" dataDxfId="4"/>
+    <tableColumn id="4" name="LCA_Climate change ILCD (kg CO2 eq)" dataDxfId="3"/>
+    <tableColumn id="7" name="LCA_Acidification ILCD (molc H+ eq)" dataDxfId="2"/>
+    <tableColumn id="8" name="LCA_Eutrophication CML baseline (kg PO4- eq)" dataDxfId="1"/>
+    <tableColumn id="9" name="LCA_Land competition CML non baseline (m2a)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7624,14 +7623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:XFD1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7676,7 +7675,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="37">
-        <v>5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E2" s="47" t="s">
         <v>123</v>
@@ -7970,7 +7969,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="37">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E16" s="2">
         <v>2.08</v>
@@ -8230,7 +8229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -9101,7 +9100,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha3">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -9232,7 +9231,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha4">
     <tabColor rgb="FFE7E6E6"/>
   </sheetPr>
@@ -10222,7 +10221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -10456,7 +10455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
@@ -10935,7 +10934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha5"/>
   <dimension ref="A1:A58"/>
   <sheetViews>

</xml_diff>